<commit_message>
small adjustment to database, continuing to near seaborn and plotting
</commit_message>
<xml_diff>
--- a/projects/firstTurnData/FirstTurnCombined.xlsx
+++ b/projects/firstTurnData/FirstTurnCombined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PNJae\Dropbox\website\PNJaenichen.github.io\projects\firstTurnData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC6BA73-12BA-48E6-9A80-659B7CEC7858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0274766A-F841-4CD8-8564-02464EB5FE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3362" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3362" uniqueCount="340">
   <si>
     <t>Yes</t>
   </si>
@@ -760,9 +760,6 @@
     <t>Solo/Solitaire Game</t>
   </si>
   <si>
-    <t>bP/Kiwi</t>
-  </si>
-  <si>
     <t>Team Based Game</t>
   </si>
   <si>
@@ -1431,8 +1428,8 @@
   <dimension ref="A1:BO128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L91" sqref="L91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,205 +1504,205 @@
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.25">
@@ -17314,7 +17311,7 @@
         <v>36</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>240</v>
+        <v>36</v>
       </c>
       <c r="M90" s="1" t="s">
         <v>36</v>
@@ -17432,7 +17429,7 @@
         <v>149</v>
       </c>
       <c r="BD90" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="BE90" s="1" t="s">
         <v>53</v>
@@ -18139,13 +18136,13 @@
         <v>54</v>
       </c>
       <c r="BB94" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="BC94" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="BC94" s="1" t="s">
+      <c r="BD94" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="BD94" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="BE94" s="1" t="s">
         <v>65</v>
@@ -18492,7 +18489,7 @@
         <v>36</v>
       </c>
       <c r="AX96" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AY96" s="1" t="s">
         <v>158</v>
@@ -18504,7 +18501,7 @@
         <v>57</v>
       </c>
       <c r="BB96" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BC96" s="1" t="s">
         <v>59</v>
@@ -19032,7 +19029,7 @@
         <v>159</v>
       </c>
       <c r="BB99" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BC99" s="1" t="s">
         <v>149</v>
@@ -19211,7 +19208,7 @@
         <v>82</v>
       </c>
       <c r="AZ100" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="BA100" s="1" t="s">
         <v>47</v>
@@ -19387,7 +19384,7 @@
         <v>46</v>
       </c>
       <c r="AY101" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AZ101" s="1" t="s">
         <v>53</v>
@@ -19738,7 +19735,7 @@
         <v>58</v>
       </c>
       <c r="AZ103" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BA103" s="1" t="s">
         <v>158</v>
@@ -19750,7 +19747,7 @@
         <v>186</v>
       </c>
       <c r="BD103" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="BE103" s="1" t="s">
         <v>144</v>
@@ -19809,7 +19806,7 @@
         <v>3.6170212765957448</v>
       </c>
       <c r="P104" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R104" s="1">
         <v>20</v>
@@ -20099,7 +20096,7 @@
         <v>150</v>
       </c>
       <c r="BB105" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BC105" s="1" t="s">
         <v>65</v>
@@ -20297,7 +20294,7 @@
         <v>3</v>
       </c>
       <c r="L107" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M107" s="1">
         <v>50</v>
@@ -20597,16 +20594,16 @@
         <v>158</v>
       </c>
       <c r="AZ108" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="BA108" s="1" t="s">
         <v>179</v>
       </c>
       <c r="BB108" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="BC108" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="BC108" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="BD108" s="1" t="s">
         <v>59</v>
@@ -20954,7 +20951,7 @@
         <v>17</v>
       </c>
       <c r="AX110" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="111" spans="1:58" x14ac:dyDescent="0.25">
@@ -21126,7 +21123,7 @@
         <v>149</v>
       </c>
       <c r="BA111" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="112" spans="1:58" x14ac:dyDescent="0.25">
@@ -21487,7 +21484,7 @@
         <v>184</v>
       </c>
       <c r="BB113" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="BC113" s="1" t="s">
         <v>95</v>
@@ -21830,7 +21827,7 @@
         <v>58</v>
       </c>
       <c r="AY115" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AZ115" s="1" t="s">
         <v>57</v>
@@ -22688,7 +22685,7 @@
         <v>175</v>
       </c>
       <c r="AZ120" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="BA120" s="1" t="s">
         <v>64</v>
@@ -22697,7 +22694,7 @@
         <v>65</v>
       </c>
       <c r="BC120" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="BD120" s="1" t="s">
         <v>53</v>
@@ -23058,7 +23055,7 @@
         <v>85</v>
       </c>
       <c r="BA122" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="BB122" s="1" t="s">
         <v>53</v>
@@ -23394,7 +23391,7 @@
         <v>36</v>
       </c>
       <c r="AX124" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AY124" s="1" t="s">
         <v>53</v>
@@ -23720,7 +23717,7 @@
         <v>92</v>
       </c>
       <c r="AY126" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="127" spans="1:56" x14ac:dyDescent="0.25">
@@ -24033,7 +24030,7 @@
         <v>54</v>
       </c>
       <c r="BC128" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="BD128" s="1" t="s">
         <v>47</v>
@@ -24065,25 +24062,25 @@
         <v>35</v>
       </c>
       <c r="B1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" t="s">
         <v>242</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>243</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>244</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>245</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>246</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>247</v>
-      </c>
-      <c r="H1" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
@@ -26650,7 +26647,7 @@
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -28846,7 +28843,7 @@
     </row>
     <row r="28" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
updates to first turn database
</commit_message>
<xml_diff>
--- a/projects/firstTurnData/FirstTurnCombined.xlsx
+++ b/projects/firstTurnData/FirstTurnCombined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PNJae\Dropbox\website\PNJaenichen.github.io\projects\firstTurnData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0274766A-F841-4CD8-8564-02464EB5FE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEE76A8-FFA9-4876-AE9D-79B00DA62DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3362" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="340">
   <si>
     <t>Yes</t>
   </si>
@@ -1428,8 +1428,8 @@
   <dimension ref="A1:BO128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L91" sqref="L91"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AU128" sqref="AU128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="S2" s="1">
         <f>IF(R2="null","null",(R2-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
-        <v>-8.9891750123122519E-2</v>
+        <v>-9.4410026492054058E-2</v>
       </c>
       <c r="T2" s="1">
         <f>IF(R2="null","null",10*((R2-$AS2)/($AT2-$AS2)))</f>
@@ -1782,7 +1782,7 @@
       </c>
       <c r="X2" s="1">
         <f>IF(W2="null","null",(W2-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
-        <v>-8.9891750123122519E-2</v>
+        <v>-9.4410026492054058E-2</v>
       </c>
       <c r="Y2" s="1">
         <f>IF(W2="null","null",10*((W2-$AS2)/($AT2-$AS2)))</f>
@@ -1830,15 +1830,15 @@
       </c>
       <c r="AL2" s="1">
         <f t="shared" ref="AL2:AL12" si="1">MIN(N2,S2,X2,AH2)</f>
-        <v>-8.9891750123122519E-2</v>
+        <v>-9.4410026492054058E-2</v>
       </c>
       <c r="AM2" s="1">
         <f t="shared" ref="AM2:AM12" si="2">AVERAGE(N2,S2,X2,AH2)</f>
-        <v>-8.9891750123122519E-2</v>
+        <v>-9.4410026492054058E-2</v>
       </c>
       <c r="AN2" s="1">
         <f t="shared" ref="AN2:AN12" si="3">MAX(N2,S2,X2,AH2)</f>
-        <v>-8.9891750123122519E-2</v>
+        <v>-9.4410026492054058E-2</v>
       </c>
       <c r="AO2" s="1">
         <f>AN2-AL2</f>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="N3" s="1">
         <f t="shared" ref="N3:N66" si="4">IF(M3="null","null",(M3-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
-        <v>0.24428441434370188</v>
+        <v>0.24131528323184503</v>
       </c>
       <c r="O3" s="1">
         <f t="shared" ref="O3:O66" si="5">IF(M3="null","null",10*((M3-$AS3)/($AT3-$AS3)))</f>
@@ -1944,7 +1944,7 @@
       </c>
       <c r="S3" s="1">
         <f t="shared" ref="S3:S66" si="6">IF(R3="null","null",(R3-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
-        <v>0.65272194869204281</v>
+        <v>0.65164621733883288</v>
       </c>
       <c r="T3" s="1">
         <f t="shared" ref="T3:T66" si="7">IF(R3="null","null",10*((R3-$AS3)/($AT3-$AS3)))</f>
@@ -1961,7 +1961,7 @@
       </c>
       <c r="X3" s="1">
         <f t="shared" ref="X3:X66" si="8">IF(W3="null","null",(W3-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
-        <v>1.1168555104515212</v>
+        <v>1.1179313697331372</v>
       </c>
       <c r="Y3" s="1">
         <f t="shared" ref="Y3:Y66" si="9">IF(W3="null","null",10*((W3-$AS3)/($AT3-$AS3)))</f>
@@ -2009,19 +2009,19 @@
       </c>
       <c r="AL3" s="1">
         <f t="shared" si="1"/>
-        <v>0.24428441434370188</v>
+        <v>0.24131528323184503</v>
       </c>
       <c r="AM3" s="1">
         <f t="shared" si="2"/>
-        <v>0.67128729116242203</v>
+        <v>0.67029762343460497</v>
       </c>
       <c r="AN3" s="1">
         <f t="shared" si="3"/>
-        <v>1.1168555104515212</v>
+        <v>1.1179313697331372</v>
       </c>
       <c r="AO3" s="1">
         <f t="shared" ref="AO3:AO12" si="14">AN3-AL3</f>
-        <v>0.87257109610781936</v>
+        <v>0.87661608650129219</v>
       </c>
       <c r="AP3" s="1" t="s">
         <v>38</v>
@@ -2103,7 +2103,7 @@
       </c>
       <c r="N4" s="1">
         <f t="shared" si="4"/>
-        <v>-0.66541736670487561</v>
+        <v>-0.67260361546099146</v>
       </c>
       <c r="O4" s="1">
         <f t="shared" si="5"/>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="S4" s="1">
         <f t="shared" si="6"/>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="T4" s="1">
         <f t="shared" si="7"/>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="X4" s="1">
         <f t="shared" si="8"/>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="Y4" s="1">
         <f t="shared" si="9"/>
@@ -2185,19 +2185,19 @@
       </c>
       <c r="AL4" s="1">
         <f t="shared" si="1"/>
-        <v>-0.66541736670487561</v>
+        <v>-0.67260361546099146</v>
       </c>
       <c r="AM4" s="1">
         <f t="shared" si="2"/>
-        <v>-0.62828668176411739</v>
+        <v>-0.63530080326944705</v>
       </c>
       <c r="AN4" s="1">
         <f t="shared" si="3"/>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="AO4" s="1">
         <f t="shared" si="14"/>
-        <v>5.5696027411137328E-2</v>
+        <v>5.5954218287316615E-2</v>
       </c>
       <c r="AP4" s="1" t="s">
         <v>38</v>
@@ -2276,7 +2276,7 @@
       </c>
       <c r="N5" s="1">
         <f t="shared" si="4"/>
-        <v>-0.85107079140866693</v>
+        <v>-0.85911767641871317</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" si="5"/>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="S5" s="1">
         <f t="shared" si="6"/>
-        <v>-0.90676681881980437</v>
+        <v>-0.91507189470602968</v>
       </c>
       <c r="T5" s="1">
         <f t="shared" si="7"/>
@@ -2310,7 +2310,7 @@
       </c>
       <c r="X5" s="1">
         <f t="shared" si="8"/>
-        <v>-0.7953747639975296</v>
+        <v>-0.80316345813139656</v>
       </c>
       <c r="Y5" s="1">
         <f t="shared" si="9"/>
@@ -2358,19 +2358,19 @@
       </c>
       <c r="AL5" s="1">
         <f t="shared" si="1"/>
-        <v>-0.90676681881980437</v>
+        <v>-0.91507189470602968</v>
       </c>
       <c r="AM5" s="1">
         <f t="shared" si="2"/>
-        <v>-0.85107079140866693</v>
+        <v>-0.85911767641871306</v>
       </c>
       <c r="AN5" s="1">
         <f t="shared" si="3"/>
-        <v>-0.7953747639975296</v>
+        <v>-0.80316345813139656</v>
       </c>
       <c r="AO5" s="1">
         <f t="shared" si="14"/>
-        <v>0.11139205482227477</v>
+        <v>0.11190843657463312</v>
       </c>
       <c r="AP5" s="1" t="s">
         <v>38</v>
@@ -2455,7 +2455,7 @@
       </c>
       <c r="N6" s="1">
         <f t="shared" si="4"/>
-        <v>-0.27554517482691387</v>
+        <v>-0.28092408744977576</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" si="5"/>
@@ -2472,7 +2472,7 @@
       </c>
       <c r="S6" s="1">
         <f t="shared" si="6"/>
-        <v>-1.5630380241605991E-2</v>
+        <v>-1.9804402108965374E-2</v>
       </c>
       <c r="T6" s="1">
         <f t="shared" si="7"/>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="X6" s="1">
         <f t="shared" si="8"/>
-        <v>5.8630989639910536E-2</v>
+        <v>5.4801222274123318E-2</v>
       </c>
       <c r="Y6" s="1">
         <f t="shared" si="9"/>
@@ -2537,19 +2537,19 @@
       </c>
       <c r="AL6" s="1">
         <f t="shared" si="1"/>
-        <v>-0.27554517482691387</v>
+        <v>-0.28092408744977576</v>
       </c>
       <c r="AM6" s="1">
         <f t="shared" si="2"/>
-        <v>-7.7514855142869779E-2</v>
+        <v>-8.1975755761539273E-2</v>
       </c>
       <c r="AN6" s="1">
         <f t="shared" si="3"/>
-        <v>5.8630989639910536E-2</v>
+        <v>5.4801222274123318E-2</v>
       </c>
       <c r="AO6" s="1">
         <f t="shared" si="14"/>
-        <v>0.33417616446682441</v>
+        <v>0.33572530972389908</v>
       </c>
       <c r="AP6" s="1" t="s">
         <v>38</v>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="N7" s="1">
         <f t="shared" si="4"/>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058624</v>
       </c>
       <c r="O7" s="1">
         <f t="shared" si="5"/>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="S7" s="1">
         <f t="shared" si="6"/>
-        <v>-0.20128380494539733</v>
+        <v>-0.20631846306668711</v>
       </c>
       <c r="T7" s="1">
         <f t="shared" si="7"/>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="X7" s="1">
         <f t="shared" si="8"/>
-        <v>-0.51689462694184252</v>
+        <v>-0.52339236669481404</v>
       </c>
       <c r="Y7" s="1">
         <f t="shared" si="9"/>
@@ -2713,19 +2713,19 @@
       </c>
       <c r="AL7" s="1">
         <f t="shared" si="1"/>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058624</v>
       </c>
       <c r="AM7" s="1">
         <f t="shared" si="2"/>
-        <v>-0.41787946709982055</v>
+        <v>-0.42391820085069581</v>
       </c>
       <c r="AN7" s="1">
         <f t="shared" si="3"/>
-        <v>-0.20128380494539733</v>
+        <v>-0.20631846306668711</v>
       </c>
       <c r="AO7" s="1">
         <f t="shared" si="14"/>
-        <v>0.33417616446682441</v>
+        <v>0.33572530972389913</v>
       </c>
       <c r="AP7" s="1" t="s">
         <v>38</v>
@@ -2804,7 +2804,7 @@
       </c>
       <c r="N8" s="1">
         <f t="shared" si="4"/>
-        <v>0.41137249657711406</v>
+        <v>0.4091779380937946</v>
       </c>
       <c r="O8" s="1">
         <f t="shared" si="5"/>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="S8" s="1">
         <f t="shared" si="6"/>
-        <v>1.0611594830403837</v>
+        <v>1.0619771514458207</v>
       </c>
       <c r="T8" s="1">
         <f t="shared" si="7"/>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="X8" s="1">
         <f t="shared" si="8"/>
-        <v>1.0240287980996254</v>
+        <v>1.0246743392542763</v>
       </c>
       <c r="Y8" s="1">
         <f t="shared" si="9"/>
@@ -2886,19 +2886,19 @@
       </c>
       <c r="AL8" s="1">
         <f t="shared" si="1"/>
-        <v>0.41137249657711406</v>
+        <v>0.4091779380937946</v>
       </c>
       <c r="AM8" s="1">
         <f t="shared" si="2"/>
-        <v>0.83218692590570775</v>
+        <v>0.83194314293129723</v>
       </c>
       <c r="AN8" s="1">
         <f t="shared" si="3"/>
-        <v>1.0611594830403837</v>
+        <v>1.0619771514458207</v>
       </c>
       <c r="AO8" s="1">
         <f t="shared" si="14"/>
-        <v>0.6497869864632696</v>
+        <v>0.65279921335202618</v>
       </c>
       <c r="AP8" s="1" t="s">
         <v>38</v>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="N9" s="1">
         <f t="shared" si="4"/>
-        <v>-0.85107079140866693</v>
+        <v>-0.85911767641871317</v>
       </c>
       <c r="O9" s="1">
         <f t="shared" si="5"/>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="S9" s="1">
         <f t="shared" si="6"/>
-        <v>-0.83250544893828782</v>
+        <v>-0.84046627032294097</v>
       </c>
       <c r="T9" s="1">
         <f t="shared" si="7"/>
@@ -3020,7 +3020,7 @@
       </c>
       <c r="X9" s="1">
         <f t="shared" si="8"/>
-        <v>-0.7953747639975296</v>
+        <v>-0.80316345813139656</v>
       </c>
       <c r="Y9" s="1">
         <f t="shared" si="9"/>
@@ -3068,19 +3068,19 @@
       </c>
       <c r="AL9" s="1">
         <f t="shared" si="1"/>
-        <v>-0.85107079140866693</v>
+        <v>-0.85911767641871317</v>
       </c>
       <c r="AM9" s="1">
         <f t="shared" si="2"/>
-        <v>-0.82631700144816145</v>
+        <v>-0.83424913495768349</v>
       </c>
       <c r="AN9" s="1">
         <f t="shared" si="3"/>
-        <v>-0.7953747639975296</v>
+        <v>-0.80316345813139656</v>
       </c>
       <c r="AO9" s="1">
         <f t="shared" si="14"/>
-        <v>5.5696027411137328E-2</v>
+        <v>5.5954218287316615E-2</v>
       </c>
       <c r="AP9" s="1" t="s">
         <v>38</v>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="N10" s="1">
         <f t="shared" si="4"/>
-        <v>-0.12702243506388078</v>
+        <v>-0.1317128386835984</v>
       </c>
       <c r="O10" s="1">
         <f t="shared" si="5"/>
@@ -3185,7 +3185,7 @@
       </c>
       <c r="S10" s="1">
         <f t="shared" si="6"/>
-        <v>-0.27554517482691387</v>
+        <v>-0.28092408744977576</v>
       </c>
       <c r="T10" s="1">
         <f t="shared" si="7"/>
@@ -3202,7 +3202,7 @@
       </c>
       <c r="X10" s="1">
         <f t="shared" si="8"/>
-        <v>-0.23841448988615557</v>
+        <v>-0.24362127525823143</v>
       </c>
       <c r="Y10" s="1">
         <f t="shared" si="9"/>
@@ -3250,19 +3250,19 @@
       </c>
       <c r="AL10" s="1">
         <f t="shared" si="1"/>
-        <v>-0.27554517482691387</v>
+        <v>-0.28092408744977576</v>
       </c>
       <c r="AM10" s="1">
         <f t="shared" si="2"/>
-        <v>-0.21366069992565007</v>
+        <v>-0.21875273379720186</v>
       </c>
       <c r="AN10" s="1">
         <f t="shared" si="3"/>
-        <v>-0.12702243506388078</v>
+        <v>-0.1317128386835984</v>
       </c>
       <c r="AO10" s="1">
         <f t="shared" si="14"/>
-        <v>0.1485227397630331</v>
+        <v>0.14921124876617736</v>
       </c>
       <c r="AP10" s="1" t="s">
         <v>38</v>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="N11" s="1">
         <f t="shared" si="4"/>
-        <v>1.9337305791482029</v>
+        <v>1.9385932379471127</v>
       </c>
       <c r="O11" s="1">
         <f t="shared" si="5"/>
@@ -3358,7 +3358,7 @@
       </c>
       <c r="S11" s="1">
         <f t="shared" si="6"/>
-        <v>1.3582049625664498</v>
+        <v>1.3603996489781753</v>
       </c>
       <c r="T11" s="1">
         <f t="shared" si="7"/>
@@ -3375,7 +3375,7 @@
       </c>
       <c r="X11" s="1">
         <f t="shared" si="8"/>
-        <v>1.2839435926849332</v>
+        <v>1.2857940245950867</v>
       </c>
       <c r="Y11" s="1">
         <f t="shared" si="9"/>
@@ -3423,19 +3423,19 @@
       </c>
       <c r="AL11" s="1">
         <f t="shared" si="1"/>
-        <v>1.2839435926849332</v>
+        <v>1.2857940245950867</v>
       </c>
       <c r="AM11" s="1">
         <f t="shared" si="2"/>
-        <v>1.5252930447998621</v>
+        <v>1.5282623038401251</v>
       </c>
       <c r="AN11" s="1">
         <f t="shared" si="3"/>
-        <v>1.9337305791482029</v>
+        <v>1.9385932379471127</v>
       </c>
       <c r="AO11" s="1">
         <f t="shared" si="14"/>
-        <v>0.64978698646326971</v>
+        <v>0.65279921335202595</v>
       </c>
       <c r="AP11" s="1" t="s">
         <v>38</v>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="N12" s="1">
         <f t="shared" si="4"/>
-        <v>-0.16415312000463905</v>
+        <v>-0.16901565087514275</v>
       </c>
       <c r="O12" s="1">
         <f t="shared" si="5"/>
@@ -3537,7 +3537,7 @@
       </c>
       <c r="S12" s="1">
         <f t="shared" si="6"/>
-        <v>0.3185457842252184</v>
+        <v>0.31592090761493374</v>
       </c>
       <c r="T12" s="1">
         <f t="shared" si="7"/>
@@ -3554,7 +3554,7 @@
       </c>
       <c r="X12" s="1">
         <f t="shared" si="8"/>
-        <v>0.65272194869204281</v>
+        <v>0.65164621733883288</v>
       </c>
       <c r="Y12" s="1">
         <f t="shared" si="9"/>
@@ -3602,19 +3602,19 @@
       </c>
       <c r="AL12" s="1">
         <f t="shared" si="1"/>
-        <v>-0.16415312000463905</v>
+        <v>-0.16901565087514275</v>
       </c>
       <c r="AM12" s="1">
         <f t="shared" si="2"/>
-        <v>0.26903820430420738</v>
+        <v>0.26618382469287466</v>
       </c>
       <c r="AN12" s="1">
         <f t="shared" si="3"/>
-        <v>0.65272194869204281</v>
+        <v>0.65164621733883288</v>
       </c>
       <c r="AO12" s="1">
         <f t="shared" si="14"/>
-        <v>0.81687506869668192</v>
+        <v>0.82066186821397569</v>
       </c>
       <c r="AP12" s="1" t="s">
         <v>38</v>
@@ -3874,7 +3874,7 @@
       </c>
       <c r="N14" s="1">
         <f t="shared" si="4"/>
-        <v>3.1404778397228466</v>
+        <v>3.1509346341723039</v>
       </c>
       <c r="O14" s="1">
         <f t="shared" si="5"/>
@@ -3891,7 +3891,7 @@
       </c>
       <c r="S14" s="1">
         <f t="shared" si="6"/>
-        <v>5.9624098952204756</v>
+        <v>5.9859483607296742</v>
       </c>
       <c r="T14" s="1">
         <f t="shared" si="7"/>
@@ -3908,7 +3908,7 @@
       </c>
       <c r="X14" s="1">
         <f t="shared" si="8"/>
-        <v>-0.75824407905677127</v>
+        <v>-0.76586064593985226</v>
       </c>
       <c r="Y14" s="1">
         <f t="shared" si="9"/>
@@ -3942,7 +3942,7 @@
       </c>
       <c r="AH14" s="1">
         <f t="shared" si="12"/>
-        <v>2.7877363327856428</v>
+        <v>2.7965579183526326</v>
       </c>
       <c r="AI14" s="1">
         <f t="shared" si="13"/>
@@ -3956,19 +3956,19 @@
       </c>
       <c r="AL14" s="1">
         <f>MIN(N14,S14,X14,AH14)</f>
-        <v>-0.75824407905677127</v>
+        <v>-0.76586064593985226</v>
       </c>
       <c r="AM14" s="1">
         <f>AVERAGE(N14,S14,X14,AH14)</f>
-        <v>2.7830949971680488</v>
+        <v>2.7918950668286895</v>
       </c>
       <c r="AN14" s="1">
         <f>MAX(N14,S14,X14,AH14)</f>
-        <v>5.9624098952204756</v>
+        <v>5.9859483607296742</v>
       </c>
       <c r="AO14" s="1">
         <f t="shared" ref="AO14" si="15">AN14-AL14</f>
-        <v>6.7206539742772469</v>
+        <v>6.7518090066695269</v>
       </c>
       <c r="AP14" s="1" t="s">
         <v>38</v>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="N15" s="1">
         <f t="shared" si="4"/>
-        <v>0.6341566062216637</v>
+        <v>0.63299481124306067</v>
       </c>
       <c r="O15" s="1">
         <f t="shared" si="5"/>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="S15" s="1">
         <f t="shared" si="6"/>
-        <v>1.8037731818555489</v>
+        <v>1.8080333952767076</v>
       </c>
       <c r="T15" s="1">
         <f t="shared" si="7"/>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="X15" s="1">
         <f t="shared" si="8"/>
-        <v>0.3185457842252184</v>
+        <v>0.31592090761493374</v>
       </c>
       <c r="Y15" s="1">
         <f t="shared" si="9"/>
@@ -4132,19 +4132,19 @@
       </c>
       <c r="AL15" s="1">
         <f>MIN(N15,S15,X15,AH15)</f>
-        <v>0.3185457842252184</v>
+        <v>0.31592090761493374</v>
       </c>
       <c r="AM15" s="1">
         <f>AVERAGE(N15,S15,X15,AH15)</f>
-        <v>0.91882519076747704</v>
+        <v>0.91898303804490056</v>
       </c>
       <c r="AN15" s="1">
         <f>MAX(N15,S15,X15,AH15)</f>
-        <v>1.8037731818555489</v>
+        <v>1.8080333952767076</v>
       </c>
       <c r="AO15" s="1">
         <f t="shared" ref="AO15:AO16" si="16">AN15-AL15</f>
-        <v>1.4852273976303305</v>
+        <v>1.4921124876617737</v>
       </c>
       <c r="AP15" s="1" t="s">
         <v>38</v>
@@ -4229,7 +4229,7 @@
       </c>
       <c r="N16" s="1">
         <f t="shared" si="4"/>
-        <v>-0.66541736670487561</v>
+        <v>-0.67260361546099146</v>
       </c>
       <c r="O16" s="1">
         <f t="shared" si="5"/>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="S16" s="1">
         <f t="shared" si="6"/>
-        <v>-0.55402531188260085</v>
+        <v>-0.56069517888635834</v>
       </c>
       <c r="T16" s="1">
         <f t="shared" si="7"/>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="X16" s="1">
         <f t="shared" si="8"/>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="Y16" s="1">
         <f t="shared" si="9"/>
@@ -4311,19 +4311,19 @@
       </c>
       <c r="AL16" s="1">
         <f>MIN(N16,S16,X16,AH16)</f>
-        <v>-0.66541736670487561</v>
+        <v>-0.67260361546099146</v>
       </c>
       <c r="AM16" s="1">
         <f>AVERAGE(N16,S16,X16,AH16)</f>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="AN16" s="1">
         <f>MAX(N16,S16,X16,AH16)</f>
-        <v>-0.55402531188260085</v>
+        <v>-0.56069517888635834</v>
       </c>
       <c r="AO16" s="1">
         <f t="shared" si="16"/>
-        <v>0.11139205482227477</v>
+        <v>0.11190843657463312</v>
       </c>
       <c r="AP16" s="1" t="s">
         <v>38</v>
@@ -4577,7 +4577,7 @@
       </c>
       <c r="N18" s="1">
         <f t="shared" si="4"/>
-        <v>0.13289235952142706</v>
+        <v>0.129406846657212</v>
       </c>
       <c r="O18" s="1">
         <f t="shared" si="5"/>
@@ -4594,7 +4594,7 @@
       </c>
       <c r="S18" s="1">
         <f t="shared" si="6"/>
-        <v>-0.36837188717880953</v>
+        <v>-0.37418111792863662</v>
       </c>
       <c r="T18" s="1">
         <f t="shared" si="7"/>
@@ -4611,7 +4611,7 @@
       </c>
       <c r="X18" s="1">
         <f t="shared" si="8"/>
-        <v>-0.38693722964918864</v>
+        <v>-0.39283252402440882</v>
       </c>
       <c r="Y18" s="1">
         <f t="shared" si="9"/>
@@ -4645,7 +4645,7 @@
       </c>
       <c r="AH18" s="1">
         <f t="shared" si="12"/>
-        <v>-8.9891750123122519E-2</v>
+        <v>-9.4410026492054058E-2</v>
       </c>
       <c r="AI18" s="1">
         <f t="shared" si="13"/>
@@ -4659,19 +4659,19 @@
       </c>
       <c r="AL18" s="1">
         <f>MIN(N18,S18,X18,AH18)</f>
-        <v>-0.38693722964918864</v>
+        <v>-0.39283252402440882</v>
       </c>
       <c r="AM18" s="1">
         <f>AVERAGE(N18,S18,X18,AH18)</f>
-        <v>-0.17807712685742341</v>
+        <v>-0.18300420544697188</v>
       </c>
       <c r="AN18" s="1">
         <f>MAX(N18,S18,X18,AH18)</f>
-        <v>0.13289235952142706</v>
+        <v>0.129406846657212</v>
       </c>
       <c r="AO18" s="1">
         <f t="shared" ref="AO18" si="17">AN18-AL18</f>
-        <v>0.51982958917061572</v>
+        <v>0.52223937068162085</v>
       </c>
       <c r="AP18" s="1" t="s">
         <v>38</v>
@@ -5091,7 +5091,7 @@
       </c>
       <c r="N21" s="1">
         <f t="shared" si="4"/>
-        <v>-0.42406791458994691</v>
+        <v>-0.43013533621595318</v>
       </c>
       <c r="O21" s="1">
         <f t="shared" si="5"/>
@@ -5125,7 +5125,7 @@
       </c>
       <c r="X21" s="1">
         <f t="shared" si="8"/>
-        <v>-0.14558777753425992</v>
+        <v>-0.15036424477937058</v>
       </c>
       <c r="Y21" s="1">
         <f t="shared" si="9"/>
@@ -5173,19 +5173,19 @@
       </c>
       <c r="AL21" s="1">
         <f>MIN(N21,S21,X21,AH21)</f>
-        <v>-0.42406791458994691</v>
+        <v>-0.43013533621595318</v>
       </c>
       <c r="AM21" s="1">
         <f>AVERAGE(N21,S21,X21,AH21)</f>
-        <v>-0.28482784606210343</v>
+        <v>-0.29024979049766186</v>
       </c>
       <c r="AN21" s="1">
         <f>MAX(N21,S21,X21,AH21)</f>
-        <v>-0.14558777753425992</v>
+        <v>-0.15036424477937058</v>
       </c>
       <c r="AO21" s="1">
         <f t="shared" ref="AO21" si="18">AN21-AL21</f>
-        <v>0.27848013705568697</v>
+        <v>0.27977109143658263</v>
       </c>
       <c r="AP21" s="1" t="s">
         <v>39</v>
@@ -5264,7 +5264,7 @@
       </c>
       <c r="N22" s="1">
         <f t="shared" si="4"/>
-        <v>-0.90676681881980437</v>
+        <v>-0.91507189470602968</v>
       </c>
       <c r="O22" s="1">
         <f t="shared" si="5"/>
@@ -5281,7 +5281,7 @@
       </c>
       <c r="S22" s="1">
         <f t="shared" si="6"/>
-        <v>-0.86963613387904604</v>
+        <v>-0.87776908251448527</v>
       </c>
       <c r="T22" s="1">
         <f t="shared" si="7"/>
@@ -5298,7 +5298,7 @@
       </c>
       <c r="X22" s="1">
         <f t="shared" si="8"/>
-        <v>-0.88820147634942526</v>
+        <v>-0.89642048861025747</v>
       </c>
       <c r="Y22" s="1">
         <f t="shared" si="9"/>
@@ -5332,7 +5332,7 @@
       </c>
       <c r="AH22" s="1">
         <f t="shared" si="12"/>
-        <v>-0.92533216129018347</v>
+        <v>-0.93372330080180177</v>
       </c>
       <c r="AI22" s="1">
         <f t="shared" si="13"/>
@@ -5346,19 +5346,19 @@
       </c>
       <c r="AL22" s="1">
         <f>MIN(N22,S22,X22,AH22)</f>
-        <v>-0.92533216129018347</v>
+        <v>-0.93372330080180177</v>
       </c>
       <c r="AM22" s="1">
         <f>AVERAGE(N22,S22,X22,AH22)</f>
-        <v>-0.89748414758461481</v>
+        <v>-0.90574619165814352</v>
       </c>
       <c r="AN22" s="1">
         <f>MAX(N22,S22,X22,AH22)</f>
-        <v>-0.86963613387904604</v>
+        <v>-0.87776908251448527</v>
       </c>
       <c r="AO22" s="1">
         <f t="shared" ref="AO22" si="19">AN22-AL22</f>
-        <v>5.5696027411137439E-2</v>
+        <v>5.5954218287316504E-2</v>
       </c>
       <c r="AP22" s="1" t="s">
         <v>38</v>
@@ -5807,7 +5807,7 @@
       </c>
       <c r="S25" s="1">
         <f t="shared" si="6"/>
-        <v>-1.0367242161124584</v>
+        <v>-1.0456317373764348</v>
       </c>
       <c r="T25" s="1">
         <f t="shared" si="7"/>
@@ -5824,7 +5824,7 @@
       </c>
       <c r="X25" s="1">
         <f t="shared" si="8"/>
-        <v>-0.46119859953070519</v>
+        <v>-0.46743814840749753</v>
       </c>
       <c r="Y25" s="1">
         <f t="shared" si="9"/>
@@ -5872,19 +5872,19 @@
       </c>
       <c r="AL25" s="1">
         <f>MIN(N25,S25,X25,AH25)</f>
-        <v>-1.0367242161124584</v>
+        <v>-1.0456317373764348</v>
       </c>
       <c r="AM25" s="1">
         <f>AVERAGE(N25,S25,X25,AH25)</f>
-        <v>-0.74896140782158183</v>
+        <v>-0.7565349428919661</v>
       </c>
       <c r="AN25" s="1">
         <f>MAX(N25,S25,X25,AH25)</f>
-        <v>-0.46119859953070519</v>
+        <v>-0.46743814840749753</v>
       </c>
       <c r="AO25" s="1">
         <f t="shared" ref="AO25" si="20">AN25-AL25</f>
-        <v>0.57552561658175316</v>
+        <v>0.57819358896893724</v>
       </c>
       <c r="AP25" s="1" t="s">
         <v>39</v>
@@ -5969,7 +5969,7 @@
       </c>
       <c r="N26" s="1">
         <f t="shared" si="4"/>
-        <v>-0.12702243506388078</v>
+        <v>-0.1317128386835984</v>
       </c>
       <c r="O26" s="1">
         <f t="shared" si="5"/>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="S26" s="1">
         <f t="shared" si="6"/>
-        <v>5.8630989639910536E-2</v>
+        <v>5.4801222274123318E-2</v>
       </c>
       <c r="T26" s="1">
         <f t="shared" si="7"/>
@@ -6003,7 +6003,7 @@
       </c>
       <c r="X26" s="1">
         <f t="shared" si="8"/>
-        <v>-0.18271846247501819</v>
+        <v>-0.18766705697091493</v>
       </c>
       <c r="Y26" s="1">
         <f t="shared" si="9"/>
@@ -6051,19 +6051,19 @@
       </c>
       <c r="AL26" s="1">
         <f>MIN(N26,S26,X26,AH26)</f>
-        <v>-0.18271846247501819</v>
+        <v>-0.18766705697091493</v>
       </c>
       <c r="AM26" s="1">
         <f>AVERAGE(N26,S26,X26,AH26)</f>
-        <v>-8.3703302632996149E-2</v>
+        <v>-8.8192891126796666E-2</v>
       </c>
       <c r="AN26" s="1">
         <f>MAX(N26,S26,X26,AH26)</f>
-        <v>5.8630989639910536E-2</v>
+        <v>5.4801222274123318E-2</v>
       </c>
       <c r="AO26" s="1">
         <f t="shared" ref="AO26" si="21">AN26-AL26</f>
-        <v>0.24134945211492873</v>
+        <v>0.24246827924503825</v>
       </c>
       <c r="AP26" s="1" t="s">
         <v>38</v>
@@ -6323,7 +6323,7 @@
       </c>
       <c r="N28" s="1">
         <f t="shared" si="4"/>
-        <v>0.52276455139938882</v>
+        <v>0.52108637466842767</v>
       </c>
       <c r="O28" s="1">
         <f t="shared" si="5"/>
@@ -6340,7 +6340,7 @@
       </c>
       <c r="S28" s="1">
         <f t="shared" si="6"/>
-        <v>1.9151652366778238</v>
+        <v>1.9199418318513406</v>
       </c>
       <c r="T28" s="1">
         <f t="shared" si="7"/>
@@ -6357,7 +6357,7 @@
       </c>
       <c r="X28" s="1">
         <f t="shared" si="8"/>
-        <v>1.9894266065593402</v>
+        <v>1.9945474562344292</v>
       </c>
       <c r="Y28" s="1">
         <f t="shared" si="9"/>
@@ -6405,19 +6405,19 @@
       </c>
       <c r="AL28" s="1">
         <f>MIN(N28,S28,X28,AH28)</f>
-        <v>0.52276455139938882</v>
+        <v>0.52108637466842767</v>
       </c>
       <c r="AM28" s="1">
         <f>AVERAGE(N28,S28,X28,AH28)</f>
-        <v>1.4757854648788511</v>
+        <v>1.4785252209180657</v>
       </c>
       <c r="AN28" s="1">
         <f>MAX(N28,S28,X28,AH28)</f>
-        <v>1.9894266065593402</v>
+        <v>1.9945474562344292</v>
       </c>
       <c r="AO28" s="1">
         <f t="shared" ref="AO28" si="22">AN28-AL28</f>
-        <v>1.4666620551599514</v>
+        <v>1.4734610815660014</v>
       </c>
       <c r="AP28" s="1" t="s">
         <v>38</v>
@@ -6671,7 +6671,7 @@
       </c>
       <c r="N30" s="1">
         <f t="shared" si="4"/>
-        <v>-0.21984914741577646</v>
+        <v>-0.22496986916245926</v>
       </c>
       <c r="O30" s="1">
         <f t="shared" si="5"/>
@@ -6688,7 +6688,7 @@
       </c>
       <c r="S30" s="1">
         <f t="shared" si="6"/>
-        <v>-0.21984914741577646</v>
+        <v>-0.22496986916245926</v>
       </c>
       <c r="T30" s="1">
         <f t="shared" si="7"/>
@@ -6705,7 +6705,7 @@
       </c>
       <c r="X30" s="1">
         <f t="shared" si="8"/>
-        <v>-0.21984914741577646</v>
+        <v>-0.22496986916245926</v>
       </c>
       <c r="Y30" s="1">
         <f t="shared" si="9"/>
@@ -6739,7 +6739,7 @@
       </c>
       <c r="AH30" s="1">
         <f t="shared" si="12"/>
-        <v>-0.27554517482691387</v>
+        <v>-0.28092408744977576</v>
       </c>
       <c r="AI30" s="1">
         <f t="shared" si="13"/>
@@ -6753,19 +6753,19 @@
       </c>
       <c r="AL30" s="1">
         <f>MIN(N30,S30,X30,AH30)</f>
-        <v>-0.27554517482691387</v>
+        <v>-0.28092408744977576</v>
       </c>
       <c r="AM30" s="1">
         <f>AVERAGE(N30,S30,X30,AH30)</f>
-        <v>-0.23377315426856082</v>
+        <v>-0.23895842373428838</v>
       </c>
       <c r="AN30" s="1">
         <f>MAX(N30,S30,X30,AH30)</f>
-        <v>-0.21984914741577646</v>
+        <v>-0.22496986916245926</v>
       </c>
       <c r="AO30" s="1">
         <f t="shared" ref="AO30" si="23">AN30-AL30</f>
-        <v>5.5696027411137411E-2</v>
+        <v>5.5954218287316504E-2</v>
       </c>
       <c r="AP30" s="1" t="s">
         <v>38</v>
@@ -7191,7 +7191,7 @@
       </c>
       <c r="N33" s="1">
         <f t="shared" si="4"/>
-        <v>3.1219124972524672</v>
+        <v>3.1322832280765316</v>
       </c>
       <c r="O33" s="1">
         <f t="shared" si="5"/>
@@ -7208,7 +7208,7 @@
       </c>
       <c r="S33" s="1">
         <f t="shared" si="6"/>
-        <v>3.0290857849005719</v>
+        <v>3.0390261975976709</v>
       </c>
       <c r="T33" s="1">
         <f t="shared" si="7"/>
@@ -7225,7 +7225,7 @@
       </c>
       <c r="X33" s="1">
         <f t="shared" si="8"/>
-        <v>3.5117846891304292</v>
+        <v>3.5239627560877476</v>
       </c>
       <c r="Y33" s="1">
         <f t="shared" si="9"/>
@@ -7273,19 +7273,19 @@
       </c>
       <c r="AL33" s="1">
         <f t="shared" ref="AL33:AL47" si="24">MIN(N33,S33,X33,AH33)</f>
-        <v>3.0290857849005719</v>
+        <v>3.0390261975976709</v>
       </c>
       <c r="AM33" s="1">
         <f t="shared" ref="AM33:AM47" si="25">AVERAGE(N33,S33,X33,AH33)</f>
-        <v>3.2209276570944891</v>
+        <v>3.2317573939206503</v>
       </c>
       <c r="AN33" s="1">
         <f t="shared" ref="AN33:AN47" si="26">MAX(N33,S33,X33,AH33)</f>
-        <v>3.5117846891304292</v>
+        <v>3.5239627560877476</v>
       </c>
       <c r="AO33" s="1">
         <f t="shared" ref="AO33" si="27">AN33-AL33</f>
-        <v>0.48269890422985728</v>
+        <v>0.48493655849007666</v>
       </c>
       <c r="AP33" s="1" t="s">
         <v>38</v>
@@ -7367,7 +7367,7 @@
       </c>
       <c r="N34" s="1">
         <f t="shared" si="4"/>
-        <v>-0.21984914741577646</v>
+        <v>-0.22496986916245926</v>
       </c>
       <c r="O34" s="1">
         <f t="shared" si="5"/>
@@ -7384,7 +7384,7 @@
       </c>
       <c r="S34" s="1">
         <f t="shared" si="6"/>
-        <v>-5.2761065182364258E-2</v>
+        <v>-5.7107214300509718E-2</v>
       </c>
       <c r="T34" s="1">
         <f t="shared" si="7"/>
@@ -7401,7 +7401,7 @@
       </c>
       <c r="X34" s="1">
         <f t="shared" si="8"/>
-        <v>0.54132989386976793</v>
+        <v>0.53973778076419976</v>
       </c>
       <c r="Y34" s="1">
         <f t="shared" si="9"/>
@@ -7435,7 +7435,7 @@
       </c>
       <c r="AH34" s="1">
         <f t="shared" si="12"/>
-        <v>7.7196332110289673E-2</v>
+        <v>7.3452628369895495E-2</v>
       </c>
       <c r="AI34" s="1">
         <f t="shared" si="13"/>
@@ -7449,19 +7449,19 @@
       </c>
       <c r="AL34" s="1">
         <f t="shared" si="24"/>
-        <v>-0.21984914741577646</v>
+        <v>-0.22496986916245926</v>
       </c>
       <c r="AM34" s="1">
         <f t="shared" si="25"/>
-        <v>8.6479003345479227E-2</v>
+        <v>8.277833141778157E-2</v>
       </c>
       <c r="AN34" s="1">
         <f t="shared" si="26"/>
-        <v>0.54132989386976793</v>
+        <v>0.53973778076419976</v>
       </c>
       <c r="AO34" s="1">
         <f t="shared" ref="AO34:AO47" si="28">AN34-AL34</f>
-        <v>0.76117904128554437</v>
+        <v>0.76470764992665896</v>
       </c>
       <c r="AP34" s="1" t="s">
         <v>38</v>
@@ -7549,7 +7549,7 @@
       </c>
       <c r="N35" s="1">
         <f t="shared" si="4"/>
-        <v>0.26284975681408101</v>
+        <v>0.25996668932761718</v>
       </c>
       <c r="O35" s="1">
         <f t="shared" si="5"/>
@@ -7566,7 +7566,7 @@
       </c>
       <c r="S35" s="1">
         <f t="shared" si="6"/>
-        <v>0.4856338664586306</v>
+        <v>0.48378356247688326</v>
       </c>
       <c r="T35" s="1">
         <f t="shared" si="7"/>
@@ -7583,7 +7583,7 @@
       </c>
       <c r="X35" s="1">
         <f t="shared" si="8"/>
-        <v>0.24428441434370188</v>
+        <v>0.24131528323184503</v>
       </c>
       <c r="Y35" s="1">
         <f t="shared" si="9"/>
@@ -7631,19 +7631,19 @@
       </c>
       <c r="AL35" s="1">
         <f t="shared" si="24"/>
-        <v>0.24428441434370188</v>
+        <v>0.24131528323184503</v>
       </c>
       <c r="AM35" s="1">
         <f t="shared" si="25"/>
-        <v>0.33092267920547119</v>
+        <v>0.32835517834544853</v>
       </c>
       <c r="AN35" s="1">
         <f t="shared" si="26"/>
-        <v>0.4856338664586306</v>
+        <v>0.48378356247688326</v>
       </c>
       <c r="AO35" s="1">
         <f t="shared" si="28"/>
-        <v>0.24134945211492873</v>
+        <v>0.24246827924503822</v>
       </c>
       <c r="AP35" s="1" t="s">
         <v>38</v>
@@ -7728,7 +7728,7 @@
       </c>
       <c r="N36" s="1">
         <f t="shared" si="4"/>
-        <v>-0.55402531188260085</v>
+        <v>-0.56069517888635834</v>
       </c>
       <c r="O36" s="1">
         <f t="shared" si="5"/>
@@ -7762,7 +7762,7 @@
       </c>
       <c r="X36" s="1">
         <f t="shared" si="8"/>
-        <v>-0.46119859953070519</v>
+        <v>-0.46743814840749753</v>
       </c>
       <c r="Y36" s="1">
         <f t="shared" si="9"/>
@@ -7796,7 +7796,7 @@
       </c>
       <c r="AH36" s="1">
         <f t="shared" si="12"/>
-        <v>-0.4797639420010843</v>
+        <v>-0.48608955450326968</v>
       </c>
       <c r="AI36" s="1">
         <f t="shared" si="13"/>
@@ -7810,19 +7810,19 @@
       </c>
       <c r="AL36" s="1">
         <f t="shared" si="24"/>
-        <v>-0.55402531188260085</v>
+        <v>-0.56069517888635834</v>
       </c>
       <c r="AM36" s="1">
         <f t="shared" si="25"/>
-        <v>-0.49832928447146346</v>
+        <v>-0.50474096059904194</v>
       </c>
       <c r="AN36" s="1">
         <f t="shared" si="26"/>
-        <v>-0.46119859953070519</v>
+        <v>-0.46743814840749753</v>
       </c>
       <c r="AO36" s="1">
         <f t="shared" si="28"/>
-        <v>9.2826712351895657E-2</v>
+        <v>9.3257030478860803E-2</v>
       </c>
       <c r="AP36" s="1" t="s">
         <v>39</v>
@@ -7898,7 +7898,7 @@
       </c>
       <c r="N37" s="1">
         <f t="shared" si="4"/>
-        <v>0.44850318151787233</v>
+        <v>0.44648075028533896</v>
       </c>
       <c r="O37" s="1">
         <f t="shared" si="5"/>
@@ -7932,7 +7932,7 @@
       </c>
       <c r="X37" s="1">
         <f t="shared" si="8"/>
-        <v>0.89407140080697145</v>
+        <v>0.8941144965838711</v>
       </c>
       <c r="Y37" s="1">
         <f t="shared" si="9"/>
@@ -7966,7 +7966,7 @@
       </c>
       <c r="AH37" s="1">
         <f t="shared" si="12"/>
-        <v>0.3185457842252184</v>
+        <v>0.31592090761493374</v>
       </c>
       <c r="AI37" s="1">
         <f t="shared" si="13"/>
@@ -7980,19 +7980,19 @@
       </c>
       <c r="AL37" s="1">
         <f t="shared" si="24"/>
-        <v>0.3185457842252184</v>
+        <v>0.31592090761493374</v>
       </c>
       <c r="AM37" s="1">
         <f t="shared" si="25"/>
-        <v>0.55370678885002078</v>
+        <v>0.55217205149471449</v>
       </c>
       <c r="AN37" s="1">
         <f t="shared" si="26"/>
-        <v>0.89407140080697145</v>
+        <v>0.8941144965838711</v>
       </c>
       <c r="AO37" s="1">
         <f t="shared" si="28"/>
-        <v>0.57552561658175305</v>
+        <v>0.57819358896893736</v>
       </c>
       <c r="AP37" s="1" t="s">
         <v>39</v>
@@ -8068,7 +8068,7 @@
       </c>
       <c r="N38" s="1">
         <f t="shared" si="4"/>
-        <v>0.59702592128090537</v>
+        <v>0.59569199905151626</v>
       </c>
       <c r="O38" s="1">
         <f t="shared" si="5"/>
@@ -8085,7 +8085,7 @@
       </c>
       <c r="S38" s="1">
         <f t="shared" si="6"/>
-        <v>1.5809890722109994</v>
+        <v>1.5842165221274414</v>
       </c>
       <c r="T38" s="1">
         <f t="shared" si="7"/>
@@ -8102,7 +8102,7 @@
       </c>
       <c r="X38" s="1">
         <f t="shared" si="8"/>
-        <v>1.5624237297406203</v>
+        <v>1.5655651160316693</v>
       </c>
       <c r="Y38" s="1">
         <f t="shared" si="9"/>
@@ -8150,19 +8150,19 @@
       </c>
       <c r="AL38" s="1">
         <f t="shared" si="24"/>
-        <v>0.59702592128090537</v>
+        <v>0.59569199905151626</v>
       </c>
       <c r="AM38" s="1">
         <f t="shared" si="25"/>
-        <v>1.246812907744175</v>
+        <v>1.2484912124035423</v>
       </c>
       <c r="AN38" s="1">
         <f t="shared" si="26"/>
-        <v>1.5809890722109994</v>
+        <v>1.5842165221274414</v>
       </c>
       <c r="AO38" s="1">
         <f t="shared" si="28"/>
-        <v>0.98396315093009401</v>
+        <v>0.98852452307592509</v>
       </c>
       <c r="AP38" s="1" t="s">
         <v>38</v>
@@ -8250,7 +8250,7 @@
       </c>
       <c r="N39" s="1">
         <f t="shared" si="4"/>
-        <v>-0.59115599682335906</v>
+        <v>-0.59799799107790275</v>
       </c>
       <c r="O39" s="1">
         <f t="shared" si="5"/>
@@ -8267,7 +8267,7 @@
       </c>
       <c r="S39" s="1">
         <f t="shared" si="6"/>
-        <v>-0.59115599682335906</v>
+        <v>-0.59799799107790275</v>
       </c>
       <c r="T39" s="1">
         <f t="shared" si="7"/>
@@ -8284,7 +8284,7 @@
       </c>
       <c r="X39" s="1">
         <f t="shared" si="8"/>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="Y39" s="1">
         <f t="shared" si="9"/>
@@ -8332,19 +8332,19 @@
       </c>
       <c r="AL39" s="1">
         <f t="shared" si="24"/>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="AM39" s="1">
         <f t="shared" si="25"/>
-        <v>-0.59734444431348555</v>
+        <v>-0.60421512644316011</v>
       </c>
       <c r="AN39" s="1">
         <f t="shared" si="26"/>
-        <v>-0.59115599682335906</v>
+        <v>-0.59799799107790275</v>
       </c>
       <c r="AO39" s="1">
         <f t="shared" si="28"/>
-        <v>1.856534247037922E-2</v>
+        <v>1.8651406095772094E-2</v>
       </c>
       <c r="AP39" s="1" t="s">
         <v>38</v>
@@ -8432,7 +8432,7 @@
       </c>
       <c r="N40" s="1">
         <f t="shared" si="4"/>
-        <v>-0.92533216129018347</v>
+        <v>-0.93372330080180177</v>
       </c>
       <c r="O40" s="1">
         <f t="shared" si="5"/>
@@ -8449,7 +8449,7 @@
       </c>
       <c r="S40" s="1">
         <f t="shared" si="6"/>
-        <v>-0.92533216129018347</v>
+        <v>-0.93372330080180177</v>
       </c>
       <c r="T40" s="1">
         <f t="shared" si="7"/>
@@ -8466,7 +8466,7 @@
       </c>
       <c r="X40" s="1">
         <f t="shared" si="8"/>
-        <v>-0.88820147634942526</v>
+        <v>-0.89642048861025747</v>
       </c>
       <c r="Y40" s="1">
         <f t="shared" si="9"/>
@@ -8514,19 +8514,19 @@
       </c>
       <c r="AL40" s="1">
         <f t="shared" si="24"/>
-        <v>-0.92533216129018347</v>
+        <v>-0.93372330080180177</v>
       </c>
       <c r="AM40" s="1">
         <f t="shared" si="25"/>
-        <v>-0.91295526630993074</v>
+        <v>-0.92128903007128704</v>
       </c>
       <c r="AN40" s="1">
         <f t="shared" si="26"/>
-        <v>-0.88820147634942526</v>
+        <v>-0.89642048861025747</v>
       </c>
       <c r="AO40" s="1">
         <f t="shared" si="28"/>
-        <v>3.7130684940758218E-2</v>
+        <v>3.7302812191544299E-2</v>
       </c>
       <c r="AP40" s="1" t="s">
         <v>38</v>
@@ -8605,7 +8605,7 @@
       </c>
       <c r="N41" s="1">
         <f t="shared" si="4"/>
-        <v>0.37424181163635578</v>
+        <v>0.37187512590225025</v>
       </c>
       <c r="O41" s="1">
         <f t="shared" si="5"/>
@@ -8622,7 +8622,7 @@
       </c>
       <c r="S41" s="1">
         <f t="shared" si="6"/>
-        <v>1.1539861953922794</v>
+        <v>1.1552341819246814</v>
       </c>
       <c r="T41" s="1">
         <f t="shared" si="7"/>
@@ -8639,7 +8639,7 @@
       </c>
       <c r="X41" s="1">
         <f t="shared" si="8"/>
-        <v>0.80124468845507579</v>
+        <v>0.80085746610501019</v>
       </c>
       <c r="Y41" s="1">
         <f t="shared" si="9"/>
@@ -8687,19 +8687,19 @@
       </c>
       <c r="AL41" s="1">
         <f t="shared" si="24"/>
-        <v>0.37424181163635578</v>
+        <v>0.37187512590225025</v>
       </c>
       <c r="AM41" s="1">
         <f t="shared" si="25"/>
-        <v>0.77649089849457031</v>
+        <v>0.77598892464398073</v>
       </c>
       <c r="AN41" s="1">
         <f t="shared" si="26"/>
-        <v>1.1539861953922794</v>
+        <v>1.1552341819246814</v>
       </c>
       <c r="AO41" s="1">
         <f t="shared" si="28"/>
-        <v>0.7797443837559237</v>
+        <v>0.78335905602243117</v>
       </c>
       <c r="AP41" s="1" t="s">
         <v>38</v>
@@ -8781,7 +8781,7 @@
       </c>
       <c r="N42" s="1">
         <f t="shared" si="4"/>
-        <v>-0.29411051729729298</v>
+        <v>-0.29957549354554797</v>
       </c>
       <c r="O42" s="1">
         <f t="shared" si="5"/>
@@ -8798,7 +8798,7 @@
       </c>
       <c r="S42" s="1">
         <f t="shared" si="6"/>
-        <v>-7.1326407652743395E-2</v>
+        <v>-7.5758620396281895E-2</v>
       </c>
       <c r="T42" s="1">
         <f t="shared" si="7"/>
@@ -8815,7 +8815,7 @@
       </c>
       <c r="X42" s="1">
         <f t="shared" si="8"/>
-        <v>-1.5630380241605991E-2</v>
+        <v>-1.9804402108965374E-2</v>
       </c>
       <c r="Y42" s="1">
         <f t="shared" si="9"/>
@@ -8863,19 +8863,19 @@
       </c>
       <c r="AL42" s="1">
         <f t="shared" si="24"/>
-        <v>-0.29411051729729298</v>
+        <v>-0.29957549354554797</v>
       </c>
       <c r="AM42" s="1">
         <f t="shared" si="25"/>
-        <v>-0.12702243506388081</v>
+        <v>-0.13171283868359843</v>
       </c>
       <c r="AN42" s="1">
         <f t="shared" si="26"/>
-        <v>-1.5630380241605991E-2</v>
+        <v>-1.9804402108965374E-2</v>
       </c>
       <c r="AO42" s="1">
         <f t="shared" si="28"/>
-        <v>0.27848013705568697</v>
+        <v>0.27977109143658258</v>
       </c>
       <c r="AP42" s="1" t="s">
         <v>38</v>
@@ -8963,7 +8963,7 @@
       </c>
       <c r="N43" s="1">
         <f t="shared" si="4"/>
-        <v>2.379298798437302</v>
+        <v>2.3862269842456447</v>
       </c>
       <c r="O43" s="1">
         <f t="shared" si="5"/>
@@ -8980,7 +8980,7 @@
       </c>
       <c r="S43" s="1">
         <f t="shared" si="6"/>
-        <v>1.952295921618582</v>
+        <v>1.9572446440428848</v>
       </c>
       <c r="T43" s="1">
         <f t="shared" si="7"/>
@@ -8997,7 +8997,7 @@
       </c>
       <c r="X43" s="1">
         <f t="shared" si="8"/>
-        <v>1.5252930447998621</v>
+        <v>1.5282623038401248</v>
       </c>
       <c r="Y43" s="1">
         <f t="shared" si="9"/>
@@ -9045,19 +9045,19 @@
       </c>
       <c r="AL43" s="1">
         <f t="shared" si="24"/>
-        <v>1.5252930447998621</v>
+        <v>1.5282623038401248</v>
       </c>
       <c r="AM43" s="1">
         <f t="shared" si="25"/>
-        <v>1.952295921618582</v>
+        <v>1.9572446440428848</v>
       </c>
       <c r="AN43" s="1">
         <f t="shared" si="26"/>
-        <v>2.379298798437302</v>
+        <v>2.3862269842456447</v>
       </c>
       <c r="AO43" s="1">
         <f t="shared" si="28"/>
-        <v>0.85400575363743991</v>
+        <v>0.85796468040551987</v>
       </c>
       <c r="AP43" s="1" t="s">
         <v>38</v>
@@ -9151,7 +9151,7 @@
       </c>
       <c r="N44" s="1">
         <f t="shared" si="4"/>
-        <v>0.83837537339583412</v>
+        <v>0.8381602782965546</v>
       </c>
       <c r="O44" s="1">
         <f t="shared" si="5"/>
@@ -9168,7 +9168,7 @@
       </c>
       <c r="S44" s="1">
         <f t="shared" si="6"/>
-        <v>0.70841797610318014</v>
+        <v>0.70760043562614938</v>
       </c>
       <c r="T44" s="1">
         <f t="shared" si="7"/>
@@ -9185,7 +9185,7 @@
       </c>
       <c r="X44" s="1">
         <f t="shared" si="8"/>
-        <v>0.24428441434370188</v>
+        <v>0.24131528323184503</v>
       </c>
       <c r="Y44" s="1">
         <f t="shared" si="9"/>
@@ -9233,19 +9233,19 @@
       </c>
       <c r="AL44" s="1">
         <f t="shared" si="24"/>
-        <v>0.24428441434370188</v>
+        <v>0.24131528323184503</v>
       </c>
       <c r="AM44" s="1">
         <f t="shared" si="25"/>
-        <v>0.59702592128090537</v>
+        <v>0.59569199905151637</v>
       </c>
       <c r="AN44" s="1">
         <f t="shared" si="26"/>
-        <v>0.83837537339583412</v>
+        <v>0.8381602782965546</v>
       </c>
       <c r="AO44" s="1">
         <f t="shared" si="28"/>
-        <v>0.59409095905213227</v>
+        <v>0.59684499506470956</v>
       </c>
       <c r="AP44" s="1" t="s">
         <v>38</v>
@@ -9330,7 +9330,7 @@
       </c>
       <c r="N45" s="1">
         <f t="shared" si="4"/>
-        <v>-0.42406791458994691</v>
+        <v>-0.43013533621595318</v>
       </c>
       <c r="O45" s="1">
         <f t="shared" si="5"/>
@@ -9347,7 +9347,7 @@
       </c>
       <c r="S45" s="1">
         <f t="shared" si="6"/>
-        <v>-0.36837188717880953</v>
+        <v>-0.37418111792863662</v>
       </c>
       <c r="T45" s="1">
         <f t="shared" si="7"/>
@@ -9364,7 +9364,7 @@
       </c>
       <c r="X45" s="1">
         <f t="shared" si="8"/>
-        <v>-0.34980654470843037</v>
+        <v>-0.35552971183286447</v>
       </c>
       <c r="Y45" s="1">
         <f t="shared" si="9"/>
@@ -9412,19 +9412,19 @@
       </c>
       <c r="AL45" s="1">
         <f t="shared" si="24"/>
-        <v>-0.42406791458994691</v>
+        <v>-0.43013533621595318</v>
       </c>
       <c r="AM45" s="1">
         <f t="shared" si="25"/>
-        <v>-0.38074878215906227</v>
+        <v>-0.3866153886591514</v>
       </c>
       <c r="AN45" s="1">
         <f t="shared" si="26"/>
-        <v>-0.34980654470843037</v>
+        <v>-0.35552971183286447</v>
       </c>
       <c r="AO45" s="1">
         <f t="shared" si="28"/>
-        <v>7.4261369881516548E-2</v>
+        <v>7.4605624383088709E-2</v>
       </c>
       <c r="AP45" s="1" t="s">
         <v>38</v>
@@ -9512,7 +9512,7 @@
       </c>
       <c r="N46" s="1">
         <f t="shared" si="4"/>
-        <v>-0.23841448988615557</v>
+        <v>-0.24362127525823143</v>
       </c>
       <c r="O46" s="1">
         <f t="shared" si="5"/>
@@ -9529,7 +9529,7 @@
       </c>
       <c r="S46" s="1">
         <f t="shared" si="6"/>
-        <v>-3.4195722711985121E-2</v>
+        <v>-3.8455808204737547E-2</v>
       </c>
       <c r="T46" s="1">
         <f t="shared" si="7"/>
@@ -9546,7 +9546,7 @@
       </c>
       <c r="X46" s="1">
         <f t="shared" si="8"/>
-        <v>-5.2761065182364258E-2</v>
+        <v>-5.7107214300509718E-2</v>
       </c>
       <c r="Y46" s="1">
         <f t="shared" si="9"/>
@@ -9594,19 +9594,19 @@
       </c>
       <c r="AL46" s="1">
         <f t="shared" si="24"/>
-        <v>-0.23841448988615557</v>
+        <v>-0.24362127525823143</v>
       </c>
       <c r="AM46" s="1">
         <f t="shared" si="25"/>
-        <v>-0.10845709259350163</v>
+        <v>-0.11306143258782624</v>
       </c>
       <c r="AN46" s="1">
         <f t="shared" si="26"/>
-        <v>-3.4195722711985121E-2</v>
+        <v>-3.8455808204737547E-2</v>
       </c>
       <c r="AO46" s="1">
         <f t="shared" si="28"/>
-        <v>0.20421876717417045</v>
+        <v>0.20516546705349389</v>
       </c>
       <c r="AP46" s="1" t="s">
         <v>38</v>
@@ -9682,7 +9682,7 @@
       </c>
       <c r="N47" s="1">
         <f t="shared" si="4"/>
-        <v>0.2071537294029436</v>
+        <v>0.20401247104030071</v>
       </c>
       <c r="O47" s="1">
         <f t="shared" si="5"/>
@@ -9699,7 +9699,7 @@
       </c>
       <c r="S47" s="1">
         <f t="shared" si="6"/>
-        <v>0.55989523634014715</v>
+        <v>0.55838918685997196</v>
       </c>
       <c r="T47" s="1">
         <f t="shared" si="7"/>
@@ -9716,7 +9716,7 @@
       </c>
       <c r="X47" s="1">
         <f t="shared" si="8"/>
-        <v>0.61559126375128448</v>
+        <v>0.61434340514728847</v>
       </c>
       <c r="Y47" s="1">
         <f t="shared" si="9"/>
@@ -9764,19 +9764,19 @@
       </c>
       <c r="AL47" s="1">
         <f t="shared" si="24"/>
-        <v>0.2071537294029436</v>
+        <v>0.20401247104030071</v>
       </c>
       <c r="AM47" s="1">
         <f t="shared" si="25"/>
-        <v>0.46088007649812512</v>
+        <v>0.45891502101585369</v>
       </c>
       <c r="AN47" s="1">
         <f t="shared" si="26"/>
-        <v>0.61559126375128448</v>
+        <v>0.61434340514728847</v>
       </c>
       <c r="AO47" s="1">
         <f t="shared" si="28"/>
-        <v>0.40843753434834085</v>
+        <v>0.41033093410698773</v>
       </c>
       <c r="AP47" s="1" t="s">
         <v>38</v>
@@ -10047,7 +10047,7 @@
       </c>
       <c r="S49" s="1">
         <f t="shared" si="6"/>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058624</v>
       </c>
       <c r="T49" s="1">
         <f t="shared" si="7"/>
@@ -10064,7 +10064,7 @@
       </c>
       <c r="X49" s="1">
         <f t="shared" si="8"/>
-        <v>-0.44263325706032602</v>
+        <v>-0.44878674231172533</v>
       </c>
       <c r="Y49" s="1">
         <f t="shared" si="9"/>
@@ -10112,19 +10112,19 @@
       </c>
       <c r="AL49" s="1">
         <f>MIN(N49,S49,X49,AH49)</f>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058624</v>
       </c>
       <c r="AM49" s="1">
         <f>AVERAGE(N49,S49,X49,AH49)</f>
-        <v>-0.48904661323627385</v>
+        <v>-0.49541525755115579</v>
       </c>
       <c r="AN49" s="1">
         <f>MAX(N49,S49,X49,AH49)</f>
-        <v>-0.44263325706032602</v>
+        <v>-0.44878674231172533</v>
       </c>
       <c r="AO49" s="1">
         <f t="shared" ref="AO49" si="29">AN49-AL49</f>
-        <v>9.2826712351895713E-2</v>
+        <v>9.3257030478860914E-2</v>
       </c>
       <c r="AP49" s="1" t="s">
         <v>39</v>
@@ -10387,7 +10387,7 @@
       </c>
       <c r="N51" s="1">
         <f t="shared" si="4"/>
-        <v>-0.46119859953070519</v>
+        <v>-0.46743814840749753</v>
       </c>
       <c r="O51" s="1">
         <f t="shared" si="5"/>
@@ -10421,7 +10421,7 @@
       </c>
       <c r="X51" s="1">
         <f t="shared" si="8"/>
-        <v>-0.23841448988615557</v>
+        <v>-0.24362127525823143</v>
       </c>
       <c r="Y51" s="1">
         <f t="shared" si="9"/>
@@ -10469,19 +10469,19 @@
       </c>
       <c r="AL51" s="1">
         <f>MIN(N51,S51,X51,AH51)</f>
-        <v>-0.46119859953070519</v>
+        <v>-0.46743814840749753</v>
       </c>
       <c r="AM51" s="1">
         <f>AVERAGE(N51,S51,X51,AH51)</f>
-        <v>-0.34980654470843037</v>
+        <v>-0.35552971183286447</v>
       </c>
       <c r="AN51" s="1">
         <f>MAX(N51,S51,X51,AH51)</f>
-        <v>-0.23841448988615557</v>
+        <v>-0.24362127525823143</v>
       </c>
       <c r="AO51" s="1">
         <f t="shared" ref="AO51" si="30">AN51-AL51</f>
-        <v>0.22278410964454962</v>
+        <v>0.2238168731492661</v>
       </c>
       <c r="AP51" s="1" t="s">
         <v>39</v>
@@ -10551,7 +10551,7 @@
       </c>
       <c r="N52" s="1">
         <f t="shared" si="4"/>
-        <v>-0.16415312000463905</v>
+        <v>-0.16901565087514275</v>
       </c>
       <c r="O52" s="1">
         <f t="shared" si="5"/>
@@ -10568,7 +10568,7 @@
       </c>
       <c r="S52" s="1">
         <f t="shared" si="6"/>
-        <v>0.11432701705104793</v>
+        <v>0.11075544056143984</v>
       </c>
       <c r="T52" s="1">
         <f t="shared" si="7"/>
@@ -10585,7 +10585,7 @@
       </c>
       <c r="X52" s="1">
         <f t="shared" si="8"/>
-        <v>-0.51689462694184252</v>
+        <v>-0.52339236669481404</v>
       </c>
       <c r="Y52" s="1">
         <f t="shared" si="9"/>
@@ -10633,19 +10633,19 @@
       </c>
       <c r="AL52" s="1">
         <f>MIN(N52,S52,X52,AH52)</f>
-        <v>-0.51689462694184252</v>
+        <v>-0.52339236669481404</v>
       </c>
       <c r="AM52" s="1">
         <f>AVERAGE(N52,S52,X52,AH52)</f>
-        <v>-0.18890690996514456</v>
+        <v>-0.1938841923361723</v>
       </c>
       <c r="AN52" s="1">
         <f>MAX(N52,S52,X52,AH52)</f>
-        <v>0.11432701705104793</v>
+        <v>0.11075544056143984</v>
       </c>
       <c r="AO52" s="1">
         <f t="shared" ref="AO52:AO53" si="31">AN52-AL52</f>
-        <v>0.63122164399289049</v>
+        <v>0.63414780725625386</v>
       </c>
       <c r="AP52" s="1" t="s">
         <v>38</v>
@@ -10727,7 +10727,7 @@
       </c>
       <c r="N53" s="1">
         <f t="shared" si="4"/>
-        <v>-0.49832928447146346</v>
+        <v>-0.50474096059904183</v>
       </c>
       <c r="O53" s="1">
         <f t="shared" si="5"/>
@@ -10744,7 +10744,7 @@
       </c>
       <c r="S53" s="1">
         <f t="shared" si="6"/>
-        <v>-0.10845709259350166</v>
+        <v>-0.11306143258782624</v>
       </c>
       <c r="T53" s="1">
         <f t="shared" si="7"/>
@@ -10761,7 +10761,7 @@
       </c>
       <c r="X53" s="1">
         <f t="shared" si="8"/>
-        <v>7.7196332110289673E-2</v>
+        <v>7.3452628369895495E-2</v>
       </c>
       <c r="Y53" s="1">
         <f t="shared" si="9"/>
@@ -10809,19 +10809,19 @@
       </c>
       <c r="AL53" s="1">
         <f>MIN(N53,S53,X53,AH53)</f>
-        <v>-0.49832928447146346</v>
+        <v>-0.50474096059904183</v>
       </c>
       <c r="AM53" s="1">
         <f>AVERAGE(N53,S53,X53,AH53)</f>
-        <v>-0.17653001498489182</v>
+        <v>-0.18144992160565751</v>
       </c>
       <c r="AN53" s="1">
         <f>MAX(N53,S53,X53,AH53)</f>
-        <v>7.7196332110289673E-2</v>
+        <v>7.3452628369895495E-2</v>
       </c>
       <c r="AO53" s="1">
         <f t="shared" si="31"/>
-        <v>0.57552561658175316</v>
+        <v>0.57819358896893736</v>
       </c>
       <c r="AP53" s="1" t="s">
         <v>38</v>
@@ -11072,7 +11072,7 @@
       </c>
       <c r="N55" s="1">
         <f t="shared" si="4"/>
-        <v>9.576167458066881E-2</v>
+        <v>9.2104034465667659E-2</v>
       </c>
       <c r="O55" s="1">
         <f t="shared" si="5"/>
@@ -11089,7 +11089,7 @@
       </c>
       <c r="S55" s="1">
         <f t="shared" si="6"/>
-        <v>0.33711112669559751</v>
+        <v>0.33457231371070589</v>
       </c>
       <c r="T55" s="1">
         <f t="shared" si="7"/>
@@ -11106,7 +11106,7 @@
       </c>
       <c r="X55" s="1">
         <f t="shared" si="8"/>
-        <v>0.41137249657711406</v>
+        <v>0.4091779380937946</v>
       </c>
       <c r="Y55" s="1">
         <f t="shared" si="9"/>
@@ -11154,19 +11154,19 @@
       </c>
       <c r="AL55" s="1">
         <f>MIN(N55,S55,X55,AH55)</f>
-        <v>9.576167458066881E-2</v>
+        <v>9.2104034465667659E-2</v>
       </c>
       <c r="AM55" s="1">
         <f>AVERAGE(N55,S55,X55,AH55)</f>
-        <v>0.28141509928446012</v>
+        <v>0.27861809542338939</v>
       </c>
       <c r="AN55" s="1">
         <f>MAX(N55,S55,X55,AH55)</f>
-        <v>0.41137249657711406</v>
+        <v>0.4091779380937946</v>
       </c>
       <c r="AO55" s="1">
         <f t="shared" ref="AO55" si="32">AN55-AL55</f>
-        <v>0.31561082199644525</v>
+        <v>0.31707390362812693</v>
       </c>
       <c r="AP55" s="1" t="s">
         <v>38</v>
@@ -11251,7 +11251,7 @@
       </c>
       <c r="N56" s="1">
         <f t="shared" si="4"/>
-        <v>-0.94389750376056258</v>
+        <v>-0.95237470689757397</v>
       </c>
       <c r="O56" s="1">
         <f t="shared" si="5"/>
@@ -11268,7 +11268,7 @@
       </c>
       <c r="S56" s="1">
         <f t="shared" si="6"/>
-        <v>-0.85107079140866693</v>
+        <v>-0.85911767641871317</v>
       </c>
       <c r="T56" s="1">
         <f t="shared" si="7"/>
@@ -11285,7 +11285,7 @@
       </c>
       <c r="X56" s="1">
         <f t="shared" si="8"/>
-        <v>-0.92533216129018347</v>
+        <v>-0.93372330080180177</v>
       </c>
       <c r="Y56" s="1">
         <f t="shared" si="9"/>
@@ -11333,19 +11333,19 @@
       </c>
       <c r="AL56" s="1">
         <f>MIN(N56,S56,X56,AH56)</f>
-        <v>-0.94389750376056258</v>
+        <v>-0.95237470689757397</v>
       </c>
       <c r="AM56" s="1">
         <f>AVERAGE(N56,S56,X56,AH56)</f>
-        <v>-0.90676681881980425</v>
+        <v>-0.91507189470602956</v>
       </c>
       <c r="AN56" s="1">
         <f>MAX(N56,S56,X56,AH56)</f>
-        <v>-0.85107079140866693</v>
+        <v>-0.85911767641871317</v>
       </c>
       <c r="AO56" s="1">
         <f t="shared" ref="AO56" si="33">AN56-AL56</f>
-        <v>9.2826712351895657E-2</v>
+        <v>9.3257030478860803E-2</v>
       </c>
       <c r="AP56" s="1" t="s">
         <v>38</v>
@@ -11602,7 +11602,7 @@
       </c>
       <c r="N58" s="1">
         <f t="shared" si="4"/>
-        <v>0.46706852398825144</v>
+        <v>0.46513215638111111</v>
       </c>
       <c r="O58" s="1">
         <f t="shared" si="5"/>
@@ -11619,7 +11619,7 @@
       </c>
       <c r="S58" s="1">
         <f t="shared" si="6"/>
-        <v>1.6181197571517576</v>
+        <v>1.6215193343189858</v>
       </c>
       <c r="T58" s="1">
         <f t="shared" si="7"/>
@@ -11636,7 +11636,7 @@
       </c>
       <c r="X58" s="1">
         <f t="shared" si="8"/>
-        <v>1.0240287980996254</v>
+        <v>1.0246743392542763</v>
       </c>
       <c r="Y58" s="1">
         <f t="shared" si="9"/>
@@ -11684,19 +11684,19 @@
       </c>
       <c r="AL58" s="1">
         <f>MIN(N58,S58,X58,AH58)</f>
-        <v>0.46706852398825144</v>
+        <v>0.46513215638111111</v>
       </c>
       <c r="AM58" s="1">
         <f>AVERAGE(N58,S58,X58,AH58)</f>
-        <v>1.0364056930798782</v>
+        <v>1.037108609984791</v>
       </c>
       <c r="AN58" s="1">
         <f>MAX(N58,S58,X58,AH58)</f>
-        <v>1.6181197571517576</v>
+        <v>1.6215193343189858</v>
       </c>
       <c r="AO58" s="1">
         <f t="shared" ref="AO58" si="34">AN58-AL58</f>
-        <v>1.1510512331635061</v>
+        <v>1.1563871779378747</v>
       </c>
       <c r="AP58" s="1" t="s">
         <v>38</v>
@@ -11947,7 +11947,7 @@
       </c>
       <c r="N60" s="1">
         <f t="shared" si="4"/>
-        <v>-0.57259065435297996</v>
+        <v>-0.57934658498213054</v>
       </c>
       <c r="O60" s="1">
         <f t="shared" si="5"/>
@@ -11964,7 +11964,7 @@
       </c>
       <c r="S60" s="1">
         <f t="shared" si="6"/>
-        <v>-7.1326407652743395E-2</v>
+        <v>-7.5758620396281895E-2</v>
       </c>
       <c r="T60" s="1">
         <f t="shared" si="7"/>
@@ -11981,7 +11981,7 @@
       </c>
       <c r="X60" s="1">
         <f t="shared" si="8"/>
-        <v>-0.34980654470843037</v>
+        <v>-0.35552971183286447</v>
       </c>
       <c r="Y60" s="1">
         <f t="shared" si="9"/>
@@ -12029,19 +12029,19 @@
       </c>
       <c r="AL60" s="1">
         <f>MIN(N60,S60,X60,AH60)</f>
-        <v>-0.57259065435297996</v>
+        <v>-0.57934658498213054</v>
       </c>
       <c r="AM60" s="1">
         <f>AVERAGE(N60,S60,X60,AH60)</f>
-        <v>-0.33124120223805126</v>
+        <v>-0.33687830573709232</v>
       </c>
       <c r="AN60" s="1">
         <f>MAX(N60,S60,X60,AH60)</f>
-        <v>-7.1326407652743395E-2</v>
+        <v>-7.5758620396281895E-2</v>
       </c>
       <c r="AO60" s="1">
         <f t="shared" ref="AO60" si="35">AN60-AL60</f>
-        <v>0.50126424670023662</v>
+        <v>0.50358796458584865</v>
       </c>
       <c r="AP60" s="1" t="s">
         <v>38</v>
@@ -12298,7 +12298,7 @@
       </c>
       <c r="N62" s="1">
         <f t="shared" si="4"/>
-        <v>-0.73967873658639216</v>
+        <v>-0.74720923984408005</v>
       </c>
       <c r="O62" s="1">
         <f t="shared" si="5"/>
@@ -12315,7 +12315,7 @@
       </c>
       <c r="S62" s="1">
         <f t="shared" si="6"/>
-        <v>-0.73967873658639216</v>
+        <v>-0.74720923984408005</v>
       </c>
       <c r="T62" s="1">
         <f t="shared" si="7"/>
@@ -12332,7 +12332,7 @@
       </c>
       <c r="X62" s="1">
         <f t="shared" si="8"/>
-        <v>-0.72111339411601305</v>
+        <v>-0.72855783374830796</v>
       </c>
       <c r="Y62" s="1">
         <f t="shared" si="9"/>
@@ -12380,19 +12380,19 @@
       </c>
       <c r="AL62" s="1">
         <f>MIN(N62,S62,X62,AH62)</f>
-        <v>-0.73967873658639216</v>
+        <v>-0.74720923984408005</v>
       </c>
       <c r="AM62" s="1">
         <f>AVERAGE(N62,S62,X62,AH62)</f>
-        <v>-0.73349028909626579</v>
+        <v>-0.74099210447882269</v>
       </c>
       <c r="AN62" s="1">
         <f>MAX(N62,S62,X62,AH62)</f>
-        <v>-0.72111339411601305</v>
+        <v>-0.72855783374830796</v>
       </c>
       <c r="AO62" s="1">
         <f t="shared" ref="AO62" si="36">AN62-AL62</f>
-        <v>1.8565342470379109E-2</v>
+        <v>1.8651406095772094E-2</v>
       </c>
       <c r="AP62" s="1" t="s">
         <v>38</v>
@@ -12643,7 +12643,7 @@
       </c>
       <c r="N64" s="1">
         <f t="shared" si="4"/>
-        <v>-0.6468520242344965</v>
+        <v>-0.65395220936521925</v>
       </c>
       <c r="O64" s="1">
         <f t="shared" si="5"/>
@@ -12677,7 +12677,7 @@
       </c>
       <c r="X64" s="1">
         <f t="shared" si="8"/>
-        <v>-0.25697983235653471</v>
+        <v>-0.26227268135400361</v>
       </c>
       <c r="Y64" s="1">
         <f t="shared" si="9"/>
@@ -12725,19 +12725,19 @@
       </c>
       <c r="AL64" s="1">
         <f>MIN(N64,S64,X64,AH64)</f>
-        <v>-0.6468520242344965</v>
+        <v>-0.65395220936521925</v>
       </c>
       <c r="AM64" s="1">
         <f>AVERAGE(N64,S64,X64,AH64)</f>
-        <v>-0.45191592829551563</v>
+        <v>-0.45811244535961143</v>
       </c>
       <c r="AN64" s="1">
         <f>MAX(N64,S64,X64,AH64)</f>
-        <v>-0.25697983235653471</v>
+        <v>-0.26227268135400361</v>
       </c>
       <c r="AO64" s="1">
         <f t="shared" ref="AO64" si="37">AN64-AL64</f>
-        <v>0.38987219187796179</v>
+        <v>0.39167952801121564</v>
       </c>
       <c r="AP64" s="1" t="s">
         <v>39</v>
@@ -13214,7 +13214,7 @@
       </c>
       <c r="N67" s="1">
         <f t="shared" ref="N67:N128" si="39">IF(M67="null","null",(M67-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
-        <v>-0.72111339411601305</v>
+        <v>-0.72855783374830796</v>
       </c>
       <c r="O67" s="1">
         <f t="shared" ref="O67:O128" si="40">IF(M67="null","null",10*((M67-$AS67)/($AT67-$AS67)))</f>
@@ -13231,7 +13231,7 @@
       </c>
       <c r="S67" s="1">
         <f t="shared" ref="S67:S128" si="41">IF(R67="null","null",(R67-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
-        <v>-0.66541736670487561</v>
+        <v>-0.67260361546099146</v>
       </c>
       <c r="T67" s="1">
         <f t="shared" ref="T67:T128" si="42">IF(R67="null","null",10*((R67-$AS67)/($AT67-$AS67)))</f>
@@ -13248,7 +13248,7 @@
       </c>
       <c r="X67" s="1">
         <f t="shared" ref="X67:X128" si="43">IF(W67="null","null",(W67-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
-        <v>-0.86963613387904604</v>
+        <v>-0.87776908251448527</v>
       </c>
       <c r="Y67" s="1">
         <f t="shared" ref="Y67:Y128" si="44">IF(W67="null","null",10*((W67-$AS67)/($AT67-$AS67)))</f>
@@ -13296,19 +13296,19 @@
       </c>
       <c r="AL67" s="1">
         <f>MIN(N67,S67,X67,AH67)</f>
-        <v>-0.86963613387904604</v>
+        <v>-0.87776908251448527</v>
       </c>
       <c r="AM67" s="1">
         <f>AVERAGE(N67,S67,X67,AH67)</f>
-        <v>-0.75205563156664479</v>
+        <v>-0.759643510574595</v>
       </c>
       <c r="AN67" s="1">
         <f>MAX(N67,S67,X67,AH67)</f>
-        <v>-0.66541736670487561</v>
+        <v>-0.67260361546099146</v>
       </c>
       <c r="AO67" s="1">
         <f t="shared" ref="AO67" si="49">AN67-AL67</f>
-        <v>0.20421876717417042</v>
+        <v>0.20516546705349381</v>
       </c>
       <c r="AP67" s="1" t="s">
         <v>38</v>
@@ -13396,7 +13396,7 @@
       </c>
       <c r="N68" s="1">
         <f t="shared" si="39"/>
-        <v>-0.18271846247501819</v>
+        <v>-0.18766705697091493</v>
       </c>
       <c r="O68" s="1">
         <f t="shared" si="40"/>
@@ -13413,7 +13413,7 @@
       </c>
       <c r="S68" s="1">
         <f t="shared" si="41"/>
-        <v>-0.18271846247501819</v>
+        <v>-0.18766705697091493</v>
       </c>
       <c r="T68" s="1">
         <f t="shared" si="42"/>
@@ -13430,7 +13430,7 @@
       </c>
       <c r="X68" s="1">
         <f t="shared" si="43"/>
-        <v>-0.42406791458994691</v>
+        <v>-0.43013533621595318</v>
       </c>
       <c r="Y68" s="1">
         <f t="shared" si="44"/>
@@ -13478,19 +13478,19 @@
       </c>
       <c r="AL68" s="1">
         <f>MIN(N68,S68,X68,AH68)</f>
-        <v>-0.42406791458994691</v>
+        <v>-0.43013533621595318</v>
       </c>
       <c r="AM68" s="1">
         <f>AVERAGE(N68,S68,X68,AH68)</f>
-        <v>-0.26316827984666108</v>
+        <v>-0.26848981671926103</v>
       </c>
       <c r="AN68" s="1">
         <f>MAX(N68,S68,X68,AH68)</f>
-        <v>-0.18271846247501819</v>
+        <v>-0.18766705697091493</v>
       </c>
       <c r="AO68" s="1">
         <f t="shared" ref="AO68:AO70" si="50">AN68-AL68</f>
-        <v>0.24134945211492873</v>
+        <v>0.24246827924503825</v>
       </c>
       <c r="AP68" s="1" t="s">
         <v>38</v>
@@ -13575,7 +13575,7 @@
       </c>
       <c r="N69" s="1">
         <f t="shared" si="39"/>
-        <v>-0.36837188717880953</v>
+        <v>-0.37418111792863662</v>
       </c>
       <c r="O69" s="1">
         <f t="shared" si="40"/>
@@ -13592,7 +13592,7 @@
       </c>
       <c r="S69" s="1">
         <f t="shared" si="41"/>
-        <v>5.8630989639910536E-2</v>
+        <v>5.4801222274123318E-2</v>
       </c>
       <c r="T69" s="1">
         <f t="shared" si="42"/>
@@ -13609,7 +13609,7 @@
       </c>
       <c r="X69" s="1">
         <f t="shared" si="43"/>
-        <v>-0.12702243506388078</v>
+        <v>-0.1317128386835984</v>
       </c>
       <c r="Y69" s="1">
         <f t="shared" si="44"/>
@@ -13657,19 +13657,19 @@
       </c>
       <c r="AL69" s="1">
         <f>MIN(N69,S69,X69,AH69)</f>
-        <v>-0.36837188717880953</v>
+        <v>-0.37418111792863662</v>
       </c>
       <c r="AM69" s="1">
         <f>AVERAGE(N69,S69,X69,AH69)</f>
-        <v>-0.14558777753425992</v>
+        <v>-0.15036424477937058</v>
       </c>
       <c r="AN69" s="1">
         <f>MAX(N69,S69,X69,AH69)</f>
-        <v>5.8630989639910536E-2</v>
+        <v>5.4801222274123318E-2</v>
       </c>
       <c r="AO69" s="1">
         <f t="shared" si="50"/>
-        <v>0.42700287681872007</v>
+        <v>0.42898234020275994</v>
       </c>
       <c r="AP69" s="1" t="s">
         <v>38</v>
@@ -13745,7 +13745,7 @@
       </c>
       <c r="N70" s="1">
         <f t="shared" si="39"/>
-        <v>0.55989523634014715</v>
+        <v>0.55838918685997196</v>
       </c>
       <c r="O70" s="1">
         <f t="shared" si="40"/>
@@ -13762,7 +13762,7 @@
       </c>
       <c r="S70" s="1">
         <f t="shared" si="41"/>
-        <v>0.68985263363280103</v>
+        <v>0.68894902953037718</v>
       </c>
       <c r="T70" s="1">
         <f t="shared" si="42"/>
@@ -13779,7 +13779,7 @@
       </c>
       <c r="X70" s="1">
         <f t="shared" si="43"/>
-        <v>0.24428441434370188</v>
+        <v>0.24131528323184503</v>
       </c>
       <c r="Y70" s="1">
         <f t="shared" si="44"/>
@@ -13827,19 +13827,19 @@
       </c>
       <c r="AL70" s="1">
         <f>MIN(N70,S70,X70,AH70)</f>
-        <v>0.24428441434370188</v>
+        <v>0.24131528323184503</v>
       </c>
       <c r="AM70" s="1">
         <f>AVERAGE(N70,S70,X70,AH70)</f>
-        <v>0.49801076143888334</v>
+        <v>0.4962178332073981</v>
       </c>
       <c r="AN70" s="1">
         <f>MAX(N70,S70,X70,AH70)</f>
-        <v>0.68985263363280103</v>
+        <v>0.68894902953037718</v>
       </c>
       <c r="AO70" s="1">
         <f t="shared" si="50"/>
-        <v>0.44556821928909918</v>
+        <v>0.44763374629853214</v>
       </c>
       <c r="AP70" s="1" t="s">
         <v>38</v>
@@ -14105,7 +14105,7 @@
       </c>
       <c r="N72" s="1">
         <f t="shared" si="39"/>
-        <v>-0.59115599682335906</v>
+        <v>-0.59799799107790275</v>
       </c>
       <c r="O72" s="1">
         <f t="shared" si="40"/>
@@ -14122,7 +14122,7 @@
       </c>
       <c r="S72" s="1">
         <f t="shared" si="41"/>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="T72" s="1">
         <f t="shared" si="42"/>
@@ -14139,7 +14139,7 @@
       </c>
       <c r="X72" s="1">
         <f t="shared" si="43"/>
-        <v>-0.7953747639975296</v>
+        <v>-0.80316345813139656</v>
       </c>
       <c r="Y72" s="1">
         <f t="shared" si="44"/>
@@ -14187,19 +14187,19 @@
       </c>
       <c r="AL72" s="1">
         <f>MIN(N72,S72,X72,AH72)</f>
-        <v>-0.7953747639975296</v>
+        <v>-0.80316345813139656</v>
       </c>
       <c r="AM72" s="1">
         <f>AVERAGE(N72,S72,X72,AH72)</f>
-        <v>-0.66541736670487561</v>
+        <v>-0.67260361546099146</v>
       </c>
       <c r="AN72" s="1">
         <f>MAX(N72,S72,X72,AH72)</f>
-        <v>-0.59115599682335906</v>
+        <v>-0.59799799107790275</v>
       </c>
       <c r="AO72" s="1">
         <f t="shared" ref="AO72" si="51">AN72-AL72</f>
-        <v>0.20421876717417053</v>
+        <v>0.20516546705349381</v>
       </c>
       <c r="AP72" s="1" t="s">
         <v>38</v>
@@ -14278,7 +14278,7 @@
       </c>
       <c r="N73" s="1">
         <f t="shared" si="39"/>
-        <v>-0.40550257211956775</v>
+        <v>-0.41148393012018097</v>
       </c>
       <c r="O73" s="1">
         <f t="shared" si="40"/>
@@ -14295,7 +14295,7 @@
       </c>
       <c r="S73" s="1">
         <f t="shared" si="41"/>
-        <v>-0.38693722964918864</v>
+        <v>-0.39283252402440882</v>
       </c>
       <c r="T73" s="1">
         <f t="shared" si="42"/>
@@ -14312,7 +14312,7 @@
       </c>
       <c r="X73" s="1">
         <f t="shared" si="43"/>
-        <v>-0.36837188717880953</v>
+        <v>-0.37418111792863662</v>
       </c>
       <c r="Y73" s="1">
         <f t="shared" si="44"/>
@@ -14360,19 +14360,19 @@
       </c>
       <c r="AL73" s="1">
         <f>MIN(N73,S73,X73,AH73)</f>
-        <v>-0.40550257211956775</v>
+        <v>-0.41148393012018097</v>
       </c>
       <c r="AM73" s="1">
         <f>AVERAGE(N73,S73,X73,AH73)</f>
-        <v>-0.38693722964918864</v>
+        <v>-0.39283252402440877</v>
       </c>
       <c r="AN73" s="1">
         <f>MAX(N73,S73,X73,AH73)</f>
-        <v>-0.36837188717880953</v>
+        <v>-0.37418111792863662</v>
       </c>
       <c r="AO73" s="1">
         <f t="shared" ref="AO73:AO76" si="52">AN73-AL73</f>
-        <v>3.7130684940758218E-2</v>
+        <v>3.7302812191544354E-2</v>
       </c>
       <c r="AP73" s="1" t="s">
         <v>38</v>
@@ -14451,7 +14451,7 @@
       </c>
       <c r="N74" s="1">
         <f t="shared" si="39"/>
-        <v>-0.21984914741577646</v>
+        <v>-0.22496986916245926</v>
       </c>
       <c r="O74" s="1">
         <f t="shared" si="40"/>
@@ -14468,7 +14468,7 @@
       </c>
       <c r="S74" s="1">
         <f t="shared" si="41"/>
-        <v>-0.55402531188260085</v>
+        <v>-0.56069517888635834</v>
       </c>
       <c r="T74" s="1">
         <f t="shared" si="42"/>
@@ -14485,7 +14485,7 @@
       </c>
       <c r="X74" s="1">
         <f t="shared" si="43"/>
-        <v>-0.18271846247501819</v>
+        <v>-0.18766705697091493</v>
       </c>
       <c r="Y74" s="1">
         <f t="shared" si="44"/>
@@ -14533,19 +14533,19 @@
       </c>
       <c r="AL74" s="1">
         <f>MIN(N74,S74,X74,AH74)</f>
-        <v>-0.55402531188260085</v>
+        <v>-0.56069517888635834</v>
       </c>
       <c r="AM74" s="1">
         <f>AVERAGE(N74,S74,X74,AH74)</f>
-        <v>-0.31886430725779852</v>
+        <v>-0.32444403500657754</v>
       </c>
       <c r="AN74" s="1">
         <f>MAX(N74,S74,X74,AH74)</f>
-        <v>-0.18271846247501819</v>
+        <v>-0.18766705697091493</v>
       </c>
       <c r="AO74" s="1">
         <f t="shared" si="52"/>
-        <v>0.37130684940758263</v>
+        <v>0.37302812191544343</v>
       </c>
       <c r="AP74" s="1" t="s">
         <v>38</v>
@@ -14624,7 +14624,7 @@
       </c>
       <c r="N75" s="1">
         <f t="shared" si="39"/>
-        <v>-0.62828668176411739</v>
+        <v>-0.63530080326944705</v>
       </c>
       <c r="O75" s="1">
         <f t="shared" si="40"/>
@@ -14641,7 +14641,7 @@
       </c>
       <c r="S75" s="1">
         <f t="shared" si="41"/>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="T75" s="1">
         <f t="shared" si="42"/>
@@ -14658,7 +14658,7 @@
       </c>
       <c r="X75" s="1">
         <f t="shared" si="43"/>
-        <v>-0.6468520242344965</v>
+        <v>-0.65395220936521925</v>
       </c>
       <c r="Y75" s="1">
         <f t="shared" si="44"/>
@@ -14706,19 +14706,19 @@
       </c>
       <c r="AL75" s="1">
         <f>MIN(N75,S75,X75,AH75)</f>
-        <v>-0.6468520242344965</v>
+        <v>-0.65395220936521925</v>
       </c>
       <c r="AM75" s="1">
         <f>AVERAGE(N75,S75,X75,AH75)</f>
-        <v>-0.62828668176411739</v>
+        <v>-0.63530080326944705</v>
       </c>
       <c r="AN75" s="1">
         <f>MAX(N75,S75,X75,AH75)</f>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="AO75" s="1">
         <f t="shared" si="52"/>
-        <v>3.7130684940758218E-2</v>
+        <v>3.730281219154441E-2</v>
       </c>
       <c r="AP75" s="1" t="s">
         <v>38</v>
@@ -14809,7 +14809,7 @@
       </c>
       <c r="N76" s="1">
         <f t="shared" si="39"/>
-        <v>-0.6468520242344965</v>
+        <v>-0.65395220936521925</v>
       </c>
       <c r="O76" s="1">
         <f t="shared" si="40"/>
@@ -14826,7 +14826,7 @@
       </c>
       <c r="S76" s="1">
         <f t="shared" si="41"/>
-        <v>-0.62828668176411739</v>
+        <v>-0.63530080326944705</v>
       </c>
       <c r="T76" s="1">
         <f t="shared" si="42"/>
@@ -14843,7 +14843,7 @@
       </c>
       <c r="X76" s="1">
         <f t="shared" si="43"/>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="Y76" s="1">
         <f t="shared" si="44"/>
@@ -14891,19 +14891,19 @@
       </c>
       <c r="AL76" s="1">
         <f>MIN(N76,S76,X76,AH76)</f>
-        <v>-0.6468520242344965</v>
+        <v>-0.65395220936521925</v>
       </c>
       <c r="AM76" s="1">
         <f>AVERAGE(N76,S76,X76,AH76)</f>
-        <v>-0.62828668176411739</v>
+        <v>-0.63530080326944705</v>
       </c>
       <c r="AN76" s="1">
         <f>MAX(N76,S76,X76,AH76)</f>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="AO76" s="1">
         <f t="shared" si="52"/>
-        <v>3.7130684940758218E-2</v>
+        <v>3.730281219154441E-2</v>
       </c>
       <c r="AP76" s="1" t="s">
         <v>38</v>
@@ -15169,7 +15169,7 @@
       </c>
       <c r="N78" s="1">
         <f t="shared" si="39"/>
-        <v>-0.46119859953070519</v>
+        <v>-0.46743814840749753</v>
       </c>
       <c r="O78" s="1">
         <f t="shared" si="40"/>
@@ -15203,7 +15203,7 @@
       </c>
       <c r="X78" s="1">
         <f t="shared" si="43"/>
-        <v>-0.27554517482691387</v>
+        <v>-0.28092408744977576</v>
       </c>
       <c r="Y78" s="1">
         <f t="shared" si="44"/>
@@ -15237,7 +15237,7 @@
       </c>
       <c r="AH78" s="1">
         <f t="shared" si="47"/>
-        <v>-0.20128380494539733</v>
+        <v>-0.20631846306668711</v>
       </c>
       <c r="AI78" s="1">
         <f t="shared" si="48"/>
@@ -15251,19 +15251,19 @@
       </c>
       <c r="AL78" s="1">
         <f t="shared" ref="AL78:AL87" si="53">MIN(N78,S78,X78,AH78)</f>
-        <v>-0.46119859953070519</v>
+        <v>-0.46743814840749753</v>
       </c>
       <c r="AM78" s="1">
         <f t="shared" ref="AM78:AM87" si="54">AVERAGE(N78,S78,X78,AH78)</f>
-        <v>-0.31267585976767215</v>
+        <v>-0.31822689964132012</v>
       </c>
       <c r="AN78" s="1">
         <f t="shared" ref="AN78:AN87" si="55">MAX(N78,S78,X78,AH78)</f>
-        <v>-0.20128380494539733</v>
+        <v>-0.20631846306668711</v>
       </c>
       <c r="AO78" s="1">
         <f t="shared" ref="AO78" si="56">AN78-AL78</f>
-        <v>0.25991479458530786</v>
+        <v>0.26111968534081043</v>
       </c>
       <c r="AP78" s="1" t="s">
         <v>39</v>
@@ -15345,7 +15345,7 @@
       </c>
       <c r="N79" s="1">
         <f t="shared" si="39"/>
-        <v>-0.83250544893828782</v>
+        <v>-0.84046627032294097</v>
       </c>
       <c r="O79" s="1">
         <f t="shared" si="40"/>
@@ -15362,7 +15362,7 @@
       </c>
       <c r="S79" s="1">
         <f t="shared" si="41"/>
-        <v>-0.90676681881980437</v>
+        <v>-0.91507189470602968</v>
       </c>
       <c r="T79" s="1">
         <f t="shared" si="42"/>
@@ -15379,7 +15379,7 @@
       </c>
       <c r="X79" s="1">
         <f t="shared" si="43"/>
-        <v>-0.70254805164563394</v>
+        <v>-0.70990642765253575</v>
       </c>
       <c r="Y79" s="1">
         <f t="shared" si="44"/>
@@ -15427,19 +15427,19 @@
       </c>
       <c r="AL79" s="1">
         <f t="shared" si="53"/>
-        <v>-0.90676681881980437</v>
+        <v>-0.91507189470602968</v>
       </c>
       <c r="AM79" s="1">
         <f t="shared" si="54"/>
-        <v>-0.81394010646790882</v>
+        <v>-0.82181486422716876</v>
       </c>
       <c r="AN79" s="1">
         <f t="shared" si="55"/>
-        <v>-0.70254805164563394</v>
+        <v>-0.70990642765253575</v>
       </c>
       <c r="AO79" s="1">
         <f t="shared" ref="AO79:AO87" si="57">AN79-AL79</f>
-        <v>0.20421876717417042</v>
+        <v>0.20516546705349392</v>
       </c>
       <c r="AP79" s="1" t="s">
         <v>38</v>
@@ -15518,7 +15518,7 @@
       </c>
       <c r="N80" s="1">
         <f t="shared" si="39"/>
-        <v>-0.94389750376056258</v>
+        <v>-0.95237470689757397</v>
       </c>
       <c r="O80" s="1">
         <f t="shared" si="40"/>
@@ -15535,7 +15535,7 @@
       </c>
       <c r="S80" s="1">
         <f t="shared" si="41"/>
-        <v>-0.90676681881980437</v>
+        <v>-0.91507189470602968</v>
       </c>
       <c r="T80" s="1">
         <f t="shared" si="42"/>
@@ -15600,19 +15600,19 @@
       </c>
       <c r="AL80" s="1">
         <f t="shared" si="53"/>
-        <v>-0.94389750376056258</v>
+        <v>-0.95237470689757397</v>
       </c>
       <c r="AM80" s="1">
         <f t="shared" si="54"/>
-        <v>-0.92533216129018347</v>
+        <v>-0.93372330080180177</v>
       </c>
       <c r="AN80" s="1">
         <f t="shared" si="55"/>
-        <v>-0.90676681881980437</v>
+        <v>-0.91507189470602968</v>
       </c>
       <c r="AO80" s="1">
         <f t="shared" si="57"/>
-        <v>3.7130684940758218E-2</v>
+        <v>3.7302812191544299E-2</v>
       </c>
       <c r="AP80" s="1" t="s">
         <v>39</v>
@@ -15711,7 +15711,7 @@
       </c>
       <c r="S81" s="1">
         <f t="shared" si="41"/>
-        <v>-0.21984914741577646</v>
+        <v>-0.22496986916245926</v>
       </c>
       <c r="T81" s="1">
         <f t="shared" si="42"/>
@@ -15728,7 +15728,7 @@
       </c>
       <c r="X81" s="1">
         <f t="shared" si="43"/>
-        <v>-0.21984914741577646</v>
+        <v>-0.22496986916245926</v>
       </c>
       <c r="Y81" s="1">
         <f t="shared" si="44"/>
@@ -15776,15 +15776,15 @@
       </c>
       <c r="AL81" s="1">
         <f t="shared" si="53"/>
-        <v>-0.21984914741577646</v>
+        <v>-0.22496986916245926</v>
       </c>
       <c r="AM81" s="1">
         <f t="shared" si="54"/>
-        <v>-0.21984914741577646</v>
+        <v>-0.22496986916245926</v>
       </c>
       <c r="AN81" s="1">
         <f t="shared" si="55"/>
-        <v>-0.21984914741577646</v>
+        <v>-0.22496986916245926</v>
       </c>
       <c r="AO81" s="1">
         <f t="shared" si="57"/>
@@ -15873,7 +15873,7 @@
       </c>
       <c r="N82" s="1">
         <f t="shared" si="39"/>
-        <v>-0.72111339411601305</v>
+        <v>-0.72855783374830796</v>
       </c>
       <c r="O82" s="1">
         <f t="shared" si="40"/>
@@ -15890,7 +15890,7 @@
       </c>
       <c r="S82" s="1">
         <f t="shared" si="41"/>
-        <v>-0.68398270917525472</v>
+        <v>-0.69125502155676355</v>
       </c>
       <c r="T82" s="1">
         <f t="shared" si="42"/>
@@ -15907,7 +15907,7 @@
       </c>
       <c r="X82" s="1">
         <f t="shared" si="43"/>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058624</v>
       </c>
       <c r="Y82" s="1">
         <f t="shared" si="44"/>
@@ -15955,19 +15955,19 @@
       </c>
       <c r="AL82" s="1">
         <f t="shared" si="53"/>
-        <v>-0.72111339411601305</v>
+        <v>-0.72855783374830796</v>
       </c>
       <c r="AM82" s="1">
         <f t="shared" si="54"/>
-        <v>-0.6468520242344965</v>
+        <v>-0.65395220936521925</v>
       </c>
       <c r="AN82" s="1">
         <f t="shared" si="55"/>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058624</v>
       </c>
       <c r="AO82" s="1">
         <f t="shared" si="57"/>
-        <v>0.18565342470379131</v>
+        <v>0.18651406095772172</v>
       </c>
       <c r="AP82" s="1" t="s">
         <v>38</v>
@@ -16046,7 +16046,7 @@
       </c>
       <c r="N83" s="1">
         <f t="shared" si="39"/>
-        <v>-0.73967873658639216</v>
+        <v>-0.74720923984408005</v>
       </c>
       <c r="O83" s="1">
         <f t="shared" si="40"/>
@@ -16063,7 +16063,7 @@
       </c>
       <c r="S83" s="1">
         <f t="shared" si="41"/>
-        <v>-0.72111339411601305</v>
+        <v>-0.72855783374830796</v>
       </c>
       <c r="T83" s="1">
         <f t="shared" si="42"/>
@@ -16080,7 +16080,7 @@
       </c>
       <c r="X83" s="1">
         <f t="shared" si="43"/>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="Y83" s="1">
         <f t="shared" si="44"/>
@@ -16128,19 +16128,19 @@
       </c>
       <c r="AL83" s="1">
         <f t="shared" si="53"/>
-        <v>-0.73967873658639216</v>
+        <v>-0.74720923984408005</v>
       </c>
       <c r="AM83" s="1">
         <f t="shared" si="54"/>
-        <v>-0.69017115666538109</v>
+        <v>-0.69747215692202091</v>
       </c>
       <c r="AN83" s="1">
         <f t="shared" si="55"/>
-        <v>-0.60972133929373828</v>
+        <v>-0.61664939717367484</v>
       </c>
       <c r="AO83" s="1">
         <f t="shared" si="57"/>
-        <v>0.12995739729265388</v>
+        <v>0.13055984267040521</v>
       </c>
       <c r="AP83" s="1" t="s">
         <v>38</v>
@@ -16222,7 +16222,7 @@
       </c>
       <c r="N84" s="1">
         <f t="shared" si="39"/>
-        <v>-0.7953747639975296</v>
+        <v>-0.80316345813139656</v>
       </c>
       <c r="O84" s="1">
         <f t="shared" si="40"/>
@@ -16239,7 +16239,7 @@
       </c>
       <c r="S84" s="1">
         <f t="shared" si="41"/>
-        <v>-0.42406791458994691</v>
+        <v>-0.43013533621595318</v>
       </c>
       <c r="T84" s="1">
         <f t="shared" si="42"/>
@@ -16256,7 +16256,7 @@
       </c>
       <c r="X84" s="1">
         <f t="shared" si="43"/>
-        <v>-0.23841448988615557</v>
+        <v>-0.24362127525823143</v>
       </c>
       <c r="Y84" s="1">
         <f t="shared" si="44"/>
@@ -16304,19 +16304,19 @@
       </c>
       <c r="AL84" s="1">
         <f t="shared" si="53"/>
-        <v>-0.7953747639975296</v>
+        <v>-0.80316345813139656</v>
       </c>
       <c r="AM84" s="1">
         <f t="shared" si="54"/>
-        <v>-0.48595238949121072</v>
+        <v>-0.49230668986852705</v>
       </c>
       <c r="AN84" s="1">
         <f t="shared" si="55"/>
-        <v>-0.23841448988615557</v>
+        <v>-0.24362127525823143</v>
       </c>
       <c r="AO84" s="1">
         <f t="shared" si="57"/>
-        <v>0.55696027411137405</v>
+        <v>0.55954218287316515</v>
       </c>
       <c r="AP84" s="1" t="s">
         <v>38</v>
@@ -16410,7 +16410,7 @@
       </c>
       <c r="N85" s="1">
         <f t="shared" si="39"/>
-        <v>-0.20128380494539733</v>
+        <v>-0.20631846306668711</v>
       </c>
       <c r="O85" s="1">
         <f t="shared" si="40"/>
@@ -16427,7 +16427,7 @@
       </c>
       <c r="S85" s="1">
         <f t="shared" si="41"/>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058624</v>
       </c>
       <c r="T85" s="1">
         <f t="shared" si="42"/>
@@ -16444,7 +16444,7 @@
       </c>
       <c r="X85" s="1">
         <f t="shared" si="43"/>
-        <v>-0.25697983235653471</v>
+        <v>-0.26227268135400361</v>
       </c>
       <c r="Y85" s="1">
         <f t="shared" si="44"/>
@@ -16492,19 +16492,19 @@
       </c>
       <c r="AL85" s="1">
         <f t="shared" si="53"/>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058624</v>
       </c>
       <c r="AM85" s="1">
         <f t="shared" si="54"/>
-        <v>-0.33124120223805126</v>
+        <v>-0.33687830573709232</v>
       </c>
       <c r="AN85" s="1">
         <f t="shared" si="55"/>
-        <v>-0.20128380494539733</v>
+        <v>-0.20631846306668711</v>
       </c>
       <c r="AO85" s="1">
         <f t="shared" si="57"/>
-        <v>0.33417616446682441</v>
+        <v>0.33572530972389913</v>
       </c>
       <c r="AP85" s="1" t="s">
         <v>38</v>
@@ -16580,7 +16580,7 @@
       </c>
       <c r="N86" s="1">
         <f t="shared" si="39"/>
-        <v>-0.51689462694184252</v>
+        <v>-0.52339236669481404</v>
       </c>
       <c r="O86" s="1">
         <f t="shared" si="40"/>
@@ -16597,7 +16597,7 @@
       </c>
       <c r="S86" s="1">
         <f t="shared" si="41"/>
-        <v>-0.49832928447146346</v>
+        <v>-0.50474096059904183</v>
       </c>
       <c r="T86" s="1">
         <f t="shared" si="42"/>
@@ -16614,7 +16614,7 @@
       </c>
       <c r="X86" s="1">
         <f t="shared" si="43"/>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058624</v>
       </c>
       <c r="Y86" s="1">
         <f t="shared" si="44"/>
@@ -16662,19 +16662,19 @@
       </c>
       <c r="AL86" s="1">
         <f t="shared" si="53"/>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058624</v>
       </c>
       <c r="AM86" s="1">
         <f t="shared" si="54"/>
-        <v>-0.51689462694184252</v>
+        <v>-0.52339236669481404</v>
       </c>
       <c r="AN86" s="1">
         <f t="shared" si="55"/>
-        <v>-0.49832928447146346</v>
+        <v>-0.50474096059904183</v>
       </c>
       <c r="AO86" s="1">
         <f t="shared" si="57"/>
-        <v>3.7130684940758274E-2</v>
+        <v>3.730281219154441E-2</v>
       </c>
       <c r="AP86" s="1" t="s">
         <v>38</v>
@@ -16762,7 +16762,7 @@
       </c>
       <c r="N87" s="1">
         <f t="shared" si="39"/>
-        <v>0.35567646916597667</v>
+        <v>0.3532237198064781</v>
       </c>
       <c r="O87" s="1">
         <f t="shared" si="40"/>
@@ -16779,7 +16779,7 @@
       </c>
       <c r="S87" s="1">
         <f t="shared" si="41"/>
-        <v>0.83837537339583412</v>
+        <v>0.8381602782965546</v>
       </c>
       <c r="T87" s="1">
         <f t="shared" si="42"/>
@@ -16796,7 +16796,7 @@
       </c>
       <c r="X87" s="1">
         <f t="shared" si="43"/>
-        <v>1.0425941405700045</v>
+        <v>1.0433257453500484</v>
       </c>
       <c r="Y87" s="1">
         <f t="shared" si="44"/>
@@ -16844,19 +16844,19 @@
       </c>
       <c r="AL87" s="1">
         <f t="shared" si="53"/>
-        <v>0.35567646916597667</v>
+        <v>0.3532237198064781</v>
       </c>
       <c r="AM87" s="1">
         <f t="shared" si="54"/>
-        <v>0.74554866104393847</v>
+        <v>0.74490324781769368</v>
       </c>
       <c r="AN87" s="1">
         <f t="shared" si="55"/>
-        <v>1.0425941405700045</v>
+        <v>1.0433257453500484</v>
       </c>
       <c r="AO87" s="1">
         <f t="shared" si="57"/>
-        <v>0.68691767140402793</v>
+        <v>0.69010202554357036</v>
       </c>
       <c r="AP87" s="1" t="s">
         <v>38</v>
@@ -17495,7 +17495,7 @@
       </c>
       <c r="S91" s="1">
         <f t="shared" si="41"/>
-        <v>-0.90676681881980437</v>
+        <v>-0.91507189470602968</v>
       </c>
       <c r="T91" s="1">
         <f t="shared" si="42"/>
@@ -17512,7 +17512,7 @@
       </c>
       <c r="X91" s="1">
         <f t="shared" si="43"/>
-        <v>-0.92533216129018347</v>
+        <v>-0.93372330080180177</v>
       </c>
       <c r="Y91" s="1">
         <f t="shared" si="44"/>
@@ -17560,19 +17560,19 @@
       </c>
       <c r="AL91" s="1">
         <f>MIN(N91,S91,X91,AH91)</f>
-        <v>-0.92533216129018347</v>
+        <v>-0.93372330080180177</v>
       </c>
       <c r="AM91" s="1">
         <f>AVERAGE(N91,S91,X91,AH91)</f>
-        <v>-0.91604949005499392</v>
+        <v>-0.92439759775391572</v>
       </c>
       <c r="AN91" s="1">
         <f>MAX(N91,S91,X91,AH91)</f>
-        <v>-0.90676681881980437</v>
+        <v>-0.91507189470602968</v>
       </c>
       <c r="AO91" s="1">
         <f t="shared" ref="AO91" si="58">AN91-AL91</f>
-        <v>1.8565342470379109E-2</v>
+        <v>1.8651406095772094E-2</v>
       </c>
       <c r="AP91" s="1" t="s">
         <v>39</v>
@@ -17657,7 +17657,7 @@
       </c>
       <c r="N92" s="1">
         <f t="shared" si="39"/>
-        <v>-0.36837188717880953</v>
+        <v>-0.37418111792863662</v>
       </c>
       <c r="O92" s="1">
         <f t="shared" si="40"/>
@@ -17674,7 +17674,7 @@
       </c>
       <c r="S92" s="1">
         <f t="shared" si="41"/>
-        <v>-0.27554517482691387</v>
+        <v>-0.28092408744977576</v>
       </c>
       <c r="T92" s="1">
         <f t="shared" si="42"/>
@@ -17691,7 +17691,7 @@
       </c>
       <c r="X92" s="1">
         <f t="shared" si="43"/>
-        <v>-0.51689462694184252</v>
+        <v>-0.52339236669481404</v>
       </c>
       <c r="Y92" s="1">
         <f t="shared" si="44"/>
@@ -17739,19 +17739,19 @@
       </c>
       <c r="AL92" s="1">
         <f>MIN(N92,S92,X92,AH92)</f>
-        <v>-0.51689462694184252</v>
+        <v>-0.52339236669481404</v>
       </c>
       <c r="AM92" s="1">
         <f>AVERAGE(N92,S92,X92,AH92)</f>
-        <v>-0.38693722964918864</v>
+        <v>-0.39283252402440877</v>
       </c>
       <c r="AN92" s="1">
         <f>MAX(N92,S92,X92,AH92)</f>
-        <v>-0.27554517482691387</v>
+        <v>-0.28092408744977576</v>
       </c>
       <c r="AO92" s="1">
         <f t="shared" ref="AO92:AO128" si="59">AN92-AL92</f>
-        <v>0.24134945211492864</v>
+        <v>0.24246827924503828</v>
       </c>
       <c r="AP92" s="1" t="s">
         <v>38</v>
@@ -17833,7 +17833,7 @@
       </c>
       <c r="N93" s="1">
         <f t="shared" si="39"/>
-        <v>0.44850318151787233</v>
+        <v>0.44648075028533896</v>
       </c>
       <c r="O93" s="1">
         <f t="shared" si="40"/>
@@ -17850,7 +17850,7 @@
       </c>
       <c r="S93" s="1">
         <f t="shared" si="41"/>
-        <v>0.4856338664586306</v>
+        <v>0.48378356247688326</v>
       </c>
       <c r="T93" s="1">
         <f t="shared" si="42"/>
@@ -17867,7 +17867,7 @@
       </c>
       <c r="X93" s="1">
         <f t="shared" si="43"/>
-        <v>0.26284975681408101</v>
+        <v>0.25996668932761718</v>
       </c>
       <c r="Y93" s="1">
         <f t="shared" si="44"/>
@@ -17915,19 +17915,19 @@
       </c>
       <c r="AL93" s="1">
         <f>MIN(N93,S93,X93,AH93)</f>
-        <v>0.26284975681408101</v>
+        <v>0.25996668932761718</v>
       </c>
       <c r="AM93" s="1">
         <f>AVERAGE(N93,S93,X93,AH93)</f>
-        <v>0.39899560159686137</v>
+        <v>0.39674366736327982</v>
       </c>
       <c r="AN93" s="1">
         <f>MAX(N93,S93,X93,AH93)</f>
-        <v>0.4856338664586306</v>
+        <v>0.48378356247688326</v>
       </c>
       <c r="AO93" s="1">
         <f t="shared" si="59"/>
-        <v>0.22278410964454959</v>
+        <v>0.22381687314926607</v>
       </c>
       <c r="AP93" s="1" t="s">
         <v>38</v>
@@ -18003,7 +18003,7 @@
       </c>
       <c r="N94" s="1">
         <f t="shared" si="39"/>
-        <v>0.67128729116242192</v>
+        <v>0.67029762343460497</v>
       </c>
       <c r="O94" s="1">
         <f t="shared" si="40"/>
@@ -18020,7 +18020,7 @@
       </c>
       <c r="S94" s="1">
         <f t="shared" si="41"/>
-        <v>1.0054634556292463</v>
+        <v>1.006022933158504</v>
       </c>
       <c r="T94" s="1">
         <f t="shared" si="42"/>
@@ -18037,7 +18037,7 @@
       </c>
       <c r="X94" s="1">
         <f t="shared" si="43"/>
-        <v>0.67128729116242192</v>
+        <v>0.67029762343460497</v>
       </c>
       <c r="Y94" s="1">
         <f t="shared" si="44"/>
@@ -18085,19 +18085,19 @@
       </c>
       <c r="AL94" s="1">
         <f>MIN(N94,S94,X94,AH94)</f>
-        <v>0.67128729116242192</v>
+        <v>0.67029762343460497</v>
       </c>
       <c r="AM94" s="1">
         <f>AVERAGE(N94,S94,X94,AH94)</f>
-        <v>0.78267934598469679</v>
+        <v>0.78220606000923798</v>
       </c>
       <c r="AN94" s="1">
         <f>MAX(N94,S94,X94,AH94)</f>
-        <v>1.0054634556292463</v>
+        <v>1.006022933158504</v>
       </c>
       <c r="AO94" s="1">
         <f t="shared" si="59"/>
-        <v>0.33417616446682441</v>
+        <v>0.33572530972389902</v>
       </c>
       <c r="AP94" s="1" t="s">
         <v>38</v>
@@ -18191,7 +18191,7 @@
       </c>
       <c r="N95" s="1">
         <f t="shared" si="39"/>
-        <v>-1.5630380241605991E-2</v>
+        <v>-1.9804402108965374E-2</v>
       </c>
       <c r="O95" s="1">
         <f t="shared" si="40"/>
@@ -18208,7 +18208,7 @@
       </c>
       <c r="S95" s="1">
         <f t="shared" si="41"/>
-        <v>8.115989621784454</v>
+        <v>8.1495114678392468</v>
       </c>
       <c r="T95" s="1">
         <f t="shared" si="42"/>
@@ -18225,7 +18225,7 @@
       </c>
       <c r="X95" s="1">
         <f t="shared" si="43"/>
-        <v>-0.94389750376056258</v>
+        <v>-0.95237470689757397</v>
       </c>
       <c r="Y95" s="1">
         <f t="shared" si="44"/>
@@ -18273,19 +18273,19 @@
       </c>
       <c r="AL95" s="1">
         <f>MIN(N95,S95,X95,AH95)</f>
-        <v>-0.94389750376056258</v>
+        <v>-0.95237470689757397</v>
       </c>
       <c r="AM95" s="1">
         <f>AVERAGE(N95,S95,X95,AH95)</f>
-        <v>2.3854872459274286</v>
+        <v>2.3924441196109023</v>
       </c>
       <c r="AN95" s="1">
         <f>MAX(N95,S95,X95,AH95)</f>
-        <v>8.115989621784454</v>
+        <v>8.1495114678392468</v>
       </c>
       <c r="AO95" s="1">
         <f t="shared" si="59"/>
-        <v>9.059887125545016</v>
+        <v>9.1018861747368209</v>
       </c>
       <c r="AP95" s="1" t="s">
         <v>38</v>
@@ -18550,7 +18550,7 @@
       </c>
       <c r="N97" s="1">
         <f t="shared" si="39"/>
-        <v>1.3210742776256916</v>
+        <v>1.3230968367866309</v>
       </c>
       <c r="O97" s="1">
         <f t="shared" si="40"/>
@@ -18567,7 +18567,7 @@
       </c>
       <c r="S97" s="1">
         <f t="shared" si="41"/>
-        <v>1.8965998942074447</v>
+        <v>1.9012904257555683</v>
       </c>
       <c r="T97" s="1">
         <f t="shared" si="42"/>
@@ -18584,7 +18584,7 @@
       </c>
       <c r="X97" s="1">
         <f t="shared" si="43"/>
-        <v>1.0982901679811419</v>
+        <v>1.0992799636373649</v>
       </c>
       <c r="Y97" s="1">
         <f t="shared" si="44"/>
@@ -18632,19 +18632,19 @@
       </c>
       <c r="AL97" s="1">
         <f t="shared" ref="AL97:AL128" si="60">MIN(N97,S97,X97,AH97)</f>
-        <v>1.0982901679811419</v>
+        <v>1.0992799636373649</v>
       </c>
       <c r="AM97" s="1">
         <f t="shared" ref="AM97:AM128" si="61">AVERAGE(N97,S97,X97,AH97)</f>
-        <v>1.4386547799380927</v>
+        <v>1.4412224087265215</v>
       </c>
       <c r="AN97" s="1">
         <f t="shared" ref="AN97:AN128" si="62">MAX(N97,S97,X97,AH97)</f>
-        <v>1.8965998942074447</v>
+        <v>1.9012904257555683</v>
       </c>
       <c r="AO97" s="1">
         <f t="shared" si="59"/>
-        <v>0.79830972622630281</v>
+        <v>0.80201046211820337</v>
       </c>
       <c r="AP97" s="1" t="s">
         <v>38</v>
@@ -18729,7 +18729,7 @@
       </c>
       <c r="N98" s="1">
         <f t="shared" si="39"/>
-        <v>0.59702592128090537</v>
+        <v>0.59569199905151626</v>
       </c>
       <c r="O98" s="1">
         <f t="shared" si="40"/>
@@ -18746,7 +18746,7 @@
       </c>
       <c r="S98" s="1">
         <f t="shared" si="41"/>
-        <v>1.1354208529219003</v>
+        <v>1.1365827758289093</v>
       </c>
       <c r="T98" s="1">
         <f t="shared" si="42"/>
@@ -18763,7 +18763,7 @@
       </c>
       <c r="X98" s="1">
         <f t="shared" si="43"/>
-        <v>1.0425941405700045</v>
+        <v>1.0433257453500484</v>
       </c>
       <c r="Y98" s="1">
         <f t="shared" si="44"/>
@@ -18811,19 +18811,19 @@
       </c>
       <c r="AL98" s="1">
         <f t="shared" si="60"/>
-        <v>0.59702592128090537</v>
+        <v>0.59569199905151626</v>
       </c>
       <c r="AM98" s="1">
         <f t="shared" si="61"/>
-        <v>0.92501363825760341</v>
+        <v>0.92520017341015792</v>
       </c>
       <c r="AN98" s="1">
         <f t="shared" si="62"/>
-        <v>1.1354208529219003</v>
+        <v>1.1365827758289093</v>
       </c>
       <c r="AO98" s="1">
         <f t="shared" si="59"/>
-        <v>0.53839493164099494</v>
+        <v>0.54089077677739306</v>
       </c>
       <c r="AP98" s="1" t="s">
         <v>38</v>
@@ -18896,7 +18896,7 @@
       </c>
       <c r="N99" s="1">
         <f t="shared" si="39"/>
-        <v>0.3185457842252184</v>
+        <v>0.31592090761493374</v>
       </c>
       <c r="O99" s="1">
         <f t="shared" si="40"/>
@@ -18913,7 +18913,7 @@
       </c>
       <c r="S99" s="1">
         <f t="shared" si="41"/>
-        <v>0.39280715410673495</v>
+        <v>0.3905265319980224</v>
       </c>
       <c r="T99" s="1">
         <f t="shared" si="42"/>
@@ -18930,7 +18930,7 @@
       </c>
       <c r="X99" s="1">
         <f t="shared" si="43"/>
-        <v>0.39280715410673495</v>
+        <v>0.3905265319980224</v>
       </c>
       <c r="Y99" s="1">
         <f t="shared" si="44"/>
@@ -18978,19 +18978,19 @@
       </c>
       <c r="AL99" s="1">
         <f t="shared" si="60"/>
-        <v>0.3185457842252184</v>
+        <v>0.31592090761493374</v>
       </c>
       <c r="AM99" s="1">
         <f t="shared" si="61"/>
-        <v>0.36805336414622941</v>
+        <v>0.36565799053699283</v>
       </c>
       <c r="AN99" s="1">
         <f t="shared" si="62"/>
-        <v>0.39280715410673495</v>
+        <v>0.3905265319980224</v>
       </c>
       <c r="AO99" s="1">
         <f t="shared" si="59"/>
-        <v>7.4261369881516548E-2</v>
+        <v>7.4605624383088653E-2</v>
       </c>
       <c r="AP99" s="1" t="s">
         <v>38</v>
@@ -19081,7 +19081,7 @@
       </c>
       <c r="N100" s="1">
         <f t="shared" si="39"/>
-        <v>9.576167458066881E-2</v>
+        <v>9.2104034465667659E-2</v>
       </c>
       <c r="O100" s="1">
         <f t="shared" si="40"/>
@@ -19115,7 +19115,7 @@
       </c>
       <c r="X100" s="1">
         <f t="shared" si="43"/>
-        <v>0.11432701705104793</v>
+        <v>0.11075544056143984</v>
       </c>
       <c r="Y100" s="1">
         <f t="shared" si="44"/>
@@ -19163,19 +19163,19 @@
       </c>
       <c r="AL100" s="1">
         <f t="shared" si="60"/>
-        <v>9.576167458066881E-2</v>
+        <v>9.2104034465667659E-2</v>
       </c>
       <c r="AM100" s="1">
         <f t="shared" si="61"/>
-        <v>0.10504434581585836</v>
+        <v>0.10142973751355375</v>
       </c>
       <c r="AN100" s="1">
         <f t="shared" si="62"/>
-        <v>0.11432701705104793</v>
+        <v>0.11075544056143984</v>
       </c>
       <c r="AO100" s="1">
         <f t="shared" si="59"/>
-        <v>1.8565342470379123E-2</v>
+        <v>1.8651406095772177E-2</v>
       </c>
       <c r="AP100" s="1" t="s">
         <v>39</v>
@@ -19260,7 +19260,7 @@
       </c>
       <c r="N101" s="1">
         <f t="shared" si="39"/>
-        <v>-0.42406791458994691</v>
+        <v>-0.43013533621595318</v>
       </c>
       <c r="O101" s="1">
         <f t="shared" si="40"/>
@@ -19277,7 +19277,7 @@
       </c>
       <c r="S101" s="1">
         <f t="shared" si="41"/>
-        <v>-0.29411051729729298</v>
+        <v>-0.29957549354554797</v>
       </c>
       <c r="T101" s="1">
         <f t="shared" si="42"/>
@@ -19294,7 +19294,7 @@
       </c>
       <c r="X101" s="1">
         <f t="shared" si="43"/>
-        <v>-0.38693722964918864</v>
+        <v>-0.39283252402440882</v>
       </c>
       <c r="Y101" s="1">
         <f t="shared" si="44"/>
@@ -19342,19 +19342,19 @@
       </c>
       <c r="AL101" s="1">
         <f t="shared" si="60"/>
-        <v>-0.42406791458994691</v>
+        <v>-0.43013533621595318</v>
       </c>
       <c r="AM101" s="1">
         <f t="shared" si="61"/>
-        <v>-0.36837188717880953</v>
+        <v>-0.37418111792863668</v>
       </c>
       <c r="AN101" s="1">
         <f t="shared" si="62"/>
-        <v>-0.29411051729729298</v>
+        <v>-0.29957549354554797</v>
       </c>
       <c r="AO101" s="1">
         <f t="shared" si="59"/>
-        <v>0.12995739729265393</v>
+        <v>0.13055984267040521</v>
       </c>
       <c r="AP101" s="1" t="s">
         <v>38</v>
@@ -19436,7 +19436,7 @@
       </c>
       <c r="N102" s="1">
         <f t="shared" si="39"/>
-        <v>-0.27554517482691387</v>
+        <v>-0.28092408744977576</v>
       </c>
       <c r="O102" s="1">
         <f t="shared" si="40"/>
@@ -19453,7 +19453,7 @@
       </c>
       <c r="S102" s="1">
         <f t="shared" si="41"/>
-        <v>0.29998044175483929</v>
+        <v>0.29726950151916154</v>
       </c>
       <c r="T102" s="1">
         <f t="shared" si="42"/>
@@ -19470,7 +19470,7 @@
       </c>
       <c r="X102" s="1">
         <f t="shared" si="43"/>
-        <v>-1.5630380241605991E-2</v>
+        <v>-1.9804402108965374E-2</v>
       </c>
       <c r="Y102" s="1">
         <f t="shared" si="44"/>
@@ -19518,19 +19518,19 @@
       </c>
       <c r="AL102" s="1">
         <f t="shared" si="60"/>
-        <v>-0.27554517482691387</v>
+        <v>-0.28092408744977576</v>
       </c>
       <c r="AM102" s="1">
         <f t="shared" si="61"/>
-        <v>2.9349622287731408E-3</v>
+        <v>-1.1529960131931988E-3</v>
       </c>
       <c r="AN102" s="1">
         <f t="shared" si="62"/>
-        <v>0.29998044175483929</v>
+        <v>0.29726950151916154</v>
       </c>
       <c r="AO102" s="1">
         <f t="shared" si="59"/>
-        <v>0.57552561658175316</v>
+        <v>0.57819358896893736</v>
       </c>
       <c r="AP102" s="1" t="s">
         <v>38</v>
@@ -19799,7 +19799,7 @@
       </c>
       <c r="N104" s="1">
         <f t="shared" si="39"/>
-        <v>-0.66541736670487561</v>
+        <v>-0.67260361546099146</v>
       </c>
       <c r="O104" s="1">
         <f t="shared" si="40"/>
@@ -19813,7 +19813,7 @@
       </c>
       <c r="S104" s="1">
         <f t="shared" si="41"/>
-        <v>-0.57259065435297996</v>
+        <v>-0.57934658498213054</v>
       </c>
       <c r="T104" s="1">
         <f t="shared" si="42"/>
@@ -19827,7 +19827,7 @@
       </c>
       <c r="X104" s="1">
         <f t="shared" si="43"/>
-        <v>-0.29411051729729298</v>
+        <v>-0.29957549354554797</v>
       </c>
       <c r="Y104" s="1">
         <f t="shared" si="44"/>
@@ -19872,19 +19872,19 @@
       </c>
       <c r="AL104" s="1">
         <f t="shared" si="60"/>
-        <v>-0.66541736670487561</v>
+        <v>-0.67260361546099146</v>
       </c>
       <c r="AM104" s="1">
         <f t="shared" si="61"/>
-        <v>-0.51070617945171615</v>
+        <v>-0.51717523132955667</v>
       </c>
       <c r="AN104" s="1">
         <f t="shared" si="62"/>
-        <v>-0.29411051729729298</v>
+        <v>-0.29957549354554797</v>
       </c>
       <c r="AO104" s="1">
         <f t="shared" si="59"/>
-        <v>0.37130684940758263</v>
+        <v>0.37302812191544349</v>
       </c>
       <c r="AP104" s="1" t="s">
         <v>38</v>
@@ -19963,7 +19963,7 @@
       </c>
       <c r="N105" s="1">
         <f t="shared" si="39"/>
-        <v>-0.75824407905677127</v>
+        <v>-0.76586064593985226</v>
       </c>
       <c r="O105" s="1">
         <f t="shared" si="40"/>
@@ -19980,7 +19980,7 @@
       </c>
       <c r="S105" s="1">
         <f t="shared" si="41"/>
-        <v>-0.51689462694184252</v>
+        <v>-0.52339236669481404</v>
       </c>
       <c r="T105" s="1">
         <f t="shared" si="42"/>
@@ -19997,7 +19997,7 @@
       </c>
       <c r="X105" s="1">
         <f t="shared" si="43"/>
-        <v>-0.33124120223805126</v>
+        <v>-0.33687830573709232</v>
       </c>
       <c r="Y105" s="1">
         <f t="shared" si="44"/>
@@ -20014,7 +20014,7 @@
       </c>
       <c r="AC105" s="1">
         <f t="shared" si="45"/>
-        <v>-0.38693722964918864</v>
+        <v>-0.39283252402440882</v>
       </c>
       <c r="AD105" s="1">
         <f t="shared" si="46"/>
@@ -20045,19 +20045,19 @@
       </c>
       <c r="AL105" s="1">
         <f t="shared" si="60"/>
-        <v>-0.75824407905677127</v>
+        <v>-0.76586064593985226</v>
       </c>
       <c r="AM105" s="1">
         <f t="shared" si="61"/>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058613</v>
       </c>
       <c r="AN105" s="1">
         <f t="shared" si="62"/>
-        <v>-0.33124120223805126</v>
+        <v>-0.33687830573709232</v>
       </c>
       <c r="AO105" s="1">
         <f t="shared" si="59"/>
-        <v>0.42700287681872001</v>
+        <v>0.42898234020275994</v>
       </c>
       <c r="AP105" s="1" t="s">
         <v>38</v>
@@ -20301,7 +20301,7 @@
       </c>
       <c r="N107" s="1">
         <f t="shared" si="39"/>
-        <v>-1.5630380241605991E-2</v>
+        <v>-1.9804402108965374E-2</v>
       </c>
       <c r="O107" s="1">
         <f t="shared" si="40"/>
@@ -20349,7 +20349,7 @@
       </c>
       <c r="AC107" s="1">
         <f t="shared" si="45"/>
-        <v>5.8630989639910536E-2</v>
+        <v>5.4801222274123318E-2</v>
       </c>
       <c r="AD107" s="1">
         <f t="shared" si="46"/>
@@ -20377,15 +20377,15 @@
       </c>
       <c r="AL107" s="1">
         <f t="shared" si="60"/>
-        <v>-1.5630380241605991E-2</v>
+        <v>-1.9804402108965374E-2</v>
       </c>
       <c r="AM107" s="1">
         <f t="shared" si="61"/>
-        <v>-1.5630380241605991E-2</v>
+        <v>-1.9804402108965374E-2</v>
       </c>
       <c r="AN107" s="1">
         <f t="shared" si="62"/>
-        <v>-1.5630380241605991E-2</v>
+        <v>-1.9804402108965374E-2</v>
       </c>
       <c r="AO107" s="1">
         <f t="shared" si="59"/>
@@ -20830,7 +20830,7 @@
       </c>
       <c r="N110" s="1">
         <f t="shared" si="39"/>
-        <v>-0.55402531188260085</v>
+        <v>-0.56069517888635834</v>
       </c>
       <c r="O110" s="1">
         <f t="shared" si="40"/>
@@ -20864,7 +20864,7 @@
       </c>
       <c r="X110" s="1">
         <f t="shared" si="43"/>
-        <v>-0.70254805164563394</v>
+        <v>-0.70990642765253575</v>
       </c>
       <c r="Y110" s="1">
         <f t="shared" si="44"/>
@@ -20898,7 +20898,7 @@
       </c>
       <c r="AH110" s="1">
         <f t="shared" si="47"/>
-        <v>-0.72111339411601305</v>
+        <v>-0.72855783374830796</v>
       </c>
       <c r="AI110" s="1">
         <f t="shared" si="48"/>
@@ -20912,19 +20912,19 @@
       </c>
       <c r="AL110" s="1">
         <f t="shared" si="60"/>
-        <v>-0.72111339411601305</v>
+        <v>-0.72855783374830796</v>
       </c>
       <c r="AM110" s="1">
         <f t="shared" si="61"/>
-        <v>-0.65922891921474924</v>
+        <v>-0.66638648009573398</v>
       </c>
       <c r="AN110" s="1">
         <f t="shared" si="62"/>
-        <v>-0.55402531188260085</v>
+        <v>-0.56069517888635834</v>
       </c>
       <c r="AO110" s="1">
         <f t="shared" si="59"/>
-        <v>0.16708808223341221</v>
+        <v>0.16786265486194962</v>
       </c>
       <c r="AP110" s="1" t="s">
         <v>39</v>
@@ -21169,7 +21169,7 @@
       </c>
       <c r="N112" s="1">
         <f t="shared" si="39"/>
-        <v>-0.57259065435297996</v>
+        <v>-0.57934658498213054</v>
       </c>
       <c r="O112" s="1">
         <f t="shared" si="40"/>
@@ -21186,7 +21186,7 @@
       </c>
       <c r="S112" s="1">
         <f t="shared" si="41"/>
-        <v>-0.62828668176411739</v>
+        <v>-0.63530080326944705</v>
       </c>
       <c r="T112" s="1">
         <f t="shared" si="42"/>
@@ -21203,7 +21203,7 @@
       </c>
       <c r="X112" s="1">
         <f t="shared" si="43"/>
-        <v>-0.73967873658639216</v>
+        <v>-0.74720923984408005</v>
       </c>
       <c r="Y112" s="1">
         <f t="shared" si="44"/>
@@ -21251,19 +21251,19 @@
       </c>
       <c r="AL112" s="1">
         <f t="shared" si="60"/>
-        <v>-0.73967873658639216</v>
+        <v>-0.74720923984408005</v>
       </c>
       <c r="AM112" s="1">
         <f t="shared" si="61"/>
-        <v>-0.6468520242344965</v>
+        <v>-0.65395220936521925</v>
       </c>
       <c r="AN112" s="1">
         <f t="shared" si="62"/>
-        <v>-0.57259065435297996</v>
+        <v>-0.57934658498213054</v>
       </c>
       <c r="AO112" s="1">
         <f t="shared" si="59"/>
-        <v>0.16708808223341221</v>
+        <v>0.16786265486194951</v>
       </c>
       <c r="AP112" s="1" t="s">
         <v>38</v>
@@ -21351,7 +21351,7 @@
       </c>
       <c r="N113" s="1">
         <f t="shared" si="39"/>
-        <v>2.1500304699152272E-2</v>
+        <v>1.749841008257897E-2</v>
       </c>
       <c r="O113" s="1">
         <f t="shared" si="40"/>
@@ -21368,7 +21368,7 @@
       </c>
       <c r="S113" s="1">
         <f t="shared" si="41"/>
-        <v>0.26284975681408101</v>
+        <v>0.25996668932761718</v>
       </c>
       <c r="T113" s="1">
         <f t="shared" si="42"/>
@@ -21385,7 +21385,7 @@
       </c>
       <c r="X113" s="1">
         <f t="shared" si="43"/>
-        <v>0.29998044175483929</v>
+        <v>0.29726950151916154</v>
       </c>
       <c r="Y113" s="1">
         <f t="shared" si="44"/>
@@ -21433,19 +21433,19 @@
       </c>
       <c r="AL113" s="1">
         <f t="shared" si="60"/>
-        <v>2.1500304699152272E-2</v>
+        <v>1.749841008257897E-2</v>
       </c>
       <c r="AM113" s="1">
         <f t="shared" si="61"/>
-        <v>0.19477683442269086</v>
+        <v>0.1915782003097859</v>
       </c>
       <c r="AN113" s="1">
         <f t="shared" si="62"/>
-        <v>0.29998044175483929</v>
+        <v>0.29726950151916154</v>
       </c>
       <c r="AO113" s="1">
         <f t="shared" si="59"/>
-        <v>0.27848013705568703</v>
+        <v>0.27977109143658258</v>
       </c>
       <c r="AP113" s="1" t="s">
         <v>38</v>
@@ -21533,7 +21533,7 @@
       </c>
       <c r="N114" s="1">
         <f t="shared" si="39"/>
-        <v>-0.18271846247501819</v>
+        <v>-0.18766705697091493</v>
       </c>
       <c r="O114" s="1">
         <f t="shared" si="40"/>
@@ -21550,7 +21550,7 @@
       </c>
       <c r="S114" s="1">
         <f t="shared" si="41"/>
-        <v>-0.31267585976767209</v>
+        <v>-0.31822689964132012</v>
       </c>
       <c r="T114" s="1">
         <f t="shared" si="42"/>
@@ -21567,7 +21567,7 @@
       </c>
       <c r="X114" s="1">
         <f t="shared" si="43"/>
-        <v>-0.31267585976767209</v>
+        <v>-0.31822689964132012</v>
       </c>
       <c r="Y114" s="1">
         <f t="shared" si="44"/>
@@ -21584,7 +21584,7 @@
       </c>
       <c r="AC114" s="1">
         <f t="shared" si="45"/>
-        <v>-0.25697983235653471</v>
+        <v>-0.26227268135400361</v>
       </c>
       <c r="AD114" s="1">
         <f t="shared" si="46"/>
@@ -21615,19 +21615,19 @@
       </c>
       <c r="AL114" s="1">
         <f t="shared" si="60"/>
-        <v>-0.31267585976767209</v>
+        <v>-0.31822689964132012</v>
       </c>
       <c r="AM114" s="1">
         <f t="shared" si="61"/>
-        <v>-0.26935672733678745</v>
+        <v>-0.2747069520845184</v>
       </c>
       <c r="AN114" s="1">
         <f t="shared" si="62"/>
-        <v>-0.18271846247501819</v>
+        <v>-0.18766705697091493</v>
       </c>
       <c r="AO114" s="1">
         <f t="shared" si="59"/>
-        <v>0.1299573972926539</v>
+        <v>0.13055984267040519</v>
       </c>
       <c r="AP114" s="1" t="s">
         <v>38</v>
@@ -21703,7 +21703,7 @@
       </c>
       <c r="N115" s="1">
         <f t="shared" si="39"/>
-        <v>-0.86963613387904604</v>
+        <v>-0.87776908251448527</v>
       </c>
       <c r="O115" s="1">
         <f t="shared" si="40"/>
@@ -21737,7 +21737,7 @@
       </c>
       <c r="X115" s="1">
         <f t="shared" si="43"/>
-        <v>-0.85107079140866693</v>
+        <v>-0.85911767641871317</v>
       </c>
       <c r="Y115" s="1">
         <f t="shared" si="44"/>
@@ -21771,7 +21771,7 @@
       </c>
       <c r="AH115" s="1">
         <f t="shared" si="47"/>
-        <v>-0.86963613387904604</v>
+        <v>-0.87776908251448527</v>
       </c>
       <c r="AI115" s="1">
         <f t="shared" si="48"/>
@@ -21785,19 +21785,19 @@
       </c>
       <c r="AL115" s="1">
         <f t="shared" si="60"/>
-        <v>-0.86963613387904604</v>
+        <v>-0.87776908251448527</v>
       </c>
       <c r="AM115" s="1">
         <f t="shared" si="61"/>
-        <v>-0.86344768638891967</v>
+        <v>-0.87155194714922801</v>
       </c>
       <c r="AN115" s="1">
         <f t="shared" si="62"/>
-        <v>-0.85107079140866693</v>
+        <v>-0.85911767641871317</v>
       </c>
       <c r="AO115" s="1">
         <f t="shared" si="59"/>
-        <v>1.8565342470379109E-2</v>
+        <v>1.8651406095772094E-2</v>
       </c>
       <c r="AP115" s="1" t="s">
         <v>39</v>
@@ -21876,7 +21876,7 @@
       </c>
       <c r="N116" s="1">
         <f t="shared" si="39"/>
-        <v>-0.46119859953070519</v>
+        <v>-0.46743814840749753</v>
       </c>
       <c r="O116" s="1">
         <f t="shared" si="40"/>
@@ -21890,7 +21890,7 @@
       </c>
       <c r="S116" s="1">
         <f t="shared" si="41"/>
-        <v>0.11432701705104793</v>
+        <v>0.11075544056143984</v>
       </c>
       <c r="T116" s="1">
         <f t="shared" si="42"/>
@@ -21904,7 +21904,7 @@
       </c>
       <c r="X116" s="1">
         <f t="shared" si="43"/>
-        <v>-0.34980654470843037</v>
+        <v>-0.35552971183286447</v>
       </c>
       <c r="Y116" s="1">
         <f t="shared" si="44"/>
@@ -21949,19 +21949,19 @@
       </c>
       <c r="AL116" s="1">
         <f t="shared" si="60"/>
-        <v>-0.46119859953070519</v>
+        <v>-0.46743814840749753</v>
       </c>
       <c r="AM116" s="1">
         <f t="shared" si="61"/>
-        <v>-0.2322260423960292</v>
+        <v>-0.23740413989297404</v>
       </c>
       <c r="AN116" s="1">
         <f t="shared" si="62"/>
-        <v>0.11432701705104793</v>
+        <v>0.11075544056143984</v>
       </c>
       <c r="AO116" s="1">
         <f t="shared" si="59"/>
-        <v>0.57552561658175316</v>
+        <v>0.57819358896893736</v>
       </c>
       <c r="AP116" s="1" t="s">
         <v>38</v>
@@ -22037,7 +22037,7 @@
       </c>
       <c r="N117" s="1">
         <f t="shared" si="39"/>
-        <v>-0.77680942152715038</v>
+        <v>-0.78451205203562446</v>
       </c>
       <c r="O117" s="1">
         <f t="shared" si="40"/>
@@ -22071,7 +22071,7 @@
       </c>
       <c r="X117" s="1">
         <f t="shared" si="43"/>
-        <v>-0.66541736670487561</v>
+        <v>-0.67260361546099146</v>
       </c>
       <c r="Y117" s="1">
         <f t="shared" si="44"/>
@@ -22105,7 +22105,7 @@
       </c>
       <c r="AH117" s="1">
         <f t="shared" si="47"/>
-        <v>-0.81394010646790871</v>
+        <v>-0.82181486422716876</v>
       </c>
       <c r="AI117" s="1">
         <f t="shared" si="48"/>
@@ -22119,19 +22119,19 @@
       </c>
       <c r="AL117" s="1">
         <f t="shared" si="60"/>
-        <v>-0.81394010646790871</v>
+        <v>-0.82181486422716876</v>
       </c>
       <c r="AM117" s="1">
         <f t="shared" si="61"/>
-        <v>-0.75205563156664501</v>
+        <v>-0.759643510574595</v>
       </c>
       <c r="AN117" s="1">
         <f t="shared" si="62"/>
-        <v>-0.66541736670487561</v>
+        <v>-0.67260361546099146</v>
       </c>
       <c r="AO117" s="1">
         <f t="shared" si="59"/>
-        <v>0.1485227397630331</v>
+        <v>0.14921124876617731</v>
       </c>
       <c r="AP117" s="1" t="s">
         <v>39</v>
@@ -22207,7 +22207,7 @@
       </c>
       <c r="N118" s="1">
         <f t="shared" si="39"/>
-        <v>-0.29411051729729298</v>
+        <v>-0.29957549354554797</v>
       </c>
       <c r="O118" s="1">
         <f t="shared" si="40"/>
@@ -22224,7 +22224,7 @@
       </c>
       <c r="S118" s="1">
         <f t="shared" si="41"/>
-        <v>-1.5630380241605991E-2</v>
+        <v>-1.9804402108965374E-2</v>
       </c>
       <c r="T118" s="1">
         <f t="shared" si="42"/>
@@ -22241,7 +22241,7 @@
       </c>
       <c r="X118" s="1">
         <f t="shared" si="43"/>
-        <v>0.15145770199180619</v>
+        <v>0.14805825275298418</v>
       </c>
       <c r="Y118" s="1">
         <f t="shared" si="44"/>
@@ -22289,19 +22289,19 @@
       </c>
       <c r="AL118" s="1">
         <f t="shared" si="60"/>
-        <v>-0.29411051729729298</v>
+        <v>-0.29957549354554797</v>
       </c>
       <c r="AM118" s="1">
         <f t="shared" si="61"/>
-        <v>-5.2761065182364265E-2</v>
+        <v>-5.7107214300509725E-2</v>
       </c>
       <c r="AN118" s="1">
         <f t="shared" si="62"/>
-        <v>0.15145770199180619</v>
+        <v>0.14805825275298418</v>
       </c>
       <c r="AO118" s="1">
         <f t="shared" si="59"/>
-        <v>0.44556821928909918</v>
+        <v>0.44763374629853214</v>
       </c>
       <c r="AP118" s="1" t="s">
         <v>38</v>
@@ -22392,7 +22392,7 @@
       </c>
       <c r="N119" s="1">
         <f t="shared" si="39"/>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058624</v>
       </c>
       <c r="O119" s="1">
         <f t="shared" si="40"/>
@@ -22423,7 +22423,7 @@
       </c>
       <c r="X119" s="1">
         <f t="shared" si="43"/>
-        <v>7.7196332110289673E-2</v>
+        <v>7.3452628369895495E-2</v>
       </c>
       <c r="Y119" s="1">
         <f t="shared" si="44"/>
@@ -22468,19 +22468,19 @@
       </c>
       <c r="AL119" s="1">
         <f t="shared" si="60"/>
-        <v>-0.53545996941222174</v>
+        <v>-0.54204377279058624</v>
       </c>
       <c r="AM119" s="1">
         <f t="shared" si="61"/>
-        <v>-0.22913181865096605</v>
+        <v>-0.23429557221034536</v>
       </c>
       <c r="AN119" s="1">
         <f t="shared" si="62"/>
-        <v>7.7196332110289673E-2</v>
+        <v>7.3452628369895495E-2</v>
       </c>
       <c r="AO119" s="1">
         <f t="shared" si="59"/>
-        <v>0.61265630152251138</v>
+        <v>0.61549640116048177</v>
       </c>
       <c r="AP119" s="1" t="s">
         <v>39</v>
@@ -22743,7 +22743,7 @@
       </c>
       <c r="N121" s="1">
         <f t="shared" si="39"/>
-        <v>-0.29411051729729298</v>
+        <v>-0.29957549354554797</v>
       </c>
       <c r="O121" s="1">
         <f t="shared" si="40"/>
@@ -22760,7 +22760,7 @@
       </c>
       <c r="S121" s="1">
         <f t="shared" si="41"/>
-        <v>-0.16415312000463905</v>
+        <v>-0.16901565087514275</v>
       </c>
       <c r="T121" s="1">
         <f t="shared" si="42"/>
@@ -22777,7 +22777,7 @@
       </c>
       <c r="X121" s="1">
         <f t="shared" si="43"/>
-        <v>-0.34980654470843037</v>
+        <v>-0.35552971183286447</v>
       </c>
       <c r="Y121" s="1">
         <f t="shared" si="44"/>
@@ -22825,19 +22825,19 @@
       </c>
       <c r="AL121" s="1">
         <f t="shared" si="60"/>
-        <v>-0.34980654470843037</v>
+        <v>-0.35552971183286447</v>
       </c>
       <c r="AM121" s="1">
         <f t="shared" si="61"/>
-        <v>-0.26935672733678745</v>
+        <v>-0.2747069520845184</v>
       </c>
       <c r="AN121" s="1">
         <f t="shared" si="62"/>
-        <v>-0.16415312000463905</v>
+        <v>-0.16901565087514275</v>
       </c>
       <c r="AO121" s="1">
         <f t="shared" si="59"/>
-        <v>0.18565342470379131</v>
+        <v>0.18651406095772172</v>
       </c>
       <c r="AP121" s="1" t="s">
         <v>38</v>
@@ -22925,7 +22925,7 @@
       </c>
       <c r="N122" s="1">
         <f t="shared" si="39"/>
-        <v>-0.85107079140866693</v>
+        <v>-0.85911767641871317</v>
       </c>
       <c r="O122" s="1">
         <f t="shared" si="40"/>
@@ -22942,7 +22942,7 @@
       </c>
       <c r="S122" s="1">
         <f t="shared" si="41"/>
-        <v>-0.7953747639975296</v>
+        <v>-0.80316345813139656</v>
       </c>
       <c r="T122" s="1">
         <f t="shared" si="42"/>
@@ -22959,7 +22959,7 @@
       </c>
       <c r="X122" s="1">
         <f t="shared" si="43"/>
-        <v>-0.92533216129018347</v>
+        <v>-0.93372330080180177</v>
       </c>
       <c r="Y122" s="1">
         <f t="shared" si="44"/>
@@ -23007,19 +23007,19 @@
       </c>
       <c r="AL122" s="1">
         <f t="shared" si="60"/>
-        <v>-0.92533216129018347</v>
+        <v>-0.93372330080180177</v>
       </c>
       <c r="AM122" s="1">
         <f t="shared" si="61"/>
-        <v>-0.8572592388987933</v>
+        <v>-0.86533481178397054</v>
       </c>
       <c r="AN122" s="1">
         <f t="shared" si="62"/>
-        <v>-0.7953747639975296</v>
+        <v>-0.80316345813139656</v>
       </c>
       <c r="AO122" s="1">
         <f t="shared" si="59"/>
-        <v>0.12995739729265388</v>
+        <v>0.13055984267040521</v>
       </c>
       <c r="AP122" s="1" t="s">
         <v>38</v>
@@ -23101,7 +23101,7 @@
       </c>
       <c r="N123" s="1">
         <f t="shared" si="39"/>
-        <v>-7.1326407652743395E-2</v>
+        <v>-7.5758620396281895E-2</v>
       </c>
       <c r="O123" s="1">
         <f t="shared" si="40"/>
@@ -23118,7 +23118,7 @@
       </c>
       <c r="S123" s="1">
         <f t="shared" si="41"/>
-        <v>0.2071537294029436</v>
+        <v>0.20401247104030071</v>
       </c>
       <c r="T123" s="1">
         <f t="shared" si="42"/>
@@ -23135,7 +23135,7 @@
       </c>
       <c r="X123" s="1">
         <f t="shared" si="43"/>
-        <v>5.8630989639910536E-2</v>
+        <v>5.4801222274123318E-2</v>
       </c>
       <c r="Y123" s="1">
         <f t="shared" si="44"/>
@@ -23183,19 +23183,19 @@
       </c>
       <c r="AL123" s="1">
         <f t="shared" si="60"/>
-        <v>-7.1326407652743395E-2</v>
+        <v>-7.5758620396281895E-2</v>
       </c>
       <c r="AM123" s="1">
         <f t="shared" si="61"/>
-        <v>6.4819437130036919E-2</v>
+        <v>6.101835763938071E-2</v>
       </c>
       <c r="AN123" s="1">
         <f t="shared" si="62"/>
-        <v>0.2071537294029436</v>
+        <v>0.20401247104030071</v>
       </c>
       <c r="AO123" s="1">
         <f t="shared" si="59"/>
-        <v>0.27848013705568697</v>
+        <v>0.27977109143658263</v>
       </c>
       <c r="AP123" s="1" t="s">
         <v>38</v>
@@ -23440,7 +23440,7 @@
       </c>
       <c r="N125" s="1">
         <f t="shared" si="39"/>
-        <v>7.7196332110289673E-2</v>
+        <v>7.3452628369895495E-2</v>
       </c>
       <c r="O125" s="1">
         <f t="shared" si="40"/>
@@ -23474,7 +23474,7 @@
       </c>
       <c r="X125" s="1">
         <f t="shared" si="43"/>
-        <v>-0.20128380494539733</v>
+        <v>-0.20631846306668711</v>
       </c>
       <c r="Y125" s="1">
         <f t="shared" si="44"/>
@@ -23522,19 +23522,19 @@
       </c>
       <c r="AL125" s="1">
         <f t="shared" si="60"/>
-        <v>-0.20128380494539733</v>
+        <v>-0.20631846306668711</v>
       </c>
       <c r="AM125" s="1">
         <f t="shared" si="61"/>
-        <v>-6.2043736417553827E-2</v>
+        <v>-6.6432917348395806E-2</v>
       </c>
       <c r="AN125" s="1">
         <f t="shared" si="62"/>
-        <v>7.7196332110289673E-2</v>
+        <v>7.3452628369895495E-2</v>
       </c>
       <c r="AO125" s="1">
         <f t="shared" si="59"/>
-        <v>0.27848013705568697</v>
+        <v>0.27977109143658263</v>
       </c>
       <c r="AP125" s="1" t="s">
         <v>39</v>
@@ -23763,7 +23763,7 @@
       </c>
       <c r="N127" s="1">
         <f t="shared" si="39"/>
-        <v>-0.25697983235653471</v>
+        <v>-0.26227268135400361</v>
       </c>
       <c r="O127" s="1">
         <f t="shared" si="40"/>
@@ -23797,7 +23797,7 @@
       </c>
       <c r="X127" s="1">
         <f t="shared" si="43"/>
-        <v>5.8630989639910536E-2</v>
+        <v>5.4801222274123318E-2</v>
       </c>
       <c r="Y127" s="1">
         <f t="shared" si="44"/>
@@ -23845,19 +23845,19 @@
       </c>
       <c r="AL127" s="1">
         <f t="shared" si="60"/>
-        <v>-0.25697983235653471</v>
+        <v>-0.26227268135400361</v>
       </c>
       <c r="AM127" s="1">
         <f t="shared" si="61"/>
-        <v>-9.9174421358312087E-2</v>
+        <v>-0.10373572953994015</v>
       </c>
       <c r="AN127" s="1">
         <f t="shared" si="62"/>
-        <v>5.8630989639910536E-2</v>
+        <v>5.4801222274123318E-2</v>
       </c>
       <c r="AO127" s="1">
         <f t="shared" si="59"/>
-        <v>0.31561082199644525</v>
+        <v>0.31707390362812693</v>
       </c>
       <c r="AP127" s="1" t="s">
         <v>39</v>
@@ -23906,12 +23906,15 @@
       <c r="C128" s="6">
         <v>3</v>
       </c>
+      <c r="D128" s="1">
+        <v>40</v>
+      </c>
       <c r="E128" s="1">
         <v>37</v>
       </c>
       <c r="F128" s="1">
         <f t="shared" si="38"/>
-        <v>-37</v>
+        <v>3</v>
       </c>
       <c r="G128" s="1">
         <v>1.67</v>
@@ -23925,37 +23928,79 @@
       <c r="J128" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="K128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L128" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M128" s="1">
+        <v>65</v>
+      </c>
       <c r="N128" s="1">
         <f t="shared" si="39"/>
-        <v>-0.94389750376056258</v>
+        <v>0.25996668932761718</v>
       </c>
       <c r="O128" s="1">
         <f t="shared" si="40"/>
-        <v>-8.0392156862745097</v>
+        <v>4.7058823529411766</v>
+      </c>
+      <c r="P128" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q128" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R128" s="1">
+        <v>81</v>
       </c>
       <c r="S128" s="1">
         <f t="shared" si="41"/>
-        <v>-0.94389750376056258</v>
+        <v>0.55838918685997196</v>
       </c>
       <c r="T128" s="1">
         <f t="shared" si="42"/>
-        <v>-8.0392156862745097</v>
+        <v>7.8431372549019605</v>
+      </c>
+      <c r="U128" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V128" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W128" s="1">
+        <v>67</v>
       </c>
       <c r="X128" s="1">
         <f t="shared" si="43"/>
-        <v>-0.94389750376056258</v>
+        <v>0.29726950151916154</v>
       </c>
       <c r="Y128" s="1">
         <f t="shared" si="44"/>
-        <v>-8.0392156862745097</v>
-      </c>
-      <c r="AC128" s="1">
+        <v>5.0980392156862742</v>
+      </c>
+      <c r="Z128" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA128" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB128" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC128" s="1" t="str">
         <f t="shared" si="45"/>
-        <v>-0.94389750376056258</v>
-      </c>
-      <c r="AD128" s="1">
+        <v>null</v>
+      </c>
+      <c r="AD128" s="1" t="str">
         <f t="shared" si="46"/>
-        <v>-8.0392156862745097</v>
+        <v>null</v>
+      </c>
+      <c r="AE128" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF128" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="AG128" s="1" t="s">
         <v>36</v>
@@ -23976,19 +24021,19 @@
       </c>
       <c r="AL128" s="1">
         <f t="shared" si="60"/>
-        <v>-0.94389750376056258</v>
+        <v>0.25996668932761718</v>
       </c>
       <c r="AM128" s="1">
         <f t="shared" si="61"/>
-        <v>-0.94389750376056247</v>
+        <v>0.37187512590225019</v>
       </c>
       <c r="AN128" s="1">
         <f t="shared" si="62"/>
-        <v>-0.94389750376056258</v>
+        <v>0.55838918685997196</v>
       </c>
       <c r="AO128" s="1">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>0.29842249753235478</v>
       </c>
       <c r="AP128" s="1" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Updated First Turn database
</commit_message>
<xml_diff>
--- a/projects/firstTurnData/FirstTurnCombined.xlsx
+++ b/projects/firstTurnData/FirstTurnCombined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PNJae\Dropbox\website\PNJaenichen.github.io\projects\firstTurnData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEE76A8-FFA9-4876-AE9D-79B00DA62DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E02BFD-4E3A-4D20-A751-BB4045651333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
+    <workbookView xWindow="-30" yWindow="0" windowWidth="28830" windowHeight="15600" activeTab="1" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3426" uniqueCount="346">
   <si>
     <t>Yes</t>
   </si>
@@ -1059,6 +1059,24 @@
   <si>
     <t>mechanic18</t>
   </si>
+  <si>
+    <t>Nidavellir</t>
+  </si>
+  <si>
+    <t>Villainous</t>
+  </si>
+  <si>
+    <t>Inner Compass</t>
+  </si>
+  <si>
+    <t>Constrained Bidding</t>
+  </si>
+  <si>
+    <t>Turn Order: Auction</t>
+  </si>
+  <si>
+    <t>Victory Points as a Resource</t>
+  </si>
 </sst>
 </file>
 
@@ -1425,11 +1443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796E82C3-294D-4E4E-8DE4-13BF7BF427EB}">
-  <dimension ref="A1:BO128"/>
+  <dimension ref="A1:BO131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="V1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AU128" sqref="AU128"/>
+      <selection pane="bottomLeft" activeCell="M131" sqref="M131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12974,7 +12992,7 @@
         <v>90</v>
       </c>
       <c r="F66" s="1">
-        <f t="shared" ref="F66:F128" si="38">D66-E66</f>
+        <f t="shared" ref="F66:F129" si="38">D66-E66</f>
         <v>30</v>
       </c>
       <c r="G66" s="1">
@@ -13234,7 +13252,7 @@
         <v>-0.67260361546099146</v>
       </c>
       <c r="T67" s="1">
-        <f t="shared" ref="T67:T128" si="42">IF(R67="null","null",10*((R67-$AS67)/($AT67-$AS67)))</f>
+        <f t="shared" ref="T67:T130" si="42">IF(R67="null","null",10*((R67-$AS67)/($AT67-$AS67)))</f>
         <v>5.3125</v>
       </c>
       <c r="U67" s="1" t="s">
@@ -24078,6 +24096,420 @@
         <v>272</v>
       </c>
       <c r="BD128" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="129" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>128</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C129" s="6">
+        <v>3</v>
+      </c>
+      <c r="E129" s="1">
+        <v>45</v>
+      </c>
+      <c r="F129" s="1">
+        <f t="shared" si="38"/>
+        <v>-45</v>
+      </c>
+      <c r="G129" s="1">
+        <v>2.16</v>
+      </c>
+      <c r="H129" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="I129" s="1">
+        <v>295</v>
+      </c>
+      <c r="J129" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N129" s="1">
+        <f t="shared" ref="N129:N131" si="63">IF(M129="null","null",(M129-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="O129" s="1">
+        <f t="shared" ref="O129:O131" si="64">IF(M129="null","null",10*((M129-$AS129)/($AT129-$AS129)))</f>
+        <v>-11.785714285714286</v>
+      </c>
+      <c r="S129" s="1">
+        <f t="shared" ref="S129:S131" si="65">IF(R129="null","null",(R129-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="T129" s="1">
+        <f t="shared" si="42"/>
+        <v>-11.785714285714286</v>
+      </c>
+      <c r="X129" s="1">
+        <f t="shared" ref="X129:X131" si="66">IF(W129="null","null",(W129-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="Y129" s="1">
+        <f t="shared" ref="Y129:Y131" si="67">IF(W129="null","null",10*((W129-$AS129)/($AT129-$AS129)))</f>
+        <v>-11.785714285714286</v>
+      </c>
+      <c r="AB129" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC129" s="1" t="str">
+        <f t="shared" ref="AC129:AC131" si="68">IF(AB129="null","null",(AB129-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>null</v>
+      </c>
+      <c r="AD129" s="1" t="str">
+        <f t="shared" ref="AD129:AD131" si="69">IF(AB129="null","null",10*((AB129-$AS129)/($AT129-$AS129)))</f>
+        <v>null</v>
+      </c>
+      <c r="AE129" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF129" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG129" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH129" s="1" t="str">
+        <f t="shared" ref="AH129:AH131" si="70">IF(AG129="null","null",(AG129-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>null</v>
+      </c>
+      <c r="AI129" s="1" t="str">
+        <f t="shared" ref="AI129:AI131" si="71">IF(AG129="null","null",10*((AG129-$AS129)/($AT129-$AS129)))</f>
+        <v>null</v>
+      </c>
+      <c r="AJ129" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK129" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL129" s="1">
+        <f t="shared" ref="AL129:AL131" si="72">MIN(N129,S129,X129,AH129)</f>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="AM129" s="1">
+        <f t="shared" ref="AM129:AM131" si="73">AVERAGE(N129,S129,X129,AH129)</f>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="AN129" s="1">
+        <f t="shared" ref="AN129:AN131" si="74">MAX(N129,S129,X129,AH129)</f>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="AO129" s="1">
+        <f t="shared" ref="AO129:AO131" si="75">AN129-AL129</f>
+        <v>0</v>
+      </c>
+      <c r="AP129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ129" s="1">
+        <v>296.56862745098039</v>
+      </c>
+      <c r="AR129" s="1">
+        <v>36.226098272908693</v>
+      </c>
+      <c r="AS129" s="1">
+        <v>231</v>
+      </c>
+      <c r="AT129" s="1">
+        <v>427</v>
+      </c>
+      <c r="AU129" s="1">
+        <v>270</v>
+      </c>
+      <c r="AV129" s="1">
+        <v>318</v>
+      </c>
+      <c r="AW129" s="1">
+        <v>298</v>
+      </c>
+      <c r="AX129" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY129" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="AZ129" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA129" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="BB129" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="BC129" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="130" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>129</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C130" s="6">
+        <v>3</v>
+      </c>
+      <c r="E130" s="1">
+        <v>50</v>
+      </c>
+      <c r="F130" s="1">
+        <f t="shared" ref="F130:F131" si="76">D130-E130</f>
+        <v>-50</v>
+      </c>
+      <c r="G130" s="1">
+        <v>2.42</v>
+      </c>
+      <c r="H130" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="I130" s="1">
+        <v>639</v>
+      </c>
+      <c r="J130" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N130" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>null</v>
+      </c>
+      <c r="O130" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>null</v>
+      </c>
+      <c r="R130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S130" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>null</v>
+      </c>
+      <c r="T130" s="1" t="str">
+        <f t="shared" si="42"/>
+        <v>null</v>
+      </c>
+      <c r="W130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X130" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>null</v>
+      </c>
+      <c r="Y130" s="1" t="str">
+        <f t="shared" si="67"/>
+        <v>null</v>
+      </c>
+      <c r="AB130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC130" s="1" t="str">
+        <f t="shared" si="68"/>
+        <v>null</v>
+      </c>
+      <c r="AD130" s="1" t="str">
+        <f t="shared" si="69"/>
+        <v>null</v>
+      </c>
+      <c r="AE130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH130" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>null</v>
+      </c>
+      <c r="AI130" s="1" t="str">
+        <f t="shared" si="71"/>
+        <v>null</v>
+      </c>
+      <c r="AJ130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL130" s="1">
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+      <c r="AM130" s="1" t="e">
+        <f t="shared" si="73"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AN130" s="1">
+        <f t="shared" si="74"/>
+        <v>0</v>
+      </c>
+      <c r="AO130" s="1">
+        <f t="shared" si="75"/>
+        <v>0</v>
+      </c>
+      <c r="AP130" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX130" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY130" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ130" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="131" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>130</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C131" s="6">
+        <v>3</v>
+      </c>
+      <c r="E131" s="1">
+        <v>60</v>
+      </c>
+      <c r="F131" s="1">
+        <f t="shared" si="76"/>
+        <v>-60</v>
+      </c>
+      <c r="G131" s="1">
+        <v>2</v>
+      </c>
+      <c r="H131" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="I131" s="1">
+        <v>13006</v>
+      </c>
+      <c r="J131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M131" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N131" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>null</v>
+      </c>
+      <c r="O131" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>null</v>
+      </c>
+      <c r="P131" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q131" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S131" s="1">
+        <f t="shared" si="65"/>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="T131" s="1" t="e">
+        <f t="shared" ref="T131" si="77">IF(R131="null","null",10*((R131-$AS131)/($AT131-$AS131)))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W131" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X131" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>null</v>
+      </c>
+      <c r="Y131" s="1" t="str">
+        <f t="shared" si="67"/>
+        <v>null</v>
+      </c>
+      <c r="Z131" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA131" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC131" s="1">
+        <f t="shared" si="68"/>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="AD131" s="1" t="e">
+        <f t="shared" si="69"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG131" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH131" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>null</v>
+      </c>
+      <c r="AI131" s="1" t="str">
+        <f t="shared" si="71"/>
+        <v>null</v>
+      </c>
+      <c r="AJ131" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK131" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL131" s="1">
+        <f t="shared" si="72"/>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="AM131" s="1">
+        <f t="shared" si="73"/>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="AN131" s="1">
+        <f t="shared" si="74"/>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="AO131" s="1">
+        <f t="shared" si="75"/>
+        <v>0</v>
+      </c>
+      <c r="AP131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AX131" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AY131" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -24088,12 +24520,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCBA7DA-4A7C-4BD5-95F2-6CD93F57778E}">
-  <dimension ref="A1:BG96"/>
+  <dimension ref="A1:BG107"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AX1" activePane="topRight" state="frozen"/>
       <selection activeCell="A58" sqref="A58"/>
-      <selection pane="topRight" activeCell="B95" sqref="B95:H96"/>
+      <selection pane="topRight" activeCell="BH98" sqref="BH98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41581,6 +42013,648 @@
         <v>80</v>
       </c>
     </row>
+    <row r="97" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B97">
+        <f t="shared" ref="B97:B98" si="21">AVERAGE(I97:BG97)</f>
+        <v>296.56862745098039</v>
+      </c>
+      <c r="C97">
+        <f t="shared" ref="C97:C98" si="22">_xlfn.STDEV.S(I97:BG97)</f>
+        <v>36.226098272908693</v>
+      </c>
+      <c r="D97">
+        <f t="shared" ref="D97:D98" si="23">MIN(I97:BG97)</f>
+        <v>231</v>
+      </c>
+      <c r="E97">
+        <f t="shared" ref="E97:E98" si="24">MAX(J97:BG97)</f>
+        <v>427</v>
+      </c>
+      <c r="F97">
+        <f t="shared" ref="F97:F98" si="25">_xlfn.QUARTILE.EXC(I97:BG97,1)</f>
+        <v>270</v>
+      </c>
+      <c r="G97">
+        <f t="shared" ref="G97:G98" si="26">_xlfn.QUARTILE.EXC(I97:BG97,3)</f>
+        <v>318</v>
+      </c>
+      <c r="H97">
+        <f t="shared" ref="H97:H98" si="27">MEDIAN(I97:BG97)</f>
+        <v>298</v>
+      </c>
+      <c r="I97">
+        <v>332</v>
+      </c>
+      <c r="J97">
+        <v>294</v>
+      </c>
+      <c r="K97">
+        <v>278</v>
+      </c>
+      <c r="L97">
+        <v>246</v>
+      </c>
+      <c r="M97">
+        <v>286</v>
+      </c>
+      <c r="N97">
+        <v>271</v>
+      </c>
+      <c r="O97">
+        <v>270</v>
+      </c>
+      <c r="P97">
+        <v>254</v>
+      </c>
+      <c r="Q97">
+        <v>231</v>
+      </c>
+      <c r="R97">
+        <v>310</v>
+      </c>
+      <c r="S97">
+        <v>264</v>
+      </c>
+      <c r="T97">
+        <v>294</v>
+      </c>
+      <c r="U97">
+        <v>277</v>
+      </c>
+      <c r="V97">
+        <v>268</v>
+      </c>
+      <c r="W97">
+        <v>316</v>
+      </c>
+      <c r="X97">
+        <v>310</v>
+      </c>
+      <c r="Y97">
+        <v>317</v>
+      </c>
+      <c r="Z97">
+        <v>325</v>
+      </c>
+      <c r="AA97">
+        <v>318</v>
+      </c>
+      <c r="AB97">
+        <v>312</v>
+      </c>
+      <c r="AC97">
+        <v>299</v>
+      </c>
+      <c r="AD97">
+        <v>325</v>
+      </c>
+      <c r="AE97">
+        <v>350</v>
+      </c>
+      <c r="AF97">
+        <v>314</v>
+      </c>
+      <c r="AG97">
+        <v>321</v>
+      </c>
+      <c r="AH97">
+        <v>305</v>
+      </c>
+      <c r="AI97">
+        <v>313</v>
+      </c>
+      <c r="AJ97">
+        <v>289</v>
+      </c>
+      <c r="AK97">
+        <v>336</v>
+      </c>
+      <c r="AL97">
+        <v>351</v>
+      </c>
+      <c r="AM97">
+        <v>287</v>
+      </c>
+      <c r="AN97">
+        <v>356</v>
+      </c>
+      <c r="AO97">
+        <v>427</v>
+      </c>
+      <c r="AP97">
+        <v>247</v>
+      </c>
+      <c r="AQ97">
+        <v>296</v>
+      </c>
+      <c r="AR97">
+        <v>327</v>
+      </c>
+      <c r="AS97">
+        <v>302</v>
+      </c>
+      <c r="AT97">
+        <v>274</v>
+      </c>
+      <c r="AU97">
+        <v>260</v>
+      </c>
+      <c r="AV97">
+        <v>247</v>
+      </c>
+      <c r="AW97">
+        <v>252</v>
+      </c>
+      <c r="AX97">
+        <v>286</v>
+      </c>
+      <c r="AY97">
+        <v>316</v>
+      </c>
+      <c r="AZ97">
+        <v>300</v>
+      </c>
+      <c r="BA97">
+        <v>231</v>
+      </c>
+      <c r="BB97">
+        <v>321</v>
+      </c>
+      <c r="BC97">
+        <v>298</v>
+      </c>
+      <c r="BD97">
+        <v>254</v>
+      </c>
+      <c r="BE97">
+        <v>287</v>
+      </c>
+      <c r="BF97">
+        <v>320</v>
+      </c>
+      <c r="BG97">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="98" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="21"/>
+        <v>57.921568627450981</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="22"/>
+        <v>12.440005043817136</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="23"/>
+        <v>25</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="24"/>
+        <v>85</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="25"/>
+        <v>50</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="26"/>
+        <v>66</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="27"/>
+        <v>59</v>
+      </c>
+      <c r="I98">
+        <v>63</v>
+      </c>
+      <c r="J98">
+        <v>62</v>
+      </c>
+      <c r="K98">
+        <v>49</v>
+      </c>
+      <c r="L98">
+        <v>59</v>
+      </c>
+      <c r="M98">
+        <v>59</v>
+      </c>
+      <c r="N98">
+        <v>66</v>
+      </c>
+      <c r="O98">
+        <v>65</v>
+      </c>
+      <c r="P98">
+        <v>62</v>
+      </c>
+      <c r="Q98">
+        <v>61</v>
+      </c>
+      <c r="R98">
+        <v>50</v>
+      </c>
+      <c r="S98">
+        <v>47</v>
+      </c>
+      <c r="T98">
+        <v>40</v>
+      </c>
+      <c r="U98">
+        <v>70</v>
+      </c>
+      <c r="V98">
+        <v>61</v>
+      </c>
+      <c r="W98">
+        <v>50</v>
+      </c>
+      <c r="X98">
+        <v>71</v>
+      </c>
+      <c r="Y98">
+        <v>56</v>
+      </c>
+      <c r="Z98">
+        <v>72</v>
+      </c>
+      <c r="AA98">
+        <v>57</v>
+      </c>
+      <c r="AB98">
+        <v>51</v>
+      </c>
+      <c r="AC98">
+        <v>25</v>
+      </c>
+      <c r="AD98">
+        <v>85</v>
+      </c>
+      <c r="AE98">
+        <v>34</v>
+      </c>
+      <c r="AF98">
+        <v>31</v>
+      </c>
+      <c r="AG98">
+        <v>50</v>
+      </c>
+      <c r="AH98">
+        <v>32</v>
+      </c>
+      <c r="AI98">
+        <v>53</v>
+      </c>
+      <c r="AJ98">
+        <v>59</v>
+      </c>
+      <c r="AK98">
+        <v>61</v>
+      </c>
+      <c r="AL98">
+        <v>47</v>
+      </c>
+      <c r="AM98">
+        <v>59</v>
+      </c>
+      <c r="AN98">
+        <v>72</v>
+      </c>
+      <c r="AO98">
+        <v>69</v>
+      </c>
+      <c r="AP98">
+        <v>62</v>
+      </c>
+      <c r="AQ98">
+        <v>58</v>
+      </c>
+      <c r="AR98">
+        <v>76</v>
+      </c>
+      <c r="AS98">
+        <v>70</v>
+      </c>
+      <c r="AT98">
+        <v>69</v>
+      </c>
+      <c r="AU98">
+        <v>71</v>
+      </c>
+      <c r="AV98">
+        <v>45</v>
+      </c>
+      <c r="AW98">
+        <v>60</v>
+      </c>
+      <c r="AX98">
+        <v>49</v>
+      </c>
+      <c r="AY98">
+        <v>70</v>
+      </c>
+      <c r="AZ98">
+        <v>57</v>
+      </c>
+      <c r="BA98">
+        <v>84</v>
+      </c>
+      <c r="BB98">
+        <v>57</v>
+      </c>
+      <c r="BC98">
+        <v>49</v>
+      </c>
+      <c r="BD98">
+        <v>63</v>
+      </c>
+      <c r="BE98">
+        <v>57</v>
+      </c>
+      <c r="BF98">
+        <v>52</v>
+      </c>
+      <c r="BG98">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="99" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B99" t="e">
+        <f t="shared" ref="B99:B107" si="28">AVERAGE(I99:BG99)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C99" t="e">
+        <f t="shared" ref="C99:C107" si="29">_xlfn.STDEV.S(I99:BG99)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D99">
+        <f t="shared" ref="D99:D107" si="30">MIN(I99:BG99)</f>
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <f t="shared" ref="E99:E107" si="31">MAX(J99:BG99)</f>
+        <v>0</v>
+      </c>
+      <c r="F99" t="e">
+        <f t="shared" ref="F99:F107" si="32">_xlfn.QUARTILE.EXC(I99:BG99,1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G99" t="e">
+        <f t="shared" ref="G99:G107" si="33">_xlfn.QUARTILE.EXC(I99:BG99,3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="H99" t="e">
+        <f t="shared" ref="H99:H107" si="34">MEDIAN(I99:BG99)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="100" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B100" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C100" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="F100" t="e">
+        <f t="shared" si="32"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G100" t="e">
+        <f t="shared" si="33"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H100" t="e">
+        <f t="shared" si="34"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="101" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B101" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C101" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="F101" t="e">
+        <f t="shared" si="32"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G101" t="e">
+        <f t="shared" si="33"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H101" t="e">
+        <f t="shared" si="34"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="102" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B102" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C102" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="F102" t="e">
+        <f t="shared" si="32"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G102" t="e">
+        <f t="shared" si="33"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H102" t="e">
+        <f t="shared" si="34"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="103" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B103" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C103" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="F103" t="e">
+        <f t="shared" si="32"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G103" t="e">
+        <f t="shared" si="33"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H103" t="e">
+        <f t="shared" si="34"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="104" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B104" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C104" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="F104" t="e">
+        <f t="shared" si="32"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G104" t="e">
+        <f t="shared" si="33"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H104" t="e">
+        <f t="shared" si="34"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="105" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B105" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C105" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="F105" t="e">
+        <f t="shared" si="32"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G105" t="e">
+        <f t="shared" si="33"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H105" t="e">
+        <f t="shared" si="34"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="106" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B106" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C106" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="F106" t="e">
+        <f t="shared" si="32"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G106" t="e">
+        <f t="shared" si="33"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H106" t="e">
+        <f t="shared" si="34"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="107" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B107" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C107" t="e">
+        <f t="shared" si="29"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="F107" t="e">
+        <f t="shared" si="32"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G107" t="e">
+        <f t="shared" si="33"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H107" t="e">
+        <f t="shared" si="34"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated FirstTurn database, finished functions to do NHL requests, started the bs4 work to clean the play by play data
</commit_message>
<xml_diff>
--- a/projects/firstTurnData/FirstTurnCombined.xlsx
+++ b/projects/firstTurnData/FirstTurnCombined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PNJae\Dropbox\website\PNJaenichen.github.io\projects\firstTurnData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E02BFD-4E3A-4D20-A751-BB4045651333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB8BA22-F107-4818-8FE9-2E88F7D70F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="0" windowWidth="28830" windowHeight="15600" activeTab="1" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3426" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3434" uniqueCount="346">
   <si>
     <t>Yes</t>
   </si>
@@ -1445,9 +1445,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796E82C3-294D-4E4E-8DE4-13BF7BF427EB}">
   <dimension ref="A1:BO131"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M131" sqref="M131"/>
+      <selection pane="bottomLeft" activeCell="O129" sqref="O129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24109,12 +24109,15 @@
       <c r="C129" s="6">
         <v>3</v>
       </c>
+      <c r="D129" s="1">
+        <v>50</v>
+      </c>
       <c r="E129" s="1">
         <v>45</v>
       </c>
       <c r="F129" s="1">
         <f t="shared" si="38"/>
-        <v>-45</v>
+        <v>5</v>
       </c>
       <c r="G129" s="1">
         <v>2.16</v>
@@ -24128,29 +24131,62 @@
       <c r="J129" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="K129" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M129" s="1">
+        <v>237</v>
+      </c>
       <c r="N129" s="1">
         <f t="shared" ref="N129:N131" si="63">IF(M129="null","null",(M129-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
-        <v>-0.95237470689757397</v>
+        <v>3.4680085378004311</v>
       </c>
       <c r="O129" s="1">
         <f t="shared" ref="O129:O131" si="64">IF(M129="null","null",10*((M129-$AS129)/($AT129-$AS129)))</f>
-        <v>-11.785714285714286</v>
+        <v>0.30612244897959184</v>
+      </c>
+      <c r="P129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R129" s="1">
+        <v>221</v>
       </c>
       <c r="S129" s="1">
         <f t="shared" ref="S129:S131" si="65">IF(R129="null","null",(R129-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
-        <v>-0.95237470689757397</v>
+        <v>3.1695860402680762</v>
       </c>
       <c r="T129" s="1">
         <f t="shared" si="42"/>
-        <v>-11.785714285714286</v>
+        <v>-0.51020408163265307</v>
+      </c>
+      <c r="U129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V129" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W129" s="1">
+        <v>280</v>
       </c>
       <c r="X129" s="1">
         <f t="shared" ref="X129:X131" si="66">IF(W129="null","null",(W129-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
-        <v>-0.95237470689757397</v>
+        <v>4.2700189999186344</v>
       </c>
       <c r="Y129" s="1">
         <f t="shared" ref="Y129:Y131" si="67">IF(W129="null","null",10*((W129-$AS129)/($AT129-$AS129)))</f>
-        <v>-11.785714285714286</v>
+        <v>2.5</v>
+      </c>
+      <c r="Z129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA129" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="AB129" s="1" t="s">
         <v>36</v>
@@ -24188,19 +24224,19 @@
       </c>
       <c r="AL129" s="1">
         <f t="shared" ref="AL129:AL131" si="72">MIN(N129,S129,X129,AH129)</f>
-        <v>-0.95237470689757397</v>
+        <v>3.1695860402680762</v>
       </c>
       <c r="AM129" s="1">
         <f t="shared" ref="AM129:AM131" si="73">AVERAGE(N129,S129,X129,AH129)</f>
-        <v>-0.95237470689757397</v>
+        <v>3.6358711926623806</v>
       </c>
       <c r="AN129" s="1">
         <f t="shared" ref="AN129:AN131" si="74">MAX(N129,S129,X129,AH129)</f>
-        <v>-0.95237470689757397</v>
+        <v>4.2700189999186344</v>
       </c>
       <c r="AO129" s="1">
         <f t="shared" ref="AO129:AO131" si="75">AN129-AL129</f>
-        <v>0</v>
+        <v>1.1004329596505582</v>
       </c>
       <c r="AP129" s="1" t="s">
         <v>38</v>
@@ -24522,7 +24558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCBA7DA-4A7C-4BD5-95F2-6CD93F57778E}">
   <dimension ref="A1:BG107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+    <sheetView topLeftCell="A66" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AX1" activePane="topRight" state="frozen"/>
       <selection activeCell="A58" sqref="A58"/>
       <selection pane="topRight" activeCell="BH98" sqref="BH98"/>

</xml_diff>

<commit_message>
Updated FirstTurnCast csv file with recent played game
</commit_message>
<xml_diff>
--- a/projects/firstTurnData/FirstTurnCombined.xlsx
+++ b/projects/firstTurnData/FirstTurnCombined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PNJae\Dropbox\website\PNJaenichen.github.io\projects\firstTurnData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB8BA22-F107-4818-8FE9-2E88F7D70F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EE74BB-B62D-451A-8D01-E0AB28CE2B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3434" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3446" uniqueCount="346">
   <si>
     <t>Yes</t>
   </si>
@@ -1445,9 +1445,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796E82C3-294D-4E4E-8DE4-13BF7BF427EB}">
   <dimension ref="A1:BO131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O129" sqref="O129"/>
+      <selection pane="bottomLeft" activeCell="AO134" sqref="AO134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24291,12 +24291,15 @@
       <c r="C130" s="6">
         <v>3</v>
       </c>
+      <c r="D130" s="1">
+        <v>60</v>
+      </c>
       <c r="E130" s="1">
         <v>50</v>
       </c>
       <c r="F130" s="1">
         <f t="shared" ref="F130:F131" si="76">D130-E130</f>
-        <v>-50</v>
+        <v>10</v>
       </c>
       <c r="G130" s="1">
         <v>2.42</v>
@@ -24310,6 +24313,12 @@
       <c r="J130" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="K130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L130" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="M130" s="1" t="s">
         <v>36</v>
       </c>
@@ -24321,6 +24330,12 @@
         <f t="shared" si="64"/>
         <v>null</v>
       </c>
+      <c r="P130" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q130" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="R130" s="1" t="s">
         <v>36</v>
       </c>
@@ -24332,6 +24347,12 @@
         <f t="shared" si="42"/>
         <v>null</v>
       </c>
+      <c r="U130" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V130" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="W130" s="1" t="s">
         <v>36</v>
       </c>
@@ -24343,6 +24364,12 @@
         <f t="shared" si="67"/>
         <v>null</v>
       </c>
+      <c r="Z130" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA130" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="AB130" s="1" t="s">
         <v>36</v>
       </c>
@@ -24377,21 +24404,17 @@
       <c r="AK130" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL130" s="1">
-        <f t="shared" si="72"/>
-        <v>0</v>
-      </c>
-      <c r="AM130" s="1" t="e">
-        <f t="shared" si="73"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AN130" s="1">
-        <f t="shared" si="74"/>
-        <v>0</v>
-      </c>
-      <c r="AO130" s="1">
-        <f t="shared" si="75"/>
-        <v>0</v>
+      <c r="AL130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO130" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="AP130" s="1" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
updated first turn dataset
</commit_message>
<xml_diff>
--- a/projects/firstTurnData/FirstTurnCombined.xlsx
+++ b/projects/firstTurnData/FirstTurnCombined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PNJae\Dropbox\website\PNJaenichen.github.io\projects\firstTurnData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EE74BB-B62D-451A-8D01-E0AB28CE2B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E79195-CD87-4082-A14E-B23A50271C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3446" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3490" uniqueCount="352">
   <si>
     <t>Yes</t>
   </si>
@@ -1077,6 +1077,24 @@
   <si>
     <t>Victory Points as a Resource</t>
   </si>
+  <si>
+    <t>Pipeline</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Turn Order: Claim Action</t>
+  </si>
+  <si>
+    <t>Citadels</t>
+  </si>
+  <si>
+    <t>Lose A Turn</t>
+  </si>
+  <si>
+    <t>Turn Order: Role Order</t>
+  </si>
 </sst>
 </file>
 
@@ -1443,11 +1461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796E82C3-294D-4E4E-8DE4-13BF7BF427EB}">
-  <dimension ref="A1:BO131"/>
+  <dimension ref="A1:BO133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AO134" sqref="AO134"/>
+      <selection pane="bottomLeft" activeCell="AO136" sqref="AO136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24099,7 +24117,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="129" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -24209,11 +24227,11 @@
         <v>36</v>
       </c>
       <c r="AH129" s="1" t="str">
-        <f t="shared" ref="AH129:AH131" si="70">IF(AG129="null","null",(AG129-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <f t="shared" ref="AH129:AH132" si="70">IF(AG129="null","null",(AG129-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
         <v>null</v>
       </c>
       <c r="AI129" s="1" t="str">
-        <f t="shared" ref="AI129:AI131" si="71">IF(AG129="null","null",10*((AG129-$AS129)/($AT129-$AS129)))</f>
+        <f t="shared" ref="AI129:AI132" si="71">IF(AG129="null","null",10*((AG129-$AS129)/($AT129-$AS129)))</f>
         <v>null</v>
       </c>
       <c r="AJ129" s="1" t="s">
@@ -24223,19 +24241,19 @@
         <v>36</v>
       </c>
       <c r="AL129" s="1">
-        <f t="shared" ref="AL129:AL131" si="72">MIN(N129,S129,X129,AH129)</f>
+        <f t="shared" ref="AL129:AL132" si="72">MIN(N129,S129,X129,AH129)</f>
         <v>3.1695860402680762</v>
       </c>
       <c r="AM129" s="1">
-        <f t="shared" ref="AM129:AM131" si="73">AVERAGE(N129,S129,X129,AH129)</f>
+        <f t="shared" ref="AM129:AM132" si="73">AVERAGE(N129,S129,X129,AH129)</f>
         <v>3.6358711926623806</v>
       </c>
       <c r="AN129" s="1">
-        <f t="shared" ref="AN129:AN131" si="74">MAX(N129,S129,X129,AH129)</f>
+        <f t="shared" ref="AN129:AN132" si="74">MAX(N129,S129,X129,AH129)</f>
         <v>4.2700189999186344</v>
       </c>
       <c r="AO129" s="1">
-        <f t="shared" ref="AO129:AO131" si="75">AN129-AL129</f>
+        <f t="shared" ref="AO129:AO132" si="75">AN129-AL129</f>
         <v>1.1004329596505582</v>
       </c>
       <c r="AP129" s="1" t="s">
@@ -24281,7 +24299,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="130" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -24298,7 +24316,7 @@
         <v>50</v>
       </c>
       <c r="F130" s="1">
-        <f t="shared" ref="F130:F131" si="76">D130-E130</f>
+        <f t="shared" ref="F130:F133" si="76">D130-E130</f>
         <v>10</v>
       </c>
       <c r="G130" s="1">
@@ -24450,7 +24468,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="131" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -24570,6 +24588,340 @@
       </c>
       <c r="AY131" s="1" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="132" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>131</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="D132" s="1">
+        <v>90</v>
+      </c>
+      <c r="E132" s="1">
+        <v>90</v>
+      </c>
+      <c r="F132" s="1">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="G132" s="1">
+        <v>3.87</v>
+      </c>
+      <c r="H132" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="I132" s="1">
+        <v>421</v>
+      </c>
+      <c r="J132" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K132" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M132" s="1">
+        <v>193</v>
+      </c>
+      <c r="N132" s="1">
+        <f t="shared" ref="N132" si="78">IF(M132="null","null",(M132-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>2.6473466695864554</v>
+      </c>
+      <c r="O132" s="1">
+        <f t="shared" ref="O132" si="79">IF(M132="null","null",10*((M132-$AS132)/($AT132-$AS132)))</f>
+        <v>-0.26209677419354838</v>
+      </c>
+      <c r="P132" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q132" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R132" s="1">
+        <v>70</v>
+      </c>
+      <c r="S132" s="1">
+        <f t="shared" ref="S132" si="80">IF(R132="null","null",(R132-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>0.3532237198064781</v>
+      </c>
+      <c r="T132" s="1">
+        <f t="shared" ref="T132" si="81">IF(R132="null","null",10*((R132-$AS132)/($AT132-$AS132)))</f>
+        <v>-1.502016129032258</v>
+      </c>
+      <c r="U132" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V132" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W132" s="1">
+        <v>199</v>
+      </c>
+      <c r="X132" s="1">
+        <f t="shared" ref="X132" si="82">IF(W132="null","null",(W132-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>2.7592551061610884</v>
+      </c>
+      <c r="Y132" s="1">
+        <f t="shared" ref="Y132" si="83">IF(W132="null","null",10*((W132-$AS132)/($AT132-$AS132)))</f>
+        <v>-0.20161290322580644</v>
+      </c>
+      <c r="Z132" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA132" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB132" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC132" s="1" t="str">
+        <f t="shared" ref="AC132" si="84">IF(AB132="null","null",(AB132-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>null</v>
+      </c>
+      <c r="AD132" s="1" t="str">
+        <f t="shared" ref="AD132" si="85">IF(AB132="null","null",10*((AB132-$AS132)/($AT132-$AS132)))</f>
+        <v>null</v>
+      </c>
+      <c r="AE132" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF132" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG132" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH132" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>null</v>
+      </c>
+      <c r="AI132" s="1" t="str">
+        <f t="shared" si="71"/>
+        <v>null</v>
+      </c>
+      <c r="AJ132" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK132" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL132" s="1">
+        <f t="shared" si="72"/>
+        <v>0.3532237198064781</v>
+      </c>
+      <c r="AM132" s="1">
+        <f t="shared" si="73"/>
+        <v>1.9199418318513406</v>
+      </c>
+      <c r="AN132" s="1">
+        <f t="shared" si="74"/>
+        <v>2.7592551061610884</v>
+      </c>
+      <c r="AO132" s="1">
+        <f t="shared" si="75"/>
+        <v>2.4060313863546101</v>
+      </c>
+      <c r="AP132" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ132" s="1">
+        <v>598.39215686274508</v>
+      </c>
+      <c r="AR132" s="1">
+        <v>267.4393447816812</v>
+      </c>
+      <c r="AS132" s="1">
+        <v>219</v>
+      </c>
+      <c r="AT132" s="1">
+        <v>1211</v>
+      </c>
+      <c r="AU132" s="1">
+        <v>365</v>
+      </c>
+      <c r="AV132" s="1">
+        <v>841</v>
+      </c>
+      <c r="AW132" s="1">
+        <v>591</v>
+      </c>
+      <c r="AX132" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY132" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AZ132" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA132" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BB132" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="BC132" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="BD132" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE132" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="133" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>132</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="E133" s="1">
+        <v>40</v>
+      </c>
+      <c r="F133" s="1">
+        <f t="shared" si="76"/>
+        <v>-40</v>
+      </c>
+      <c r="G133" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="H133" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="I133" s="1">
+        <v>424</v>
+      </c>
+      <c r="N133" s="1">
+        <f t="shared" ref="N133" si="86">IF(M133="null","null",(M133-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="O133" s="1">
+        <f t="shared" ref="O133" si="87">IF(M133="null","null",10*((M133-$AS133)/($AT133-$AS133)))</f>
+        <v>-2.0588235294117645</v>
+      </c>
+      <c r="S133" s="1">
+        <f t="shared" ref="S133" si="88">IF(R133="null","null",(R133-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="T133" s="1">
+        <f t="shared" ref="T133" si="89">IF(R133="null","null",10*((R133-$AS133)/($AT133-$AS133)))</f>
+        <v>-2.0588235294117645</v>
+      </c>
+      <c r="X133" s="1">
+        <f t="shared" ref="X133" si="90">IF(W133="null","null",(W133-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="Y133" s="1">
+        <f t="shared" ref="Y133" si="91">IF(W133="null","null",10*((W133-$AS133)/($AT133-$AS133)))</f>
+        <v>-2.0588235294117645</v>
+      </c>
+      <c r="AB133" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC133" s="1" t="str">
+        <f t="shared" ref="AC133" si="92">IF(AB133="null","null",(AB133-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>null</v>
+      </c>
+      <c r="AD133" s="1" t="str">
+        <f t="shared" ref="AD133" si="93">IF(AB133="null","null",10*((AB133-$AS133)/($AT133-$AS133)))</f>
+        <v>null</v>
+      </c>
+      <c r="AE133" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF133" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG133" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH133" s="1" t="str">
+        <f t="shared" ref="AH133" si="94">IF(AG133="null","null",(AG133-AVERAGE($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))/_xlfn.STDEV.P($M$2:$M$128,$R$2:$R$128,$AG$2:$AG$128,$W$2:$W$128,$AB$2:$AB$128))</f>
+        <v>null</v>
+      </c>
+      <c r="AI133" s="1" t="str">
+        <f t="shared" ref="AI133" si="95">IF(AG133="null","null",10*((AG133-$AS133)/($AT133-$AS133)))</f>
+        <v>null</v>
+      </c>
+      <c r="AJ133" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK133" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL133" s="1">
+        <f t="shared" ref="AL133" si="96">MIN(N133,S133,X133,AH133)</f>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="AM133" s="1">
+        <f t="shared" ref="AM133" si="97">AVERAGE(N133,S133,X133,AH133)</f>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="AN133" s="1">
+        <f t="shared" ref="AN133" si="98">MAX(N133,S133,X133,AH133)</f>
+        <v>-0.95237470689757397</v>
+      </c>
+      <c r="AO133" s="1">
+        <f t="shared" ref="AO133" si="99">AN133-AL133</f>
+        <v>0</v>
+      </c>
+      <c r="AP133" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ133" s="1">
+        <v>22.666666666666668</v>
+      </c>
+      <c r="AR133" s="1">
+        <v>8.086202240030028</v>
+      </c>
+      <c r="AS133" s="1">
+        <v>7</v>
+      </c>
+      <c r="AT133" s="1">
+        <v>41</v>
+      </c>
+      <c r="AU133" s="1">
+        <v>17</v>
+      </c>
+      <c r="AV133" s="1">
+        <v>30</v>
+      </c>
+      <c r="AW133" s="1">
+        <v>21</v>
+      </c>
+      <c r="AX133" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY133" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ133" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA133" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="BB133" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BC133" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="BD133" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -24581,10 +24933,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCBA7DA-4A7C-4BD5-95F2-6CD93F57778E}">
   <dimension ref="A1:BG107"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AX1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A58" sqref="A58"/>
-      <selection pane="topRight" activeCell="BH98" sqref="BH98"/>
+      <selection pane="topRight" activeCell="B100" sqref="B100:H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42445,63 +42797,375 @@
       </c>
     </row>
     <row r="99" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B99" t="e">
+      <c r="A99" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B99">
         <f t="shared" ref="B99:B107" si="28">AVERAGE(I99:BG99)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C99" t="e">
+        <v>598.39215686274508</v>
+      </c>
+      <c r="C99">
         <f t="shared" ref="C99:C107" si="29">_xlfn.STDEV.S(I99:BG99)</f>
-        <v>#DIV/0!</v>
+        <v>267.4393447816812</v>
       </c>
       <c r="D99">
         <f t="shared" ref="D99:D107" si="30">MIN(I99:BG99)</f>
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="E99">
         <f t="shared" ref="E99:E107" si="31">MAX(J99:BG99)</f>
-        <v>0</v>
-      </c>
-      <c r="F99" t="e">
+        <v>1211</v>
+      </c>
+      <c r="F99">
         <f t="shared" ref="F99:F107" si="32">_xlfn.QUARTILE.EXC(I99:BG99,1)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G99" t="e">
+        <v>365</v>
+      </c>
+      <c r="G99">
         <f t="shared" ref="G99:G107" si="33">_xlfn.QUARTILE.EXC(I99:BG99,3)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H99" t="e">
+        <v>841</v>
+      </c>
+      <c r="H99">
         <f t="shared" ref="H99:H107" si="34">MEDIAN(I99:BG99)</f>
-        <v>#NUM!</v>
+        <v>591</v>
+      </c>
+      <c r="I99">
+        <v>464</v>
+      </c>
+      <c r="J99">
+        <v>1168</v>
+      </c>
+      <c r="K99">
+        <v>395</v>
+      </c>
+      <c r="L99">
+        <v>400</v>
+      </c>
+      <c r="M99">
+        <v>332</v>
+      </c>
+      <c r="N99">
+        <v>225</v>
+      </c>
+      <c r="O99">
+        <v>841</v>
+      </c>
+      <c r="P99">
+        <v>581</v>
+      </c>
+      <c r="Q99">
+        <v>647</v>
+      </c>
+      <c r="R99">
+        <v>301</v>
+      </c>
+      <c r="S99">
+        <v>955</v>
+      </c>
+      <c r="T99">
+        <v>490</v>
+      </c>
+      <c r="U99">
+        <v>729</v>
+      </c>
+      <c r="V99">
+        <v>274</v>
+      </c>
+      <c r="W99">
+        <v>417</v>
+      </c>
+      <c r="X99">
+        <v>219</v>
+      </c>
+      <c r="Y99">
+        <v>379</v>
+      </c>
+      <c r="Z99">
+        <v>254</v>
+      </c>
+      <c r="AA99">
+        <v>357</v>
+      </c>
+      <c r="AB99">
+        <v>591</v>
+      </c>
+      <c r="AC99">
+        <v>908</v>
+      </c>
+      <c r="AD99">
+        <v>761</v>
+      </c>
+      <c r="AE99">
+        <v>702</v>
+      </c>
+      <c r="AF99">
+        <v>939</v>
+      </c>
+      <c r="AG99">
+        <v>687</v>
+      </c>
+      <c r="AH99">
+        <v>841</v>
+      </c>
+      <c r="AI99">
+        <v>581</v>
+      </c>
+      <c r="AJ99">
+        <v>490</v>
+      </c>
+      <c r="AK99">
+        <v>955</v>
+      </c>
+      <c r="AL99">
+        <v>301</v>
+      </c>
+      <c r="AM99">
+        <v>274</v>
+      </c>
+      <c r="AN99">
+        <v>417</v>
+      </c>
+      <c r="AO99">
+        <v>729</v>
+      </c>
+      <c r="AP99">
+        <v>254</v>
+      </c>
+      <c r="AQ99">
+        <v>379</v>
+      </c>
+      <c r="AR99">
+        <v>219</v>
+      </c>
+      <c r="AS99">
+        <v>861</v>
+      </c>
+      <c r="AT99">
+        <v>876</v>
+      </c>
+      <c r="AU99">
+        <v>970</v>
+      </c>
+      <c r="AV99">
+        <v>591</v>
+      </c>
+      <c r="AW99">
+        <v>357</v>
+      </c>
+      <c r="AX99">
+        <v>908</v>
+      </c>
+      <c r="AY99">
+        <v>939</v>
+      </c>
+      <c r="AZ99">
+        <v>702</v>
+      </c>
+      <c r="BA99">
+        <v>761</v>
+      </c>
+      <c r="BB99">
+        <v>611</v>
+      </c>
+      <c r="BC99">
+        <v>795</v>
+      </c>
+      <c r="BD99">
+        <v>726</v>
+      </c>
+      <c r="BE99">
+        <v>1211</v>
+      </c>
+      <c r="BF99">
+        <v>389</v>
+      </c>
+      <c r="BG99">
+        <v>365</v>
       </c>
     </row>
     <row r="100" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B100" t="e">
+      <c r="A100" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B100">
         <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C100" t="e">
+        <v>22.666666666666668</v>
+      </c>
+      <c r="C100">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>8.086202240030028</v>
       </c>
       <c r="D100">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E100">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="F100" t="e">
+        <v>41</v>
+      </c>
+      <c r="F100">
         <f t="shared" si="32"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="G100" t="e">
+        <v>17</v>
+      </c>
+      <c r="G100">
         <f t="shared" si="33"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H100" t="e">
+        <v>30</v>
+      </c>
+      <c r="H100">
         <f t="shared" si="34"/>
-        <v>#NUM!</v>
+        <v>21</v>
+      </c>
+      <c r="I100">
+        <v>33</v>
+      </c>
+      <c r="J100">
+        <v>33</v>
+      </c>
+      <c r="K100">
+        <v>18</v>
+      </c>
+      <c r="L100">
+        <v>34</v>
+      </c>
+      <c r="M100">
+        <v>33</v>
+      </c>
+      <c r="N100">
+        <v>20</v>
+      </c>
+      <c r="O100">
+        <v>18</v>
+      </c>
+      <c r="P100">
+        <v>25</v>
+      </c>
+      <c r="Q100">
+        <v>21</v>
+      </c>
+      <c r="R100">
+        <v>16</v>
+      </c>
+      <c r="S100">
+        <v>10</v>
+      </c>
+      <c r="T100">
+        <v>34</v>
+      </c>
+      <c r="U100">
+        <v>25</v>
+      </c>
+      <c r="V100">
+        <v>23</v>
+      </c>
+      <c r="W100">
+        <v>21</v>
+      </c>
+      <c r="X100">
+        <v>33</v>
+      </c>
+      <c r="Y100">
+        <v>17</v>
+      </c>
+      <c r="Z100">
+        <v>16</v>
+      </c>
+      <c r="AA100">
+        <v>10</v>
+      </c>
+      <c r="AB100">
+        <v>32</v>
+      </c>
+      <c r="AC100">
+        <v>31</v>
+      </c>
+      <c r="AD100">
+        <v>28</v>
+      </c>
+      <c r="AE100">
+        <v>17</v>
+      </c>
+      <c r="AF100">
+        <v>41</v>
+      </c>
+      <c r="AG100">
+        <v>27</v>
+      </c>
+      <c r="AH100">
+        <v>20</v>
+      </c>
+      <c r="AI100">
+        <v>18</v>
+      </c>
+      <c r="AJ100">
+        <v>28</v>
+      </c>
+      <c r="AK100">
+        <v>25</v>
+      </c>
+      <c r="AL100">
+        <v>21</v>
+      </c>
+      <c r="AM100">
+        <v>17</v>
+      </c>
+      <c r="AN100">
+        <v>20</v>
+      </c>
+      <c r="AO100">
+        <v>10</v>
+      </c>
+      <c r="AP100">
+        <v>9</v>
+      </c>
+      <c r="AQ100">
+        <v>7</v>
+      </c>
+      <c r="AR100">
+        <v>34</v>
+      </c>
+      <c r="AS100">
+        <v>31</v>
+      </c>
+      <c r="AT100">
+        <v>27</v>
+      </c>
+      <c r="AU100">
+        <v>21</v>
+      </c>
+      <c r="AV100">
+        <v>28</v>
+      </c>
+      <c r="AW100">
+        <v>22</v>
+      </c>
+      <c r="AX100">
+        <v>21</v>
+      </c>
+      <c r="AY100">
+        <v>12</v>
+      </c>
+      <c r="AZ100">
+        <v>30</v>
+      </c>
+      <c r="BA100">
+        <v>15</v>
+      </c>
+      <c r="BB100">
+        <v>13</v>
+      </c>
+      <c r="BC100">
+        <v>13</v>
+      </c>
+      <c r="BD100">
+        <v>32</v>
+      </c>
+      <c r="BE100">
+        <v>25</v>
+      </c>
+      <c r="BF100">
+        <v>25</v>
+      </c>
+      <c r="BG100">
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:59" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated FT database and made changes to some of the visuals to create show notes
</commit_message>
<xml_diff>
--- a/projects/firstTurnData/FirstTurnCombined.xlsx
+++ b/projects/firstTurnData/FirstTurnCombined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PNJae\Dropbox\website\PNJaenichen.github.io\projects\firstTurnData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A222A588-7392-4AFB-A6D0-83A2BC065E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE338A7-B9B6-4089-A87B-9069A6E2B87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="2715" windowWidth="29040" windowHeight="15840" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
+    <workbookView xWindow="-240" yWindow="0" windowWidth="29040" windowHeight="15600" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3022" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3022" uniqueCount="323">
   <si>
     <t>Yes</t>
   </si>
@@ -328,9 +328,6 @@
     <t>Fantastic Factories</t>
   </si>
   <si>
-    <t xml:space="preserve">no </t>
-  </si>
-  <si>
     <t>kiwi</t>
   </si>
   <si>
@@ -482,9 +479,6 @@
   </si>
   <si>
     <t>Yokohama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes </t>
   </si>
   <si>
     <t>Kait</t>
@@ -1404,8 +1398,8 @@
   <dimension ref="A1:FJ136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R134" sqref="R134"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I138" sqref="I138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,42 +1407,42 @@
     <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="40" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="19.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="21.140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5703125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5703125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="19.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="21.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" style="1" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="19.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="21.140625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="12.5703125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="16.5703125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="14.7109375" style="1" customWidth="1"/>
+    <col min="34" max="34" width="22.42578125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="24.5703125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="15.7109375" style="1" customWidth="1"/>
+    <col min="37" max="37" width="19.85546875" style="1" customWidth="1"/>
+    <col min="38" max="40" width="16.7109375" style="1" customWidth="1"/>
+    <col min="41" max="41" width="16" style="1" customWidth="1"/>
     <col min="42" max="42" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="43" max="44" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -1576,499 +1570,499 @@
   <sheetData>
     <row r="1" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="AV1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="AX1" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AY1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="CK1" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AZ1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="BA1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="CW1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="CX1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="DC1" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="DD1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="DE1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="DN1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="DO1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="BB1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="BC1" s="1" t="s">
+      <c r="DR1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="DS1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="DT1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="DU1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="DV1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="DW1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="DX1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="DY1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="EA1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="EB1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="EC1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="ED1" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="EE1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="EF1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="EG1" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="EH1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="EI1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="EJ1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="EK1" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="EL1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="EM1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="EN1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="EO1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="EP1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="EQ1" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="ER1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="ES1" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="ET1" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="EU1" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="EV1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="EW1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="EX1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="EY1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="EZ1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="FA1" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="FB1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="FC1" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="FD1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="FE1" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="FF1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="FG1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="FH1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="BD1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="BZ1" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="CA1" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="CB1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="CC1" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="CD1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="CF1" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="CH1" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="CI1" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="CJ1" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="CK1" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="CL1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="CM1" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="CN1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="CO1" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="CP1" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="CQ1" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="CR1" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="CS1" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="CT1" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="CU1" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="CV1" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="CW1" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="CX1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="CY1" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="CZ1" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="DA1" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="DB1" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="DC1" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="DD1" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="DE1" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="DF1" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="DG1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="DH1" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="DI1" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="DJ1" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="DL1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="DM1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="DN1" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="DO1" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="DP1" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="DQ1" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="DR1" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="DS1" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="DT1" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="DU1" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="DV1" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="DW1" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="DX1" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="DY1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="DZ1" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="EA1" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="EB1" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="EC1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="ED1" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="EE1" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="EF1" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="EG1" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="EH1" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="EI1" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="EJ1" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="EK1" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="EL1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="EM1" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="EN1" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="EO1" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="EP1" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="EQ1" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="ER1" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="ES1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="ET1" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="EU1" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="EV1" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="EW1" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="EX1" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="EY1" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="EZ1" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="FA1" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="FB1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="FC1" s="1" t="s">
+      <c r="FI1" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="FD1" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="FE1" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="FF1" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="FG1" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="FH1" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="FI1" s="1" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:166" x14ac:dyDescent="0.25">
@@ -44687,7 +44681,7 @@
         <v>-1.5023441718644308</v>
       </c>
       <c r="Z85" s="1" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="AA85" s="1" t="s">
         <v>39</v>
@@ -45149,7 +45143,7 @@
         <v>3</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L86" s="1" t="s">
         <v>41</v>
@@ -46147,7 +46141,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C88" s="6">
         <v>3</v>
@@ -46656,7 +46650,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C89" s="6">
         <v>3</v>
@@ -47165,7 +47159,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C90" s="6">
         <v>3</v>
@@ -47658,7 +47652,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C91" s="6">
         <v>3</v>
@@ -48171,7 +48165,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C92" s="6">
         <v>3</v>
@@ -48684,7 +48678,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C93" s="6">
         <v>3</v>
@@ -49197,7 +49191,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C94" s="6">
         <v>3</v>
@@ -49710,7 +49704,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C95" s="6">
         <v>3</v>
@@ -50223,7 +50217,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C96" s="6">
         <v>3</v>
@@ -50732,7 +50726,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C97" s="6">
         <v>3</v>
@@ -51245,7 +51239,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C98" s="6">
         <v>3</v>
@@ -51758,7 +51752,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C99" s="6">
         <v>3</v>
@@ -52271,7 +52265,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C100" s="6">
         <v>3</v>
@@ -52784,7 +52778,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C101" s="6">
         <v>3</v>
@@ -53298,7 +53292,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C102" s="6">
         <v>3</v>
@@ -53811,7 +53805,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C103" s="6">
         <v>3</v>
@@ -54320,7 +54314,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C104" s="6">
         <v>3</v>
@@ -54365,7 +54359,7 @@
         <v>-0.83902850324068046</v>
       </c>
       <c r="P104" s="1" t="s">
-        <v>148</v>
+        <v>38</v>
       </c>
       <c r="Q104" s="7"/>
       <c r="R104" s="1">
@@ -54827,7 +54821,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C105" s="6">
         <v>3</v>
@@ -55340,7 +55334,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C106" s="6">
         <v>3</v>
@@ -55837,7 +55831,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C107" s="6">
         <v>3</v>
@@ -55866,7 +55860,7 @@
       </c>
       <c r="K107" s="7"/>
       <c r="L107" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M107" s="1">
         <v>50</v>
@@ -56344,7 +56338,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C108" s="6">
         <v>3</v>
@@ -56853,7 +56847,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C109" s="6">
         <v>3</v>
@@ -57362,7 +57356,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C110" s="6">
         <v>3</v>
@@ -57875,7 +57869,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C111" s="6">
         <v>3</v>
@@ -58384,7 +58378,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C112" s="6">
         <v>3</v>
@@ -58897,7 +58891,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C113" s="6">
         <v>3</v>
@@ -59410,7 +59404,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C114" s="6">
         <v>3</v>
@@ -59921,7 +59915,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C115" s="6">
         <v>3</v>
@@ -60434,7 +60428,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C116" s="6">
         <v>3</v>
@@ -60941,7 +60935,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C117" s="6">
         <v>3</v>
@@ -61454,7 +61448,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C118" s="6">
         <v>3</v>
@@ -61967,7 +61961,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C119" s="6">
         <v>3</v>
@@ -62476,7 +62470,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C120" s="6">
         <v>3</v>
@@ -62985,7 +62979,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C121" s="6">
         <v>3</v>
@@ -63498,7 +63492,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C122" s="6">
         <v>3</v>
@@ -64009,7 +64003,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C123" s="6">
         <v>3</v>
@@ -64520,7 +64514,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C124" s="6">
         <v>3</v>
@@ -65025,7 +65019,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C125" s="6">
         <v>3</v>
@@ -65538,7 +65532,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C126" s="6">
         <v>3</v>
@@ -66039,7 +66033,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C127" s="6">
         <v>3</v>
@@ -66552,7 +66546,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C128" s="6">
         <v>3</v>
@@ -67065,7 +67059,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C129" s="6">
         <v>3</v>
@@ -67578,7 +67572,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C130" s="6">
         <v>3</v>
@@ -68087,10 +68081,10 @@
         <v>131</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D131" s="1">
         <v>90</v>
@@ -68600,10 +68594,10 @@
         <v>132</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D132" s="1">
         <v>60</v>
@@ -69113,10 +69107,10 @@
         <v>133</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D133" s="7"/>
       <c r="E133" s="1">
@@ -69608,18 +69602,20 @@
         <v>134</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D134" s="7"/>
+        <v>201</v>
+      </c>
+      <c r="D134" s="8">
+        <v>45</v>
+      </c>
       <c r="E134" s="1">
         <v>45</v>
       </c>
       <c r="F134" s="1">
         <f t="shared" si="32"/>
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="G134" s="1">
         <v>2.2000000000000002</v>
@@ -70103,10 +70099,10 @@
         <v>135</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D135" s="8">
         <v>130</v>
@@ -70151,7 +70147,7 @@
         <v>38</v>
       </c>
       <c r="Q135" s="8" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="R135" s="8">
         <v>15</v>
@@ -70230,7 +70226,7 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="AN135" s="8">
-        <f t="shared" ref="AN134:AN136" si="61">MAX(N135,S135,X135,AH135,AC135)</f>
+        <f t="shared" ref="AN135:AN136" si="61">MAX(N135,S135,X135,AH135,AC135)</f>
         <v>0.875</v>
       </c>
       <c r="AO135" s="8">
@@ -70616,10 +70612,10 @@
         <v>136</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D136" s="7"/>
       <c r="E136" s="1">
@@ -71126,25 +71122,25 @@
         <v>35</v>
       </c>
       <c r="B1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" t="s">
         <v>139</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>140</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>141</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>142</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>143</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>144</v>
-      </c>
-      <c r="H1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
@@ -73711,7 +73707,7 @@
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -75907,7 +75903,7 @@
     </row>
     <row r="28" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
@@ -83286,7 +83282,7 @@
     </row>
     <row r="68" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B68">
         <f t="shared" ref="B68:B96" si="14">AVERAGE(I68:BG68)</f>
@@ -83469,7 +83465,7 @@
     </row>
     <row r="69" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B69">
         <f t="shared" si="14"/>
@@ -83655,7 +83651,7 @@
     </row>
     <row r="70" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B70">
         <f t="shared" si="14"/>
@@ -83841,7 +83837,7 @@
     </row>
     <row r="71" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B71">
         <f t="shared" si="14"/>
@@ -83985,7 +83981,7 @@
     </row>
     <row r="72" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B72">
         <f t="shared" si="14"/>
@@ -84171,7 +84167,7 @@
     </row>
     <row r="73" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B73">
         <f t="shared" si="14"/>
@@ -84357,7 +84353,7 @@
     </row>
     <row r="74" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B74">
         <f t="shared" si="14"/>
@@ -84540,7 +84536,7 @@
     </row>
     <row r="75" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B75">
         <f t="shared" si="14"/>
@@ -84726,7 +84722,7 @@
     </row>
     <row r="76" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B76">
         <f t="shared" si="14"/>
@@ -84912,7 +84908,7 @@
     </row>
     <row r="77" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B77">
         <f t="shared" si="14"/>
@@ -85098,7 +85094,7 @@
     </row>
     <row r="78" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B78">
         <f t="shared" si="14"/>
@@ -85284,7 +85280,7 @@
     </row>
     <row r="79" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B79">
         <f t="shared" si="14"/>
@@ -85464,7 +85460,7 @@
     </row>
     <row r="80" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B80">
         <f t="shared" si="14"/>
@@ -85650,7 +85646,7 @@
     </row>
     <row r="81" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B81">
         <f t="shared" si="14"/>
@@ -85833,7 +85829,7 @@
     </row>
     <row r="82" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B82">
         <f t="shared" si="14"/>
@@ -86019,7 +86015,7 @@
     </row>
     <row r="83" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B83">
         <f t="shared" si="14"/>
@@ -86205,7 +86201,7 @@
     </row>
     <row r="84" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B84">
         <f t="shared" si="14"/>
@@ -86391,7 +86387,7 @@
     </row>
     <row r="85" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B85">
         <f t="shared" si="14"/>
@@ -86568,7 +86564,7 @@
     </row>
     <row r="86" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B86">
         <f t="shared" si="14"/>
@@ -86751,7 +86747,7 @@
     </row>
     <row r="87" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B87">
         <f t="shared" si="14"/>
@@ -86937,7 +86933,7 @@
     </row>
     <row r="88" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B88">
         <f t="shared" si="14"/>
@@ -87123,7 +87119,7 @@
     </row>
     <row r="89" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B89">
         <f t="shared" si="14"/>
@@ -87309,7 +87305,7 @@
     </row>
     <row r="90" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B90">
         <f t="shared" si="14"/>
@@ -87492,7 +87488,7 @@
     </row>
     <row r="91" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B91">
         <f t="shared" si="14"/>
@@ -87678,7 +87674,7 @@
     </row>
     <row r="92" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B92">
         <f t="shared" si="14"/>
@@ -87864,7 +87860,7 @@
     </row>
     <row r="93" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B93">
         <f t="shared" si="14"/>
@@ -88050,7 +88046,7 @@
     </row>
     <row r="94" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B94">
         <f t="shared" si="14"/>
@@ -88233,7 +88229,7 @@
     </row>
     <row r="95" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B95">
         <f t="shared" si="14"/>
@@ -88416,7 +88412,7 @@
     </row>
     <row r="96" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B96">
         <f t="shared" si="14"/>
@@ -88602,7 +88598,7 @@
     </row>
     <row r="97" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B97">
         <f t="shared" ref="B97:B98" si="21">AVERAGE(I97:BG97)</f>
@@ -88788,7 +88784,7 @@
     </row>
     <row r="98" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B98">
         <f t="shared" si="21"/>
@@ -88974,7 +88970,7 @@
     </row>
     <row r="99" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B99">
         <f t="shared" ref="B99:B106" si="28">AVERAGE(I99:BG99)</f>
@@ -89160,7 +89156,7 @@
     </row>
     <row r="100" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B100">
         <f t="shared" si="28"/>
@@ -89346,7 +89342,7 @@
     </row>
     <row r="101" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B101">
         <f t="shared" si="28"/>
@@ -89532,7 +89528,7 @@
     </row>
     <row r="102" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B102">
         <f t="shared" si="28"/>
@@ -89718,7 +89714,7 @@
     </row>
     <row r="103" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B103">
         <f t="shared" si="28"/>

</xml_diff>

<commit_message>
udpated first turn dataset
</commit_message>
<xml_diff>
--- a/projects/firstTurnData/FirstTurnCombined.xlsx
+++ b/projects/firstTurnData/FirstTurnCombined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PNJae\Dropbox\website\PNJaenichen.github.io\projects\firstTurnData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BF582C-780B-467B-A2CF-1821B0E5FB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDD159F-30B2-47A3-ABAE-7B416E6CC34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3197" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3214" uniqueCount="330">
   <si>
     <t>Yes</t>
   </si>
@@ -1026,6 +1026,9 @@
   <si>
     <t>The Isle of Cats</t>
   </si>
+  <si>
+    <t>Bruxelles 1897</t>
+  </si>
 </sst>
 </file>
 
@@ -1413,8 +1416,8 @@
   <dimension ref="A1:FK153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E144" sqref="E144"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H143" sqref="H143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74164,71 +74167,515 @@
       <c r="A142" s="1">
         <v>131</v>
       </c>
+      <c r="B142" s="2" t="s">
+        <v>329</v>
+      </c>
       <c r="C142" s="6" t="s">
         <v>324</v>
       </c>
+      <c r="D142" s="1">
+        <v>75</v>
+      </c>
+      <c r="E142" s="1">
+        <v>50</v>
+      </c>
       <c r="F142" s="7">
         <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="N142" s="7" t="e">
+        <v>25</v>
+      </c>
+      <c r="G142" s="1">
+        <v>2.91</v>
+      </c>
+      <c r="H142" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="I142" s="1">
+        <v>1585</v>
+      </c>
+      <c r="J142" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K142" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L142" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="M142" s="1">
+        <v>34</v>
+      </c>
+      <c r="N142" s="7">
         <f t="shared" ref="N142:N153" si="108">IF(M142="null", "null", (M142-$AS142)/($AT142-$AS142))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O142" s="7" t="e">
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="O142" s="7">
         <f t="shared" ref="O142:O153" si="109">IF(M142="null","null",(M142-$AQ142)/$AR142)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S142" s="7" t="e">
+        <v>-0.8024300452416393</v>
+      </c>
+      <c r="P142" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q142" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R142" s="1">
+        <v>41</v>
+      </c>
+      <c r="S142" s="7">
         <f t="shared" ref="S142:S153" si="110">IF(R142="null", "null", (R142-$AS142)/($AT142-$AS142))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T142" s="7" t="e">
+        <v>0.38636363636363635</v>
+      </c>
+      <c r="T142" s="7">
         <f t="shared" ref="T142:T153" si="111">IF(R142="null","null",(R142-$AQ142)/$AR142)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X142" s="7" t="e">
+        <v>-0.10712051574827706</v>
+      </c>
+      <c r="U142" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V142" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W142" s="1">
+        <v>27</v>
+      </c>
+      <c r="X142" s="7">
         <f t="shared" ref="X142:X153" si="112">IF(W142="null", "null", (W142-$AS142)/($AT142-$AS142))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y142" s="7" t="e">
+        <v>6.8181818181818177E-2</v>
+      </c>
+      <c r="Y142" s="7">
         <f t="shared" ref="Y142:Y153" si="113">IF(W142="null","null",(W142-$AQ142)/$AR142)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC142" s="7" t="e">
+        <v>-1.4977395747350015</v>
+      </c>
+      <c r="Z142" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA142" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB142" s="1">
+        <v>61</v>
+      </c>
+      <c r="AC142" s="7">
         <f t="shared" ref="AC142:AC153" si="114">IF(AB142="null", "null", (AB142-$AS142)/($AT142-$AS142))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD142" s="7" t="e">
+        <v>0.84090909090909094</v>
+      </c>
+      <c r="AD142" s="7">
         <f t="shared" ref="AD142:AD153" si="115">IF(AB142="null","null",(AB142-$AQ142)/$AR142)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH142" s="7" t="e">
+        <v>1.8794781399470437</v>
+      </c>
+      <c r="AE142" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF142" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG142" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH142" s="7" t="str">
         <f t="shared" ref="AH142:AH153" si="116">IF(AG142="null", "null", (AG142-$AS142)/($AT142-$AS142))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI142" s="7" t="e">
+        <v>null</v>
+      </c>
+      <c r="AI142" s="7" t="str">
         <f t="shared" ref="AI142:AI153" si="117">IF(AG142="null","null",(AG142-$AQ142)/$AR142)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AL142" s="7" t="e">
+        <v>null</v>
+      </c>
+      <c r="AJ142" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK142" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL142" s="7">
         <f t="shared" ref="AL142" si="118">MIN(N142,S142,X142,AH142,AC142)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AM142" s="7" t="e">
+        <v>6.8181818181818177E-2</v>
+      </c>
+      <c r="AM142" s="7">
         <f t="shared" ref="AM142" si="119">AVERAGE(N142,S142,X142,AH142,AC142)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AN142" s="7" t="e">
+        <v>0.38068181818181823</v>
+      </c>
+      <c r="AN142" s="7">
         <f t="shared" ref="AN142" si="120">MAX(N142,S142,X142,AH142,AC142)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AO142" s="7" t="e">
+        <v>0.84090909090909094</v>
+      </c>
+      <c r="AO142" s="7">
         <f t="shared" ref="AO142" si="121">AN142-AL142</f>
-        <v>#DIV/0!</v>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="AP142" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ142" s="1">
+        <v>42.078431372549019</v>
+      </c>
+      <c r="AR142" s="1">
+        <v>10.067458740426806</v>
+      </c>
+      <c r="AS142" s="1">
+        <v>24</v>
+      </c>
+      <c r="AT142" s="1">
+        <v>68</v>
+      </c>
+      <c r="AU142" s="1">
+        <v>36</v>
+      </c>
+      <c r="AV142" s="1">
+        <v>48</v>
+      </c>
+      <c r="AW142" s="1">
+        <v>41</v>
       </c>
       <c r="AX142" s="10">
         <f t="shared" si="79"/>
+        <v>4</v>
+      </c>
+      <c r="AY142" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ142" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH142" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG142" s="1">
+        <v>1</v>
+      </c>
+      <c r="DH142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC142" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EG142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EI142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EK142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EM142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER142" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES142" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY142" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA142" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB142" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC142" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD142" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE142" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF142" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG142" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH142" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI142" s="1">
+        <v>1</v>
+      </c>
+      <c r="FJ142" s="1">
         <v>0</v>
       </c>
     </row>
@@ -74303,6 +74750,354 @@
         <f t="shared" si="79"/>
         <v>0</v>
       </c>
+      <c r="AY143" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY143" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY143" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY143" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC143" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EG143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EI143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EK143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EM143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER143" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES143" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY143" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ143" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA143" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB143" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC143" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD143" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE143" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF143" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG143" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH143" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI143" s="1">
+        <v>0</v>
+      </c>
+      <c r="FJ143" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="144" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
@@ -74375,8 +75170,356 @@
         <f t="shared" si="79"/>
         <v>0</v>
       </c>
+      <c r="AY144" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY144" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY144" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY144" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC144" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EG144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EI144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EK144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EM144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER144" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES144" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY144" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ144" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA144" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB144" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC144" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD144" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE144" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF144" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG144" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH144" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI144" s="1">
+        <v>0</v>
+      </c>
+      <c r="FJ144" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="145" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>134</v>
       </c>
@@ -74447,8 +75590,356 @@
         <f t="shared" si="79"/>
         <v>0</v>
       </c>
+      <c r="AY145" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY145" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY145" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY145" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC145" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EG145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EI145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EK145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EM145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER145" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES145" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY145" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ145" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA145" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB145" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC145" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD145" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE145" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF145" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG145" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH145" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI145" s="1">
+        <v>0</v>
+      </c>
+      <c r="FJ145" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="146" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>135</v>
       </c>
@@ -74519,8 +76010,356 @@
         <f t="shared" si="79"/>
         <v>0</v>
       </c>
+      <c r="AY146" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY146" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY146" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY146" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC146" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EG146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EI146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EK146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EM146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER146" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES146" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY146" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ146" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA146" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB146" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC146" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD146" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE146" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF146" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG146" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH146" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI146" s="1">
+        <v>0</v>
+      </c>
+      <c r="FJ146" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="147" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>136</v>
       </c>
@@ -74591,8 +76430,356 @@
         <f t="shared" si="79"/>
         <v>0</v>
       </c>
+      <c r="AY147" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY147" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY147" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY147" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC147" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EG147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EI147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EK147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EM147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER147" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES147" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY147" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ147" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA147" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB147" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC147" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD147" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE147" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF147" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG147" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH147" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI147" s="1">
+        <v>0</v>
+      </c>
+      <c r="FJ147" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="148" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>137</v>
       </c>
@@ -74663,8 +76850,356 @@
         <f t="shared" si="79"/>
         <v>0</v>
       </c>
+      <c r="AY148" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY148" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY148" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY148" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC148" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EG148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EI148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EK148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EM148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER148" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES148" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY148" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ148" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA148" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB148" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC148" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD148" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE148" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF148" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG148" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH148" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI148" s="1">
+        <v>0</v>
+      </c>
+      <c r="FJ148" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="149" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>138</v>
       </c>
@@ -74735,8 +77270,356 @@
         <f t="shared" si="79"/>
         <v>0</v>
       </c>
+      <c r="AY149" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY149" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY149" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY149" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC149" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EG149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EI149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EK149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EM149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER149" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES149" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY149" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ149" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA149" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB149" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC149" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD149" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE149" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF149" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG149" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH149" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI149" s="1">
+        <v>0</v>
+      </c>
+      <c r="FJ149" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="150" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>139</v>
       </c>
@@ -74807,8 +77690,356 @@
         <f t="shared" si="79"/>
         <v>0</v>
       </c>
+      <c r="AY150" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY150" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY150" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY150" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC150" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EG150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EI150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EK150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EM150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER150" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES150" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY150" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ150" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA150" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB150" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC150" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD150" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE150" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF150" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG150" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH150" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI150" s="1">
+        <v>0</v>
+      </c>
+      <c r="FJ150" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="151" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>140</v>
       </c>
@@ -74879,8 +78110,356 @@
         <f t="shared" si="79"/>
         <v>0</v>
       </c>
+      <c r="AY151" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY151" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY151" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY151" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC151" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EG151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EI151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EK151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EM151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER151" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES151" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY151" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ151" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA151" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB151" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC151" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD151" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE151" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF151" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG151" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH151" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI151" s="1">
+        <v>0</v>
+      </c>
+      <c r="FJ151" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="152" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>141</v>
       </c>
@@ -74951,8 +78530,356 @@
         <f t="shared" si="79"/>
         <v>0</v>
       </c>
+      <c r="AY152" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY152" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY152" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY152" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC152" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EG152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EI152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EK152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EM152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER152" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES152" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY152" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ152" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA152" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB152" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC152" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD152" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE152" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF152" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG152" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH152" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI152" s="1">
+        <v>0</v>
+      </c>
+      <c r="FJ152" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="153" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>142</v>
       </c>
@@ -75021,6 +78948,354 @@
       </c>
       <c r="AX153" s="10">
         <f t="shared" si="79"/>
+        <v>0</v>
+      </c>
+      <c r="AY153" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY153" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY153" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DT153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DU153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DV153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DW153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DX153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DY153" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC153" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EG153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EH153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EI153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EJ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EK153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EL153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EM153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER153" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES153" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY153" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ153" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA153" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB153" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC153" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD153" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE153" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF153" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG153" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH153" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI153" s="1">
+        <v>0</v>
+      </c>
+      <c r="FJ153" s="1">
         <v>0</v>
       </c>
     </row>
@@ -75035,9 +79310,9 @@
   <dimension ref="A1:BG117"/>
   <sheetViews>
     <sheetView topLeftCell="A88" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A58" sqref="A58"/>
-      <selection pane="topRight" activeCell="B106" sqref="B106:H106"/>
+      <selection pane="topRight" activeCell="B107" sqref="B107:H107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -94368,33 +98643,189 @@
       </c>
     </row>
     <row r="107" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B107" t="e">
+      <c r="A107" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B107">
         <f t="shared" ref="B107:B117" si="35">AVERAGE(I107:BG107)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C107" t="e">
+        <v>42.078431372549019</v>
+      </c>
+      <c r="C107">
         <f t="shared" ref="C107:C117" si="36">_xlfn.STDEV.S(I107:BG107)</f>
-        <v>#DIV/0!</v>
+        <v>10.067458740426806</v>
       </c>
       <c r="D107">
         <f t="shared" ref="D107:D117" si="37">MIN(I107:BG107)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E107">
         <f t="shared" ref="E107:E117" si="38">MAX(J107:BG107)</f>
-        <v>0</v>
-      </c>
-      <c r="F107" t="e">
+        <v>68</v>
+      </c>
+      <c r="F107">
         <f t="shared" ref="F107:F117" si="39">_xlfn.QUARTILE.EXC(I107:BG107,1)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G107" t="e">
+        <v>36</v>
+      </c>
+      <c r="G107">
         <f t="shared" ref="G107:G117" si="40">_xlfn.QUARTILE.EXC(I107:BG107,3)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H107" t="e">
+        <v>48</v>
+      </c>
+      <c r="H107">
         <f t="shared" ref="H107:H117" si="41">MEDIAN(I107:BG107)</f>
-        <v>#NUM!</v>
+        <v>41</v>
+      </c>
+      <c r="I107">
+        <v>59</v>
+      </c>
+      <c r="J107">
+        <v>47</v>
+      </c>
+      <c r="K107">
+        <v>44</v>
+      </c>
+      <c r="L107">
+        <v>60</v>
+      </c>
+      <c r="M107">
+        <v>37</v>
+      </c>
+      <c r="N107">
+        <v>28</v>
+      </c>
+      <c r="O107">
+        <v>25</v>
+      </c>
+      <c r="P107">
+        <v>36</v>
+      </c>
+      <c r="Q107">
+        <v>39</v>
+      </c>
+      <c r="R107">
+        <v>47</v>
+      </c>
+      <c r="S107">
+        <v>32</v>
+      </c>
+      <c r="T107">
+        <v>24</v>
+      </c>
+      <c r="U107">
+        <v>54</v>
+      </c>
+      <c r="V107">
+        <v>68</v>
+      </c>
+      <c r="W107">
+        <v>47</v>
+      </c>
+      <c r="X107">
+        <v>39</v>
+      </c>
+      <c r="Y107">
+        <v>48</v>
+      </c>
+      <c r="Z107">
+        <v>49</v>
+      </c>
+      <c r="AA107">
+        <v>44</v>
+      </c>
+      <c r="AB107">
+        <v>37</v>
+      </c>
+      <c r="AC107">
+        <v>29</v>
+      </c>
+      <c r="AD107">
+        <v>37</v>
+      </c>
+      <c r="AE107">
+        <v>26</v>
+      </c>
+      <c r="AF107">
+        <v>36</v>
+      </c>
+      <c r="AG107">
+        <v>43</v>
+      </c>
+      <c r="AH107">
+        <v>51</v>
+      </c>
+      <c r="AI107">
+        <v>46</v>
+      </c>
+      <c r="AJ107">
+        <v>49</v>
+      </c>
+      <c r="AK107">
+        <v>34</v>
+      </c>
+      <c r="AL107">
+        <v>41</v>
+      </c>
+      <c r="AM107">
+        <v>54</v>
+      </c>
+      <c r="AN107">
+        <v>37</v>
+      </c>
+      <c r="AO107">
+        <v>37</v>
+      </c>
+      <c r="AP107">
+        <v>39</v>
+      </c>
+      <c r="AQ107">
+        <v>35</v>
+      </c>
+      <c r="AR107">
+        <v>42</v>
+      </c>
+      <c r="AS107">
+        <v>49</v>
+      </c>
+      <c r="AT107">
+        <v>46</v>
+      </c>
+      <c r="AU107">
+        <v>44</v>
+      </c>
+      <c r="AV107">
+        <v>37</v>
+      </c>
+      <c r="AW107">
+        <v>60</v>
+      </c>
+      <c r="AX107">
+        <v>40</v>
+      </c>
+      <c r="AY107">
+        <v>36</v>
+      </c>
+      <c r="AZ107">
+        <v>33</v>
+      </c>
+      <c r="BA107">
+        <v>44</v>
+      </c>
+      <c r="BB107">
+        <v>34</v>
+      </c>
+      <c r="BC107">
+        <v>63</v>
+      </c>
+      <c r="BD107">
+        <v>28</v>
+      </c>
+      <c r="BE107">
+        <v>56</v>
+      </c>
+      <c r="BF107">
+        <v>34</v>
+      </c>
+      <c r="BG107">
+        <v>42</v>
       </c>
     </row>
     <row r="108" spans="1:59" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
completed Netflix Data project for codecademy
</commit_message>
<xml_diff>
--- a/projects/firstTurnData/FirstTurnCombined.xlsx
+++ b/projects/firstTurnData/FirstTurnCombined.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PNJae\Dropbox\website\PNJaenichen.github.io\projects\firstTurnData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDD159F-30B2-47A3-ABAE-7B416E6CC34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36451507-5AD7-4AAB-8127-D645DEB84D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
+    <workbookView xWindow="-28785" yWindow="15" windowWidth="28770" windowHeight="15450" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="2" r:id="rId1"/>
@@ -1018,9 +1018,6 @@
     <t>turn_role_order</t>
   </si>
   <si>
-    <t>Intrepid</t>
-  </si>
-  <si>
     <t>Deep Space D-6 Armada</t>
   </si>
   <si>
@@ -1028,6 +1025,9 @@
   </si>
   <si>
     <t>Bruxelles 1897</t>
+  </si>
+  <si>
+    <t>Cascadia</t>
   </si>
 </sst>
 </file>
@@ -1413,11 +1413,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796E82C3-294D-4E4E-8DE4-13BF7BF427EB}">
-  <dimension ref="A1:FK153"/>
+  <dimension ref="A1:FK152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H143" sqref="H143"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V138" sqref="V138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68058,7 +68058,7 @@
         <v>50</v>
       </c>
       <c r="F130" s="1">
-        <f t="shared" ref="F130:F153" si="68">D130-E130</f>
+        <f t="shared" ref="F130:F152" si="68">D130-E130</f>
         <v>10</v>
       </c>
       <c r="G130" s="1">
@@ -68201,7 +68201,7 @@
         <v>36</v>
       </c>
       <c r="AX130" s="3">
-        <f t="shared" ref="AX130:AX153" si="79">SUM(AY130:FJ130)</f>
+        <f t="shared" ref="AX130:AX152" si="79">SUM(AY130:FJ130)</f>
         <v>3</v>
       </c>
       <c r="AY130" s="1">
@@ -72171,12 +72171,14 @@
       <c r="C138" s="6" t="s">
         <v>324</v>
       </c>
+      <c r="D138" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="E138" s="1">
         <v>60</v>
       </c>
-      <c r="F138" s="7">
-        <f t="shared" si="68"/>
-        <v>-60</v>
+      <c r="F138" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="G138" s="1">
         <v>2</v>
@@ -72190,15 +72192,18 @@
       <c r="J138" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="K138" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="M138" s="1" t="s">
         <v>36</v>
       </c>
       <c r="N138" s="7" t="str">
-        <f t="shared" ref="N138:N141" si="94">IF(M138="null", "null", (M138-$AS138)/($AT138-$AS138))</f>
+        <f t="shared" ref="N138:N140" si="94">IF(M138="null", "null", (M138-$AS138)/($AT138-$AS138))</f>
         <v>null</v>
       </c>
       <c r="O138" s="7" t="str">
-        <f t="shared" ref="O138:O141" si="95">IF(M138="null","null",(M138-$AQ138)/$AR138)</f>
+        <f t="shared" ref="O138:O140" si="95">IF(M138="null","null",(M138-$AQ138)/$AR138)</f>
         <v>null</v>
       </c>
       <c r="P138" s="1" t="s">
@@ -72207,23 +72212,32 @@
       <c r="Q138" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="R138" s="1">
+        <v>62</v>
+      </c>
       <c r="S138" s="7">
-        <f t="shared" ref="S138:S141" si="96">IF(R138="null", "null", (R138-$AS138)/($AT138-$AS138))</f>
-        <v>-0.33333333333333331</v>
+        <f t="shared" ref="S138:S140" si="96">IF(R138="null", "null", (R138-$AS138)/($AT138-$AS138))</f>
+        <v>0.49333333333333335</v>
       </c>
       <c r="T138" s="7">
-        <f t="shared" ref="T138:T141" si="97">IF(R138="null","null",(R138-$AQ138)/$AR138)</f>
-        <v>-4.3321077947441138</v>
+        <f t="shared" ref="T138:T140" si="97">IF(R138="null","null",(R138-$AQ138)/$AR138)</f>
+        <v>9.6204278079781741E-2</v>
+      </c>
+      <c r="U138" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V138" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="W138" s="1" t="s">
         <v>36</v>
       </c>
       <c r="X138" s="7" t="str">
-        <f t="shared" ref="X138:X141" si="98">IF(W138="null", "null", (W138-$AS138)/($AT138-$AS138))</f>
+        <f t="shared" ref="X138:X140" si="98">IF(W138="null", "null", (W138-$AS138)/($AT138-$AS138))</f>
         <v>null</v>
       </c>
       <c r="Y138" s="7" t="str">
-        <f t="shared" ref="Y138:Y141" si="99">IF(W138="null","null",(W138-$AQ138)/$AR138)</f>
+        <f t="shared" ref="Y138:Y140" si="99">IF(W138="null","null",(W138-$AQ138)/$AR138)</f>
         <v>null</v>
       </c>
       <c r="Z138" s="1" t="s">
@@ -72232,23 +72246,32 @@
       <c r="AA138" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="AB138" s="1">
+        <v>52</v>
+      </c>
       <c r="AC138" s="7">
-        <f t="shared" ref="AC138:AC141" si="100">IF(AB138="null", "null", (AB138-$AS138)/($AT138-$AS138))</f>
-        <v>-0.33333333333333331</v>
+        <f t="shared" ref="AC138:AC140" si="100">IF(AB138="null", "null", (AB138-$AS138)/($AT138-$AS138))</f>
+        <v>0.36</v>
       </c>
       <c r="AD138" s="7">
-        <f t="shared" ref="AD138:AD141" si="101">IF(AB138="null","null",(AB138-$AQ138)/$AR138)</f>
-        <v>-4.3321077947441138</v>
+        <f t="shared" ref="AD138:AD140" si="101">IF(AB138="null","null",(AB138-$AQ138)/$AR138)</f>
+        <v>-0.61803960463374974</v>
+      </c>
+      <c r="AE138" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF138" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="AG138" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AH138" s="7" t="str">
-        <f t="shared" ref="AH138:AH141" si="102">IF(AG138="null", "null", (AG138-$AS138)/($AT138-$AS138))</f>
+        <f t="shared" ref="AH138:AH140" si="102">IF(AG138="null", "null", (AG138-$AS138)/($AT138-$AS138))</f>
         <v>null</v>
       </c>
       <c r="AI138" s="7" t="str">
-        <f t="shared" ref="AI138:AI141" si="103">IF(AG138="null","null",(AG138-$AQ138)/$AR138)</f>
+        <f t="shared" ref="AI138:AI140" si="103">IF(AG138="null","null",(AG138-$AQ138)/$AR138)</f>
         <v>null</v>
       </c>
       <c r="AJ138" s="1" t="s">
@@ -72258,20 +72281,20 @@
         <v>36</v>
       </c>
       <c r="AL138" s="7">
-        <f t="shared" ref="AL138:AL140" si="104">MIN(N138,S138,X138,AH138,AC138)</f>
-        <v>-0.33333333333333331</v>
+        <f t="shared" ref="AL138:AL139" si="104">MIN(N138,S138,X138,AH138,AC138)</f>
+        <v>0.36</v>
       </c>
       <c r="AM138" s="7">
-        <f t="shared" ref="AM138:AM140" si="105">AVERAGE(N138,S138,X138,AH138,AC138)</f>
-        <v>-0.33333333333333331</v>
+        <f t="shared" ref="AM138:AM139" si="105">AVERAGE(N138,S138,X138,AH138,AC138)</f>
+        <v>0.42666666666666664</v>
       </c>
       <c r="AN138" s="7">
-        <f t="shared" ref="AN138:AN140" si="106">MAX(N138,S138,X138,AH138,AC138)</f>
-        <v>-0.33333333333333331</v>
+        <f t="shared" ref="AN138:AN139" si="106">MAX(N138,S138,X138,AH138,AC138)</f>
+        <v>0.49333333333333335</v>
       </c>
       <c r="AO138" s="7">
-        <f t="shared" ref="AO138:AO140" si="107">AN138-AL138</f>
-        <v>0</v>
+        <f t="shared" ref="AO138:AO139" si="107">AN138-AL138</f>
+        <v>0.13333333333333336</v>
       </c>
       <c r="AP138" s="1" t="s">
         <v>39</v>
@@ -72652,82 +72675,109 @@
     </row>
     <row r="139" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>324</v>
       </c>
+      <c r="D139" s="1">
+        <v>180</v>
+      </c>
       <c r="E139" s="1">
         <v>75</v>
       </c>
       <c r="F139" s="7">
         <f t="shared" si="68"/>
-        <v>-75</v>
+        <v>105</v>
       </c>
       <c r="G139" s="1">
-        <v>3.38</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H139" s="1">
-        <v>7.5</v>
+        <v>7.9</v>
       </c>
       <c r="I139" s="1">
-        <v>4069</v>
+        <v>98</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N139" s="7" t="str">
+        <v>3</v>
+      </c>
+      <c r="K139" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M139" s="1">
+        <v>30</v>
+      </c>
+      <c r="N139" s="7">
         <f t="shared" si="94"/>
-        <v>null</v>
-      </c>
-      <c r="O139" s="7" t="str">
+        <v>0.17293233082706766</v>
+      </c>
+      <c r="O139" s="7">
         <f t="shared" si="95"/>
-        <v>null</v>
+        <v>-1.1488613886124579</v>
       </c>
       <c r="P139" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Q139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S139" s="7" t="e">
+        <v>38</v>
+      </c>
+      <c r="R139" s="1">
+        <v>80</v>
+      </c>
+      <c r="S139" s="7">
         <f t="shared" si="96"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T139" s="7" t="e">
+        <v>0.54887218045112784</v>
+      </c>
+      <c r="T139" s="7">
         <f t="shared" si="97"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="W139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X139" s="7" t="str">
+        <v>0.46415316846520493</v>
+      </c>
+      <c r="U139" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V139" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W139" s="1">
+        <v>93</v>
+      </c>
+      <c r="X139" s="7">
         <f t="shared" si="98"/>
-        <v>null</v>
-      </c>
-      <c r="Y139" s="7" t="str">
+        <v>0.64661654135338342</v>
+      </c>
+      <c r="Y139" s="7">
         <f t="shared" si="99"/>
-        <v>null</v>
+        <v>0.88353695330539728</v>
       </c>
       <c r="Z139" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="AA139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC139" s="7" t="e">
+        <v>38</v>
+      </c>
+      <c r="AB139" s="1">
+        <v>82</v>
+      </c>
+      <c r="AC139" s="7">
         <f t="shared" si="100"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AD139" s="7" t="e">
+        <v>0.56390977443609025</v>
+      </c>
+      <c r="AD139" s="7">
         <f t="shared" si="101"/>
-        <v>#VALUE!</v>
+        <v>0.52867375074831147</v>
+      </c>
+      <c r="AE139" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF139" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="AG139" s="1" t="s">
         <v>36</v>
@@ -72746,45 +72796,49 @@
       <c r="AK139" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL139" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM139" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN139" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO139" s="7" t="s">
-        <v>36</v>
+      <c r="AL139" s="7">
+        <f t="shared" si="104"/>
+        <v>0.17293233082706766</v>
+      </c>
+      <c r="AM139" s="7">
+        <f t="shared" si="105"/>
+        <v>0.48308270676691722</v>
+      </c>
+      <c r="AN139" s="7">
+        <f t="shared" si="106"/>
+        <v>0.64661654135338342</v>
+      </c>
+      <c r="AO139" s="7">
+        <f t="shared" si="107"/>
+        <v>0.47368421052631576</v>
       </c>
       <c r="AP139" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AR139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AS139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW139" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="AQ139" s="1">
+        <v>65.612244897959187</v>
+      </c>
+      <c r="AR139" s="1">
+        <v>30.997860360656755</v>
+      </c>
+      <c r="AS139" s="1">
+        <v>7</v>
+      </c>
+      <c r="AT139" s="1">
+        <v>140</v>
+      </c>
+      <c r="AU139" s="1">
+        <v>44</v>
+      </c>
+      <c r="AV139" s="1">
+        <v>86.5</v>
+      </c>
+      <c r="AW139" s="1">
+        <v>62</v>
       </c>
       <c r="AX139" s="10">
         <f t="shared" si="79"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AY139" s="1">
         <v>0</v>
@@ -72835,7 +72889,7 @@
         <v>0</v>
       </c>
       <c r="BO139" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP139" s="1">
         <v>0</v>
@@ -72862,67 +72916,67 @@
         <v>0</v>
       </c>
       <c r="BX139" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY139" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD139" s="1">
         <v>1</v>
       </c>
-      <c r="BY139" s="1">
-        <v>0</v>
-      </c>
-      <c r="BZ139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CA139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CB139" s="1">
+      <c r="CE139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ139" s="1">
         <v>1</v>
       </c>
-      <c r="CC139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CD139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CE139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CF139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CG139" s="1">
+      <c r="CK139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO139" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP139" s="1">
         <v>1</v>
       </c>
-      <c r="CH139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CI139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CJ139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CK139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CM139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CN139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CO139" s="1">
-        <v>0</v>
-      </c>
-      <c r="CP139" s="1">
-        <v>0</v>
-      </c>
       <c r="CQ139" s="1">
         <v>0</v>
       </c>
       <c r="CR139" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CS139" s="1">
         <v>0</v>
@@ -72991,7 +73045,7 @@
         <v>0</v>
       </c>
       <c r="DO139" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DP139" s="1">
         <v>0</v>
@@ -73024,25 +73078,25 @@
         <v>0</v>
       </c>
       <c r="DZ139" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA139" s="1">
+        <v>0</v>
+      </c>
+      <c r="EB139" s="1">
+        <v>0</v>
+      </c>
+      <c r="EC139" s="1">
+        <v>0</v>
+      </c>
+      <c r="ED139" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE139" s="1">
+        <v>0</v>
+      </c>
+      <c r="EF139" s="1">
         <v>1</v>
-      </c>
-      <c r="EA139" s="1">
-        <v>0</v>
-      </c>
-      <c r="EB139" s="1">
-        <v>0</v>
-      </c>
-      <c r="EC139" s="1">
-        <v>0</v>
-      </c>
-      <c r="ED139" s="1">
-        <v>0</v>
-      </c>
-      <c r="EE139" s="1">
-        <v>0</v>
-      </c>
-      <c r="EF139" s="1">
-        <v>0</v>
       </c>
       <c r="EG139" s="1">
         <v>0</v>
@@ -73063,7 +73117,7 @@
         <v>0</v>
       </c>
       <c r="EM139" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EN139" s="1">
         <v>0</v>
@@ -73105,7 +73159,7 @@
         <v>0</v>
       </c>
       <c r="FA139" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FB139" s="1">
         <v>0</v>
@@ -73117,7 +73171,7 @@
         <v>0</v>
       </c>
       <c r="FE139" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FF139" s="1">
         <v>0</v>
@@ -73137,109 +73191,109 @@
     </row>
     <row r="140" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C140" s="6" t="s">
         <v>324</v>
       </c>
       <c r="D140" s="1">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E140" s="1">
         <v>75</v>
       </c>
       <c r="F140" s="7">
         <f t="shared" si="68"/>
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="G140" s="1">
-        <v>2.2999999999999998</v>
+        <v>2.71</v>
       </c>
       <c r="H140" s="1">
-        <v>7.9</v>
+        <v>6.6</v>
       </c>
       <c r="I140" s="1">
-        <v>98</v>
+        <v>12680</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L140" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M140" s="1">
-        <v>30</v>
-      </c>
-      <c r="N140" s="7">
+        <v>36</v>
+      </c>
+      <c r="M140" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N140" s="7" t="str">
         <f t="shared" si="94"/>
-        <v>0.17293233082706766</v>
-      </c>
-      <c r="O140" s="7">
+        <v>null</v>
+      </c>
+      <c r="O140" s="7" t="str">
         <f t="shared" si="95"/>
-        <v>-1.1488613886124579</v>
+        <v>null</v>
       </c>
       <c r="P140" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q140" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R140" s="1">
-        <v>80</v>
-      </c>
-      <c r="S140" s="7">
+      <c r="R140" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S140" s="7" t="str">
         <f t="shared" si="96"/>
-        <v>0.54887218045112784</v>
-      </c>
-      <c r="T140" s="7">
+        <v>null</v>
+      </c>
+      <c r="T140" s="7" t="str">
         <f t="shared" si="97"/>
-        <v>0.46415316846520493</v>
+        <v>null</v>
       </c>
       <c r="U140" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="V140" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="W140" s="1">
-        <v>93</v>
-      </c>
-      <c r="X140" s="7">
+        <v>36</v>
+      </c>
+      <c r="W140" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X140" s="7" t="str">
         <f t="shared" si="98"/>
-        <v>0.64661654135338342</v>
-      </c>
-      <c r="Y140" s="7">
+        <v>null</v>
+      </c>
+      <c r="Y140" s="7" t="str">
         <f t="shared" si="99"/>
-        <v>0.88353695330539728</v>
+        <v>null</v>
       </c>
       <c r="Z140" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA140" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB140" s="1">
-        <v>82</v>
-      </c>
-      <c r="AC140" s="7">
+      <c r="AB140" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC140" s="7" t="str">
         <f t="shared" si="100"/>
-        <v>0.56390977443609025</v>
-      </c>
-      <c r="AD140" s="7">
+        <v>null</v>
+      </c>
+      <c r="AD140" s="7" t="str">
         <f t="shared" si="101"/>
-        <v>0.52867375074831147</v>
+        <v>null</v>
       </c>
       <c r="AE140" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AF140" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AG140" s="1" t="s">
         <v>36</v>
@@ -73253,54 +73307,50 @@
         <v>null</v>
       </c>
       <c r="AJ140" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="AK140" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL140" s="7">
-        <f t="shared" si="104"/>
-        <v>0.17293233082706766</v>
-      </c>
-      <c r="AM140" s="7">
-        <f t="shared" si="105"/>
-        <v>0.48308270676691722</v>
-      </c>
-      <c r="AN140" s="7">
-        <f t="shared" si="106"/>
-        <v>0.64661654135338342</v>
-      </c>
-      <c r="AO140" s="7">
-        <f t="shared" si="107"/>
-        <v>0.47368421052631576</v>
+        <v>38</v>
+      </c>
+      <c r="AL140" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM140" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN140" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO140" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="AP140" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ140" s="1">
-        <v>65.612244897959187</v>
-      </c>
-      <c r="AR140" s="1">
-        <v>30.997860360656755</v>
-      </c>
-      <c r="AS140" s="1">
-        <v>7</v>
-      </c>
-      <c r="AT140" s="1">
-        <v>140</v>
-      </c>
-      <c r="AU140" s="1">
-        <v>44</v>
-      </c>
-      <c r="AV140" s="1">
-        <v>86.5</v>
-      </c>
-      <c r="AW140" s="1">
-        <v>62</v>
+        <v>39</v>
+      </c>
+      <c r="AQ140" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR140" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS140" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT140" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU140" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV140" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW140" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="AX140" s="10">
         <f t="shared" si="79"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="AY140" s="1">
         <v>0</v>
@@ -73351,35 +73401,35 @@
         <v>0</v>
       </c>
       <c r="BO140" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP140" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ140" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR140" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS140" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT140" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU140" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV140" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW140" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX140" s="1">
         <v>1</v>
       </c>
-      <c r="BP140" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ140" s="1">
-        <v>0</v>
-      </c>
-      <c r="BR140" s="1">
-        <v>0</v>
-      </c>
-      <c r="BS140" s="1">
-        <v>0</v>
-      </c>
-      <c r="BT140" s="1">
-        <v>0</v>
-      </c>
-      <c r="BU140" s="1">
-        <v>0</v>
-      </c>
-      <c r="BV140" s="1">
-        <v>0</v>
-      </c>
-      <c r="BW140" s="1">
-        <v>0</v>
-      </c>
-      <c r="BX140" s="1">
-        <v>0</v>
-      </c>
       <c r="BY140" s="1">
         <v>0</v>
       </c>
@@ -73390,137 +73440,137 @@
         <v>0</v>
       </c>
       <c r="CB140" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC140" s="1">
         <v>0</v>
       </c>
       <c r="CD140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY140" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DR140" s="1">
+        <v>0</v>
+      </c>
+      <c r="DS140" s="1">
         <v>1</v>
       </c>
-      <c r="CE140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CF140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CG140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CH140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CI140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CJ140" s="1">
-        <v>1</v>
-      </c>
-      <c r="CK140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CM140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CN140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CO140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CP140" s="1">
-        <v>1</v>
-      </c>
-      <c r="CQ140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CR140" s="1">
-        <v>1</v>
-      </c>
-      <c r="CS140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CT140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CU140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CV140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CW140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CX140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CY140" s="1">
-        <v>0</v>
-      </c>
-      <c r="CZ140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DA140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DB140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DC140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DD140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DE140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DF140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DG140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DH140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DI140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DJ140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DK140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DL140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DM140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DN140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DO140" s="1">
-        <v>1</v>
-      </c>
-      <c r="DP140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DQ140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DR140" s="1">
-        <v>0</v>
-      </c>
-      <c r="DS140" s="1">
-        <v>0</v>
-      </c>
       <c r="DT140" s="1">
         <v>0</v>
       </c>
@@ -73558,7 +73608,7 @@
         <v>0</v>
       </c>
       <c r="EF140" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EG140" s="1">
         <v>0</v>
@@ -73579,73 +73629,73 @@
         <v>0</v>
       </c>
       <c r="EM140" s="1">
+        <v>0</v>
+      </c>
+      <c r="EN140" s="1">
+        <v>0</v>
+      </c>
+      <c r="EO140" s="1">
+        <v>0</v>
+      </c>
+      <c r="EP140" s="1">
+        <v>0</v>
+      </c>
+      <c r="EQ140" s="1">
+        <v>0</v>
+      </c>
+      <c r="ER140" s="1">
+        <v>0</v>
+      </c>
+      <c r="ES140" s="1">
+        <v>0</v>
+      </c>
+      <c r="ET140" s="1">
+        <v>0</v>
+      </c>
+      <c r="EU140" s="1">
+        <v>0</v>
+      </c>
+      <c r="EV140" s="1">
+        <v>0</v>
+      </c>
+      <c r="EW140" s="1">
+        <v>0</v>
+      </c>
+      <c r="EX140" s="1">
+        <v>0</v>
+      </c>
+      <c r="EY140" s="1">
+        <v>0</v>
+      </c>
+      <c r="EZ140" s="1">
+        <v>0</v>
+      </c>
+      <c r="FA140" s="1">
+        <v>0</v>
+      </c>
+      <c r="FB140" s="1">
+        <v>0</v>
+      </c>
+      <c r="FC140" s="1">
+        <v>0</v>
+      </c>
+      <c r="FD140" s="1">
+        <v>0</v>
+      </c>
+      <c r="FE140" s="1">
+        <v>0</v>
+      </c>
+      <c r="FF140" s="1">
+        <v>0</v>
+      </c>
+      <c r="FG140" s="1">
+        <v>0</v>
+      </c>
+      <c r="FH140" s="1">
+        <v>0</v>
+      </c>
+      <c r="FI140" s="1">
         <v>1</v>
-      </c>
-      <c r="EN140" s="1">
-        <v>0</v>
-      </c>
-      <c r="EO140" s="1">
-        <v>0</v>
-      </c>
-      <c r="EP140" s="1">
-        <v>0</v>
-      </c>
-      <c r="EQ140" s="1">
-        <v>0</v>
-      </c>
-      <c r="ER140" s="1">
-        <v>1</v>
-      </c>
-      <c r="ES140" s="1">
-        <v>0</v>
-      </c>
-      <c r="ET140" s="1">
-        <v>0</v>
-      </c>
-      <c r="EU140" s="1">
-        <v>0</v>
-      </c>
-      <c r="EV140" s="1">
-        <v>0</v>
-      </c>
-      <c r="EW140" s="1">
-        <v>0</v>
-      </c>
-      <c r="EX140" s="1">
-        <v>0</v>
-      </c>
-      <c r="EY140" s="1">
-        <v>0</v>
-      </c>
-      <c r="EZ140" s="1">
-        <v>0</v>
-      </c>
-      <c r="FA140" s="1">
-        <v>1</v>
-      </c>
-      <c r="FB140" s="1">
-        <v>0</v>
-      </c>
-      <c r="FC140" s="1">
-        <v>0</v>
-      </c>
-      <c r="FD140" s="1">
-        <v>0</v>
-      </c>
-      <c r="FE140" s="1">
-        <v>0</v>
-      </c>
-      <c r="FF140" s="1">
-        <v>0</v>
-      </c>
-      <c r="FG140" s="1">
-        <v>0</v>
-      </c>
-      <c r="FH140" s="1">
-        <v>0</v>
-      </c>
-      <c r="FI140" s="1">
-        <v>0</v>
       </c>
       <c r="FJ140" s="1">
         <v>0</v>
@@ -73653,172 +73703,176 @@
     </row>
     <row r="141" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>324</v>
       </c>
       <c r="D141" s="1">
-        <v>160</v>
+        <v>75</v>
       </c>
       <c r="E141" s="1">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F141" s="7">
         <f t="shared" si="68"/>
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="G141" s="1">
-        <v>2.71</v>
+        <v>2.91</v>
       </c>
       <c r="H141" s="1">
-        <v>6.6</v>
+        <v>7.3</v>
       </c>
       <c r="I141" s="1">
-        <v>12680</v>
+        <v>1585</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N141" s="7" t="str">
-        <f t="shared" si="94"/>
-        <v>null</v>
-      </c>
-      <c r="O141" s="7" t="str">
-        <f t="shared" si="95"/>
-        <v>null</v>
+        <v>147</v>
+      </c>
+      <c r="M141" s="1">
+        <v>34</v>
+      </c>
+      <c r="N141" s="7">
+        <f t="shared" ref="N141:N152" si="108">IF(M141="null", "null", (M141-$AS141)/($AT141-$AS141))</f>
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="O141" s="7">
+        <f t="shared" ref="O141:O152" si="109">IF(M141="null","null",(M141-$AQ141)/$AR141)</f>
+        <v>-0.8024300452416393</v>
       </c>
       <c r="P141" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q141" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q141" s="1" t="s">
+      <c r="R141" s="1">
+        <v>41</v>
+      </c>
+      <c r="S141" s="7">
+        <f t="shared" ref="S141:S152" si="110">IF(R141="null", "null", (R141-$AS141)/($AT141-$AS141))</f>
+        <v>0.38636363636363635</v>
+      </c>
+      <c r="T141" s="7">
+        <f t="shared" ref="T141:T152" si="111">IF(R141="null","null",(R141-$AQ141)/$AR141)</f>
+        <v>-0.10712051574827706</v>
+      </c>
+      <c r="U141" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S141" s="7" t="str">
-        <f t="shared" si="96"/>
-        <v>null</v>
-      </c>
-      <c r="T141" s="7" t="str">
-        <f t="shared" si="97"/>
-        <v>null</v>
-      </c>
-      <c r="U141" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="V141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X141" s="7" t="str">
-        <f t="shared" si="98"/>
-        <v>null</v>
-      </c>
-      <c r="Y141" s="7" t="str">
-        <f t="shared" si="99"/>
-        <v>null</v>
+        <v>39</v>
+      </c>
+      <c r="W141" s="1">
+        <v>27</v>
+      </c>
+      <c r="X141" s="7">
+        <f t="shared" ref="X141:X152" si="112">IF(W141="null", "null", (W141-$AS141)/($AT141-$AS141))</f>
+        <v>6.8181818181818177E-2</v>
+      </c>
+      <c r="Y141" s="7">
+        <f t="shared" ref="Y141:Y152" si="113">IF(W141="null","null",(W141-$AQ141)/$AR141)</f>
+        <v>-1.4977395747350015</v>
       </c>
       <c r="Z141" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA141" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC141" s="7" t="str">
-        <f t="shared" si="100"/>
+      <c r="AB141" s="1">
+        <v>61</v>
+      </c>
+      <c r="AC141" s="7">
+        <f t="shared" ref="AC141:AC152" si="114">IF(AB141="null", "null", (AB141-$AS141)/($AT141-$AS141))</f>
+        <v>0.84090909090909094</v>
+      </c>
+      <c r="AD141" s="7">
+        <f t="shared" ref="AD141:AD152" si="115">IF(AB141="null","null",(AB141-$AQ141)/$AR141)</f>
+        <v>1.8794781399470437</v>
+      </c>
+      <c r="AE141" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF141" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG141" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH141" s="7" t="str">
+        <f t="shared" ref="AH141:AH152" si="116">IF(AG141="null", "null", (AG141-$AS141)/($AT141-$AS141))</f>
         <v>null</v>
       </c>
-      <c r="AD141" s="7" t="str">
-        <f t="shared" si="101"/>
+      <c r="AI141" s="7" t="str">
+        <f t="shared" ref="AI141:AI152" si="117">IF(AG141="null","null",(AG141-$AQ141)/$AR141)</f>
         <v>null</v>
       </c>
-      <c r="AE141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH141" s="7" t="str">
-        <f t="shared" si="102"/>
-        <v>null</v>
-      </c>
-      <c r="AI141" s="7" t="str">
-        <f t="shared" si="103"/>
-        <v>null</v>
-      </c>
       <c r="AJ141" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="AK141" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL141" s="7">
+        <f t="shared" ref="AL141" si="118">MIN(N141,S141,X141,AH141,AC141)</f>
+        <v>6.8181818181818177E-2</v>
+      </c>
+      <c r="AM141" s="7">
+        <f t="shared" ref="AM141" si="119">AVERAGE(N141,S141,X141,AH141,AC141)</f>
+        <v>0.38068181818181823</v>
+      </c>
+      <c r="AN141" s="7">
+        <f t="shared" ref="AN141" si="120">MAX(N141,S141,X141,AH141,AC141)</f>
+        <v>0.84090909090909094</v>
+      </c>
+      <c r="AO141" s="7">
+        <f t="shared" ref="AO141" si="121">AN141-AL141</f>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="AP141" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AL141" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM141" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN141" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO141" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP141" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AR141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AS141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW141" s="1" t="s">
-        <v>36</v>
+      <c r="AQ141" s="1">
+        <v>42.078431372549019</v>
+      </c>
+      <c r="AR141" s="1">
+        <v>10.067458740426806</v>
+      </c>
+      <c r="AS141" s="1">
+        <v>24</v>
+      </c>
+      <c r="AT141" s="1">
+        <v>68</v>
+      </c>
+      <c r="AU141" s="1">
+        <v>36</v>
+      </c>
+      <c r="AV141" s="1">
+        <v>48</v>
+      </c>
+      <c r="AW141" s="1">
+        <v>41</v>
       </c>
       <c r="AX141" s="10">
         <f t="shared" si="79"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AY141" s="1">
         <v>0</v>
       </c>
       <c r="AZ141" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA141" s="1">
         <v>0</v>
@@ -73842,7 +73896,7 @@
         <v>0</v>
       </c>
       <c r="BH141" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI141" s="1">
         <v>0</v>
@@ -73890,113 +73944,113 @@
         <v>0</v>
       </c>
       <c r="BX141" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY141" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CS141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY141" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ141" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA141" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB141" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC141" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD141" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE141" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF141" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG141" s="1">
         <v>1</v>
       </c>
-      <c r="BY141" s="1">
-        <v>0</v>
-      </c>
-      <c r="BZ141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CA141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CB141" s="1">
-        <v>1</v>
-      </c>
-      <c r="CC141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CD141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CE141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CF141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CG141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CH141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CI141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CJ141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CK141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CM141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CN141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CO141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CP141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CQ141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CR141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CS141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CT141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CU141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CV141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CW141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CX141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CY141" s="1">
-        <v>0</v>
-      </c>
-      <c r="CZ141" s="1">
-        <v>0</v>
-      </c>
-      <c r="DA141" s="1">
-        <v>0</v>
-      </c>
-      <c r="DB141" s="1">
-        <v>0</v>
-      </c>
-      <c r="DC141" s="1">
-        <v>0</v>
-      </c>
-      <c r="DD141" s="1">
-        <v>0</v>
-      </c>
-      <c r="DE141" s="1">
-        <v>0</v>
-      </c>
-      <c r="DF141" s="1">
-        <v>0</v>
-      </c>
-      <c r="DG141" s="1">
-        <v>0</v>
-      </c>
       <c r="DH141" s="1">
         <v>0</v>
       </c>
@@ -74031,7 +74085,7 @@
         <v>0</v>
       </c>
       <c r="DS141" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DT141" s="1">
         <v>0</v>
@@ -74082,7 +74136,7 @@
         <v>0</v>
       </c>
       <c r="EJ141" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EK141" s="1">
         <v>0</v>
@@ -74165,7 +74219,7 @@
     </row>
     <row r="142" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>329</v>
@@ -74174,94 +74228,94 @@
         <v>324</v>
       </c>
       <c r="D142" s="1">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E142" s="1">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F142" s="7">
         <f t="shared" si="68"/>
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="G142" s="1">
-        <v>2.91</v>
+        <v>1.95</v>
       </c>
       <c r="H142" s="1">
-        <v>7.3</v>
+        <v>8.1</v>
       </c>
       <c r="I142" s="1">
-        <v>1585</v>
+        <v>170</v>
       </c>
       <c r="J142" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>37</v>
+        <v>147</v>
       </c>
       <c r="L142" s="1" t="s">
         <v>147</v>
       </c>
       <c r="M142" s="1">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="N142" s="7">
-        <f t="shared" ref="N142:N153" si="108">IF(M142="null", "null", (M142-$AS142)/($AT142-$AS142))</f>
-        <v>0.22727272727272727</v>
+        <f t="shared" si="108"/>
+        <v>0.52173913043478259</v>
       </c>
       <c r="O142" s="7">
-        <f t="shared" ref="O142:O153" si="109">IF(M142="null","null",(M142-$AQ142)/$AR142)</f>
-        <v>-0.8024300452416393</v>
+        <f t="shared" si="109"/>
+        <v>-0.88953963318354645</v>
       </c>
       <c r="P142" s="1" t="s">
         <v>38</v>
       </c>
       <c r="Q142" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R142" s="1">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="S142" s="7">
-        <f t="shared" ref="S142:S153" si="110">IF(R142="null", "null", (R142-$AS142)/($AT142-$AS142))</f>
-        <v>0.38636363636363635</v>
+        <f t="shared" si="110"/>
+        <v>0.65217391304347827</v>
       </c>
       <c r="T142" s="7">
-        <f t="shared" ref="T142:T153" si="111">IF(R142="null","null",(R142-$AQ142)/$AR142)</f>
-        <v>-0.10712051574827706</v>
+        <f t="shared" si="111"/>
+        <v>-0.21744302144486663</v>
       </c>
       <c r="U142" s="1" t="s">
         <v>38</v>
       </c>
       <c r="V142" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W142" s="1">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="X142" s="7">
-        <f t="shared" ref="X142:X153" si="112">IF(W142="null", "null", (W142-$AS142)/($AT142-$AS142))</f>
-        <v>6.8181818181818177E-2</v>
+        <f t="shared" si="112"/>
+        <v>0.60869565217391308</v>
       </c>
       <c r="Y142" s="7">
-        <f t="shared" ref="Y142:Y153" si="113">IF(W142="null","null",(W142-$AQ142)/$AR142)</f>
-        <v>-1.4977395747350015</v>
+        <f t="shared" si="113"/>
+        <v>-0.4414752253577599</v>
       </c>
       <c r="Z142" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA142" s="1" t="s">
         <v>38</v>
       </c>
       <c r="AB142" s="1">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="AC142" s="7">
-        <f t="shared" ref="AC142:AC153" si="114">IF(AB142="null", "null", (AB142-$AS142)/($AT142-$AS142))</f>
-        <v>0.84090909090909094</v>
+        <f t="shared" si="114"/>
+        <v>0.69565217391304346</v>
       </c>
       <c r="AD142" s="7">
-        <f t="shared" ref="AD142:AD153" si="115">IF(AB142="null","null",(AB142-$AQ142)/$AR142)</f>
-        <v>1.8794781399470437</v>
+        <f t="shared" si="115"/>
+        <v>6.5891824680266477E-3</v>
       </c>
       <c r="AE142" s="1" t="s">
         <v>38</v>
@@ -74273,11 +74327,11 @@
         <v>36</v>
       </c>
       <c r="AH142" s="7" t="str">
-        <f t="shared" ref="AH142:AH153" si="116">IF(AG142="null", "null", (AG142-$AS142)/($AT142-$AS142))</f>
+        <f t="shared" si="116"/>
         <v>null</v>
       </c>
       <c r="AI142" s="7" t="str">
-        <f t="shared" ref="AI142:AI153" si="117">IF(AG142="null","null",(AG142-$AQ142)/$AR142)</f>
+        <f t="shared" si="117"/>
         <v>null</v>
       </c>
       <c r="AJ142" s="1" t="s">
@@ -74287,172 +74341,172 @@
         <v>36</v>
       </c>
       <c r="AL142" s="7">
-        <f t="shared" ref="AL142" si="118">MIN(N142,S142,X142,AH142,AC142)</f>
-        <v>6.8181818181818177E-2</v>
+        <f t="shared" ref="AL142:AL152" si="122">MIN(N142,S142,X142,AH142,AC142)</f>
+        <v>0.52173913043478259</v>
       </c>
       <c r="AM142" s="7">
-        <f t="shared" ref="AM142" si="119">AVERAGE(N142,S142,X142,AH142,AC142)</f>
-        <v>0.38068181818181823</v>
+        <f t="shared" ref="AM142:AM152" si="123">AVERAGE(N142,S142,X142,AH142,AC142)</f>
+        <v>0.61956521739130432</v>
       </c>
       <c r="AN142" s="7">
-        <f t="shared" ref="AN142" si="120">MAX(N142,S142,X142,AH142,AC142)</f>
-        <v>0.84090909090909094</v>
+        <f t="shared" ref="AN142:AN152" si="124">MAX(N142,S142,X142,AH142,AC142)</f>
+        <v>0.69565217391304346</v>
       </c>
       <c r="AO142" s="7">
-        <f t="shared" ref="AO142" si="121">AN142-AL142</f>
-        <v>0.77272727272727271</v>
+        <f t="shared" ref="AO142:AO152" si="125">AN142-AL142</f>
+        <v>0.17391304347826086</v>
       </c>
       <c r="AP142" s="1" t="s">
         <v>38</v>
       </c>
       <c r="AQ142" s="1">
-        <v>42.078431372549019</v>
+        <v>88.941176470588232</v>
       </c>
       <c r="AR142" s="1">
-        <v>10.067458740426806</v>
+        <v>8.9272879749807164</v>
       </c>
       <c r="AS142" s="1">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="AT142" s="1">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="AU142" s="1">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="AV142" s="1">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="AW142" s="1">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="AX142" s="10">
         <f t="shared" si="79"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AY142" s="1">
         <v>0</v>
       </c>
       <c r="AZ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY142" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD142" s="1">
         <v>1</v>
       </c>
-      <c r="BA142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BB142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BF142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BG142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH142" s="1">
+      <c r="CE142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CL142" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM142" s="1">
         <v>1</v>
       </c>
-      <c r="BI142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BJ142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BK142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BL142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BM142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BO142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BR142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BS142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BT142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BU142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BV142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BW142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BX142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BY142" s="1">
-        <v>0</v>
-      </c>
-      <c r="BZ142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CA142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CB142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CC142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CD142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CE142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CF142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CG142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CH142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CI142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CJ142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CK142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL142" s="1">
-        <v>0</v>
-      </c>
-      <c r="CM142" s="1">
-        <v>0</v>
-      </c>
       <c r="CN142" s="1">
         <v>0</v>
       </c>
@@ -74511,32 +74565,32 @@
         <v>0</v>
       </c>
       <c r="DG142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DI142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DK142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DL142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DN142" s="1">
+        <v>0</v>
+      </c>
+      <c r="DO142" s="1">
         <v>1</v>
       </c>
-      <c r="DH142" s="1">
-        <v>0</v>
-      </c>
-      <c r="DI142" s="1">
-        <v>0</v>
-      </c>
-      <c r="DJ142" s="1">
-        <v>0</v>
-      </c>
-      <c r="DK142" s="1">
-        <v>0</v>
-      </c>
-      <c r="DL142" s="1">
-        <v>0</v>
-      </c>
-      <c r="DM142" s="1">
-        <v>0</v>
-      </c>
-      <c r="DN142" s="1">
-        <v>0</v>
-      </c>
-      <c r="DO142" s="1">
-        <v>0</v>
-      </c>
       <c r="DP142" s="1">
         <v>0</v>
       </c>
@@ -74598,7 +74652,7 @@
         <v>0</v>
       </c>
       <c r="EJ142" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EK142" s="1">
         <v>0</v>
@@ -74622,7 +74676,7 @@
         <v>0</v>
       </c>
       <c r="ER142" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ES142" s="1">
         <v>0</v>
@@ -74667,13 +74721,13 @@
         <v>0</v>
       </c>
       <c r="FG142" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FH142" s="1">
         <v>0</v>
       </c>
       <c r="FI142" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FJ142" s="1">
         <v>0</v>
@@ -74681,7 +74735,7 @@
     </row>
     <row r="143" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>324</v>
@@ -74731,19 +74785,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AL143" s="7" t="e">
-        <f t="shared" ref="AL143:AL153" si="122">MIN(N143,S143,X143,AH143,AC143)</f>
+        <f t="shared" si="122"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AM143" s="7" t="e">
-        <f t="shared" ref="AM143:AM153" si="123">AVERAGE(N143,S143,X143,AH143,AC143)</f>
+        <f t="shared" si="123"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AN143" s="7" t="e">
-        <f t="shared" ref="AN143:AN153" si="124">MAX(N143,S143,X143,AH143,AC143)</f>
+        <f t="shared" si="124"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AO143" s="7" t="e">
-        <f t="shared" ref="AO143:AO153" si="125">AN143-AL143</f>
+        <f t="shared" si="125"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AX143" s="10">
@@ -75101,7 +75155,7 @@
     </row>
     <row r="144" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C144" s="6" t="s">
         <v>324</v>
@@ -75521,7 +75575,7 @@
     </row>
     <row r="145" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C145" s="6" t="s">
         <v>324</v>
@@ -75941,7 +75995,7 @@
     </row>
     <row r="146" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C146" s="6" t="s">
         <v>324</v>
@@ -76361,7 +76415,7 @@
     </row>
     <row r="147" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>324</v>
@@ -76781,7 +76835,7 @@
     </row>
     <row r="148" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C148" s="6" t="s">
         <v>324</v>
@@ -77201,7 +77255,7 @@
     </row>
     <row r="149" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>324</v>
@@ -77621,7 +77675,7 @@
     </row>
     <row r="150" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>324</v>
@@ -78041,7 +78095,7 @@
     </row>
     <row r="151" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C151" s="6" t="s">
         <v>324</v>
@@ -78461,7 +78515,7 @@
     </row>
     <row r="152" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>324</v>
@@ -78876,426 +78930,6 @@
         <v>0</v>
       </c>
       <c r="FJ152" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:166" x14ac:dyDescent="0.25">
-      <c r="A153" s="1">
-        <v>142</v>
-      </c>
-      <c r="C153" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="F153" s="7">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="N153" s="7" t="e">
-        <f t="shared" si="108"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O153" s="7" t="e">
-        <f t="shared" si="109"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S153" s="7" t="e">
-        <f t="shared" si="110"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T153" s="7" t="e">
-        <f t="shared" si="111"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X153" s="7" t="e">
-        <f t="shared" si="112"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y153" s="7" t="e">
-        <f t="shared" si="113"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC153" s="7" t="e">
-        <f t="shared" si="114"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD153" s="7" t="e">
-        <f t="shared" si="115"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH153" s="7" t="e">
-        <f t="shared" si="116"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI153" s="7" t="e">
-        <f t="shared" si="117"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AL153" s="7" t="e">
-        <f t="shared" si="122"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AM153" s="7" t="e">
-        <f t="shared" si="123"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AN153" s="7" t="e">
-        <f t="shared" si="124"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AO153" s="7" t="e">
-        <f t="shared" si="125"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AX153" s="10">
-        <f t="shared" si="79"/>
-        <v>0</v>
-      </c>
-      <c r="AY153" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BA153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BB153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BF153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BG153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BI153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BJ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BK153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BL153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BM153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BO153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BR153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BS153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BT153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BU153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BV153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BW153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BX153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BY153" s="1">
-        <v>0</v>
-      </c>
-      <c r="BZ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CA153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CB153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CC153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CD153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CE153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CF153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CG153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CH153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CI153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CJ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CK153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CM153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CN153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CO153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CP153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CQ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CR153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CS153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CT153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CU153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CV153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CW153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CX153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CY153" s="1">
-        <v>0</v>
-      </c>
-      <c r="CZ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DA153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DB153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DC153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DD153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DE153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DF153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DG153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DH153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DI153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DJ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DK153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DL153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DM153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DN153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DO153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DP153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DQ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DR153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DS153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DT153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DU153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DV153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DW153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DX153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DY153" s="1">
-        <v>0</v>
-      </c>
-      <c r="DZ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EA153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EB153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EC153" s="1">
-        <v>0</v>
-      </c>
-      <c r="ED153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EE153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EF153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EG153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EH153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EI153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EJ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EK153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EL153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EM153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EN153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EO153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EP153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EQ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="ER153" s="1">
-        <v>0</v>
-      </c>
-      <c r="ES153" s="1">
-        <v>0</v>
-      </c>
-      <c r="ET153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EU153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EV153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EW153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EX153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EY153" s="1">
-        <v>0</v>
-      </c>
-      <c r="EZ153" s="1">
-        <v>0</v>
-      </c>
-      <c r="FA153" s="1">
-        <v>0</v>
-      </c>
-      <c r="FB153" s="1">
-        <v>0</v>
-      </c>
-      <c r="FC153" s="1">
-        <v>0</v>
-      </c>
-      <c r="FD153" s="1">
-        <v>0</v>
-      </c>
-      <c r="FE153" s="1">
-        <v>0</v>
-      </c>
-      <c r="FF153" s="1">
-        <v>0</v>
-      </c>
-      <c r="FG153" s="1">
-        <v>0</v>
-      </c>
-      <c r="FH153" s="1">
-        <v>0</v>
-      </c>
-      <c r="FI153" s="1">
-        <v>0</v>
-      </c>
-      <c r="FJ153" s="1">
         <v>0</v>
       </c>
     </row>
@@ -79310,9 +78944,9 @@
   <dimension ref="A1:BG117"/>
   <sheetViews>
     <sheetView topLeftCell="A88" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection activeCell="A58" sqref="A58"/>
-      <selection pane="topRight" activeCell="B107" sqref="B107:H107"/>
+      <selection pane="topRight" activeCell="B108" sqref="B108:H108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -98464,7 +98098,7 @@
     </row>
     <row r="106" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B106">
         <f t="shared" si="28"/>
@@ -98644,7 +98278,7 @@
     </row>
     <row r="107" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B107">
         <f t="shared" ref="B107:B117" si="35">AVERAGE(I107:BG107)</f>
@@ -98829,33 +98463,189 @@
       </c>
     </row>
     <row r="108" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B108" t="e">
+      <c r="A108" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B108">
         <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C108" t="e">
+        <v>88.941176470588232</v>
+      </c>
+      <c r="C108">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>8.9272879749807164</v>
       </c>
       <c r="D108">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="E108">
         <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="F108" t="e">
+        <v>103</v>
+      </c>
+      <c r="F108">
         <f t="shared" si="39"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="G108" t="e">
+        <v>85</v>
+      </c>
+      <c r="G108">
         <f t="shared" si="40"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H108" t="e">
+        <v>95</v>
+      </c>
+      <c r="H108">
         <f t="shared" si="41"/>
-        <v>#NUM!</v>
+        <v>90</v>
+      </c>
+      <c r="I108">
+        <v>96</v>
+      </c>
+      <c r="J108">
+        <v>73</v>
+      </c>
+      <c r="K108">
+        <v>93</v>
+      </c>
+      <c r="L108">
+        <v>92</v>
+      </c>
+      <c r="M108">
+        <v>85</v>
+      </c>
+      <c r="N108">
+        <v>89</v>
+      </c>
+      <c r="O108">
+        <v>100</v>
+      </c>
+      <c r="P108">
+        <v>92</v>
+      </c>
+      <c r="Q108">
+        <v>81</v>
+      </c>
+      <c r="R108">
+        <v>95</v>
+      </c>
+      <c r="S108">
+        <v>93</v>
+      </c>
+      <c r="T108">
+        <v>88</v>
+      </c>
+      <c r="U108">
+        <v>84</v>
+      </c>
+      <c r="V108">
+        <v>101</v>
+      </c>
+      <c r="W108">
+        <v>92</v>
+      </c>
+      <c r="X108">
+        <v>88</v>
+      </c>
+      <c r="Y108">
+        <v>82</v>
+      </c>
+      <c r="Z108">
+        <v>89</v>
+      </c>
+      <c r="AA108">
+        <v>97</v>
+      </c>
+      <c r="AB108">
+        <v>93</v>
+      </c>
+      <c r="AC108">
+        <v>97</v>
+      </c>
+      <c r="AD108">
+        <v>83</v>
+      </c>
+      <c r="AE108">
+        <v>92</v>
+      </c>
+      <c r="AF108">
+        <v>92</v>
+      </c>
+      <c r="AG108">
+        <v>89</v>
+      </c>
+      <c r="AH108">
+        <v>88</v>
+      </c>
+      <c r="AI108">
+        <v>94</v>
+      </c>
+      <c r="AJ108">
+        <v>96</v>
+      </c>
+      <c r="AK108">
+        <v>96</v>
+      </c>
+      <c r="AL108">
+        <v>90</v>
+      </c>
+      <c r="AM108">
+        <v>80</v>
+      </c>
+      <c r="AN108">
+        <v>90</v>
+      </c>
+      <c r="AO108">
+        <v>101</v>
+      </c>
+      <c r="AP108">
+        <v>97</v>
+      </c>
+      <c r="AQ108">
+        <v>87</v>
+      </c>
+      <c r="AR108">
+        <v>96</v>
+      </c>
+      <c r="AS108">
+        <v>103</v>
+      </c>
+      <c r="AT108">
+        <v>92</v>
+      </c>
+      <c r="AU108">
+        <v>69</v>
+      </c>
+      <c r="AV108">
+        <v>80</v>
+      </c>
+      <c r="AW108">
+        <v>103</v>
+      </c>
+      <c r="AX108">
+        <v>93</v>
+      </c>
+      <c r="AY108">
+        <v>69</v>
+      </c>
+      <c r="AZ108">
+        <v>80</v>
+      </c>
+      <c r="BA108">
+        <v>89</v>
+      </c>
+      <c r="BB108">
+        <v>88</v>
+      </c>
+      <c r="BC108">
+        <v>80</v>
+      </c>
+      <c r="BD108">
+        <v>57</v>
+      </c>
+      <c r="BE108">
+        <v>89</v>
+      </c>
+      <c r="BF108">
+        <v>87</v>
+      </c>
+      <c r="BG108">
+        <v>86</v>
       </c>
     </row>
     <row r="109" spans="1:59" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update to FirstTurn database
</commit_message>
<xml_diff>
--- a/projects/firstTurnData/FirstTurnCombined.xlsx
+++ b/projects/firstTurnData/FirstTurnCombined.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PNJae\Dropbox\website\PNJaenichen.github.io\projects\firstTurnData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04116A88-C32A-4927-B7F0-3FF81BD91D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D9B09C-5DE2-4AF4-9C3C-A4BB173ECEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E5432155-75DF-41C9-A811-869614260F5F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3270" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3294" uniqueCount="336">
   <si>
     <t>Yes</t>
   </si>
@@ -1041,6 +1041,12 @@
   <si>
     <t>king_hill</t>
   </si>
+  <si>
+    <t>Seize the Bean</t>
+  </si>
+  <si>
+    <t>Port Royale</t>
+  </si>
 </sst>
 </file>
 
@@ -1439,7 +1445,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D145" sqref="D145"/>
+      <selection pane="bottomLeft" activeCell="K147" sqref="K147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -76230,12 +76236,15 @@
       <c r="C145" s="6" t="s">
         <v>324</v>
       </c>
+      <c r="D145" s="1">
+        <v>40</v>
+      </c>
       <c r="E145" s="1">
         <v>22</v>
       </c>
       <c r="F145" s="7">
         <f t="shared" si="68"/>
-        <v>-22</v>
+        <v>18</v>
       </c>
       <c r="G145" s="1">
         <v>2.2000000000000002</v>
@@ -76248,6 +76257,12 @@
       </c>
       <c r="J145" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="K145" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L145" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="M145" s="1" t="s">
         <v>36</v>
@@ -76260,6 +76275,12 @@
         <f t="shared" si="109"/>
         <v>null</v>
       </c>
+      <c r="P145" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q145" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="R145" s="1" t="s">
         <v>36</v>
       </c>
@@ -76271,6 +76292,12 @@
         <f t="shared" si="111"/>
         <v>null</v>
       </c>
+      <c r="U145" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V145" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="W145" s="1" t="s">
         <v>36</v>
       </c>
@@ -76282,6 +76309,12 @@
         <f t="shared" si="113"/>
         <v>null</v>
       </c>
+      <c r="Z145" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA145" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="AB145" s="1" t="s">
         <v>36</v>
       </c>
@@ -76292,6 +76325,12 @@
       <c r="AD145" s="7" t="str">
         <f t="shared" si="115"/>
         <v>null</v>
+      </c>
+      <c r="AE145" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF145" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="AG145" s="1" t="s">
         <v>36</v>
@@ -76706,72 +76745,123 @@
       <c r="A146" s="1">
         <v>136</v>
       </c>
+      <c r="B146" s="2" t="s">
+        <v>334</v>
+      </c>
       <c r="C146" s="6" t="s">
         <v>324</v>
       </c>
+      <c r="E146" s="1">
+        <v>67</v>
+      </c>
       <c r="F146" s="7">
         <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="N146" s="7" t="e">
+        <v>-67</v>
+      </c>
+      <c r="G146" s="1">
+        <v>2.68</v>
+      </c>
+      <c r="H146" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="I146" s="1">
+        <v>3248</v>
+      </c>
+      <c r="J146" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N146" s="7">
         <f t="shared" si="108"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O146" s="7" t="e">
+        <v>-0.36842105263157893</v>
+      </c>
+      <c r="O146" s="7">
         <f t="shared" si="109"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S146" s="7" t="e">
+        <v>-3.5289937510073801</v>
+      </c>
+      <c r="S146" s="7">
         <f t="shared" si="110"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T146" s="7" t="e">
+        <v>-0.36842105263157893</v>
+      </c>
+      <c r="T146" s="7">
         <f t="shared" si="111"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X146" s="7" t="e">
+        <v>-3.5289937510073801</v>
+      </c>
+      <c r="X146" s="7">
         <f t="shared" si="112"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y146" s="7" t="e">
+        <v>-0.36842105263157893</v>
+      </c>
+      <c r="Y146" s="7">
         <f t="shared" si="113"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC146" s="7" t="e">
+        <v>-3.5289937510073801</v>
+      </c>
+      <c r="AC146" s="7">
         <f t="shared" si="114"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD146" s="7" t="e">
+        <v>-0.36842105263157893</v>
+      </c>
+      <c r="AD146" s="7">
         <f t="shared" si="115"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH146" s="7" t="e">
+        <v>-3.5289937510073801</v>
+      </c>
+      <c r="AG146" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH146" s="7" t="str">
         <f t="shared" si="116"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI146" s="7" t="e">
+        <v>null</v>
+      </c>
+      <c r="AI146" s="7" t="str">
         <f t="shared" si="117"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AL146" s="7" t="e">
+        <v>null</v>
+      </c>
+      <c r="AJ146" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK146" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL146" s="7">
         <f t="shared" si="122"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AM146" s="7" t="e">
+        <v>-0.36842105263157893</v>
+      </c>
+      <c r="AM146" s="7">
         <f t="shared" si="123"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AN146" s="7" t="e">
+        <v>-0.36842105263157893</v>
+      </c>
+      <c r="AN146" s="7">
         <f t="shared" si="124"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AO146" s="7" t="e">
+        <v>-0.36842105263157893</v>
+      </c>
+      <c r="AO146" s="7">
         <f t="shared" si="125"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
+      </c>
+      <c r="AP146" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ146" s="1">
+        <v>29.134615384615383</v>
+      </c>
+      <c r="AR146" s="1">
+        <v>8.2557854845446155</v>
+      </c>
+      <c r="AS146" s="1">
+        <v>14</v>
+      </c>
+      <c r="AT146" s="1">
+        <v>52</v>
+      </c>
+      <c r="AU146" s="1">
+        <v>23</v>
+      </c>
+      <c r="AV146" s="1">
+        <v>35</v>
+      </c>
+      <c r="AW146" s="1">
+        <v>29.5</v>
       </c>
       <c r="AX146" s="10">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AY146" s="1">
         <v>0</v>
@@ -76822,7 +76912,7 @@
         <v>0</v>
       </c>
       <c r="BO146" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP146" s="1">
         <v>0</v>
@@ -76855,7 +76945,7 @@
         <v>0</v>
       </c>
       <c r="BZ146" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA146" s="1">
         <v>0</v>
@@ -76891,7 +76981,7 @@
         <v>0</v>
       </c>
       <c r="CL146" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM146" s="1">
         <v>0</v>
@@ -77032,7 +77122,7 @@
         <v>0</v>
       </c>
       <c r="EG146" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EH146" s="1">
         <v>0</v>
@@ -77062,7 +77152,7 @@
         <v>0</v>
       </c>
       <c r="EQ146" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ER146" s="1">
         <v>0</v>
@@ -77119,7 +77209,7 @@
         <v>0</v>
       </c>
       <c r="FJ146" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FK146" s="1">
         <v>0</v>
@@ -77129,72 +77219,123 @@
       <c r="A147" s="1">
         <v>137</v>
       </c>
+      <c r="B147" s="2" t="s">
+        <v>335</v>
+      </c>
       <c r="C147" s="6" t="s">
         <v>324</v>
       </c>
+      <c r="E147" s="1">
+        <v>35</v>
+      </c>
       <c r="F147" s="7">
         <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="N147" s="7" t="e">
+        <v>-35</v>
+      </c>
+      <c r="G147" s="1">
+        <v>1.62</v>
+      </c>
+      <c r="H147" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="I147" s="1">
+        <v>480</v>
+      </c>
+      <c r="J147" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N147" s="7">
         <f t="shared" si="108"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O147" s="7" t="e">
+        <v>-0.41666666666666669</v>
+      </c>
+      <c r="O147" s="7">
         <f t="shared" si="109"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S147" s="7" t="e">
+        <v>-3.3852229994773686</v>
+      </c>
+      <c r="S147" s="7">
         <f t="shared" si="110"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T147" s="7" t="e">
+        <v>-0.41666666666666669</v>
+      </c>
+      <c r="T147" s="7">
         <f t="shared" si="111"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X147" s="7" t="e">
+        <v>-3.3852229994773686</v>
+      </c>
+      <c r="X147" s="7">
         <f t="shared" si="112"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y147" s="7" t="e">
+        <v>-0.41666666666666669</v>
+      </c>
+      <c r="Y147" s="7">
         <f t="shared" si="113"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC147" s="7" t="e">
+        <v>-3.3852229994773686</v>
+      </c>
+      <c r="AC147" s="7">
         <f t="shared" si="114"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD147" s="7" t="e">
+        <v>-0.41666666666666669</v>
+      </c>
+      <c r="AD147" s="7">
         <f t="shared" si="115"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH147" s="7" t="e">
+        <v>-3.3852229994773686</v>
+      </c>
+      <c r="AG147" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH147" s="7" t="str">
         <f t="shared" si="116"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI147" s="7" t="e">
+        <v>null</v>
+      </c>
+      <c r="AI147" s="7" t="str">
         <f t="shared" si="117"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AL147" s="7" t="e">
+        <v>null</v>
+      </c>
+      <c r="AJ147" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK147" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL147" s="7">
         <f t="shared" si="122"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AM147" s="7" t="e">
+        <v>-0.41666666666666669</v>
+      </c>
+      <c r="AM147" s="7">
         <f t="shared" si="123"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AN147" s="7" t="e">
+        <v>-0.41666666666666669</v>
+      </c>
+      <c r="AN147" s="7">
         <f t="shared" si="124"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AO147" s="7" t="e">
+        <v>-0.41666666666666669</v>
+      </c>
+      <c r="AO147" s="7">
         <f t="shared" si="125"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
+      </c>
+      <c r="AP147" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ147" s="1">
+        <v>9.9038461538461533</v>
+      </c>
+      <c r="AR147" s="1">
+        <v>2.9256111503954596</v>
+      </c>
+      <c r="AS147" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT147" s="1">
+        <v>17</v>
+      </c>
+      <c r="AU147" s="1">
+        <v>7.25</v>
+      </c>
+      <c r="AV147" s="1">
+        <v>12</v>
+      </c>
+      <c r="AW147" s="1">
+        <v>9</v>
       </c>
       <c r="AX147" s="10">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AY147" s="1">
         <v>0</v>
@@ -77245,7 +77386,7 @@
         <v>0</v>
       </c>
       <c r="BO147" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP147" s="1">
         <v>0</v>
@@ -77269,7 +77410,7 @@
         <v>0</v>
       </c>
       <c r="BW147" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX147" s="1">
         <v>0</v>
@@ -77422,7 +77563,7 @@
         <v>0</v>
       </c>
       <c r="DV147" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DW147" s="1">
         <v>0</v>
@@ -77455,7 +77596,7 @@
         <v>0</v>
       </c>
       <c r="EG147" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EH147" s="1">
         <v>0</v>
@@ -79673,10 +79814,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCBA7DA-4A7C-4BD5-95F2-6CD93F57778E}">
   <dimension ref="A1:BI117"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A58" sqref="A58"/>
-      <selection pane="topRight" activeCell="B109" sqref="B109:H110"/>
+      <selection pane="topRight" activeCell="B111" sqref="B111:H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -99757,63 +99898,381 @@
       </c>
     </row>
     <row r="111" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="B111" t="e">
+      <c r="A111" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B111">
         <f t="shared" ref="B111:B117" si="42">AVERAGE(I111:BI111)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C111" t="e">
+        <v>29.134615384615383</v>
+      </c>
+      <c r="C111">
         <f t="shared" ref="C111:C117" si="43">_xlfn.STDEV.S(I111:BI111)</f>
-        <v>#DIV/0!</v>
+        <v>8.2557854845446155</v>
       </c>
       <c r="D111">
         <f t="shared" ref="D111:D117" si="44">MIN(I111:BI111)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E111">
         <f t="shared" ref="E111:E117" si="45">MAX(J111:BI111)</f>
-        <v>0</v>
-      </c>
-      <c r="F111" t="e">
+        <v>52</v>
+      </c>
+      <c r="F111">
         <f t="shared" ref="F111:F117" si="46">_xlfn.QUARTILE.EXC(I111:BI111,1)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G111" t="e">
+        <v>23</v>
+      </c>
+      <c r="G111">
         <f t="shared" ref="G111:G117" si="47">_xlfn.QUARTILE.EXC(I111:BI111,3)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H111" s="11" t="e">
+        <v>35</v>
+      </c>
+      <c r="H111" s="11">
         <f t="shared" ref="H111:H117" si="48">MEDIAN(I111:BI111)</f>
-        <v>#NUM!</v>
+        <v>29.5</v>
+      </c>
+      <c r="I111">
+        <v>25</v>
+      </c>
+      <c r="J111">
+        <v>31</v>
+      </c>
+      <c r="K111">
+        <v>25</v>
+      </c>
+      <c r="L111">
+        <v>26</v>
+      </c>
+      <c r="M111">
+        <v>29</v>
+      </c>
+      <c r="N111">
+        <v>14</v>
+      </c>
+      <c r="O111">
+        <v>34</v>
+      </c>
+      <c r="P111">
+        <v>19</v>
+      </c>
+      <c r="Q111">
+        <v>35</v>
+      </c>
+      <c r="R111">
+        <v>19</v>
+      </c>
+      <c r="S111">
+        <v>29</v>
+      </c>
+      <c r="T111">
+        <v>31</v>
+      </c>
+      <c r="U111">
+        <v>28</v>
+      </c>
+      <c r="V111">
+        <v>34</v>
+      </c>
+      <c r="W111">
+        <v>18</v>
+      </c>
+      <c r="X111">
+        <v>34</v>
+      </c>
+      <c r="Y111">
+        <v>14</v>
+      </c>
+      <c r="Z111">
+        <v>15</v>
+      </c>
+      <c r="AA111">
+        <v>23</v>
+      </c>
+      <c r="AB111">
+        <v>25</v>
+      </c>
+      <c r="AC111">
+        <v>39</v>
+      </c>
+      <c r="AD111">
+        <v>31</v>
+      </c>
+      <c r="AE111">
+        <v>26</v>
+      </c>
+      <c r="AF111">
+        <v>26</v>
+      </c>
+      <c r="AG111">
+        <v>33</v>
+      </c>
+      <c r="AH111">
+        <v>32</v>
+      </c>
+      <c r="AI111">
+        <v>39</v>
+      </c>
+      <c r="AJ111">
+        <v>45</v>
+      </c>
+      <c r="AK111">
+        <v>37</v>
+      </c>
+      <c r="AL111">
+        <v>23</v>
+      </c>
+      <c r="AM111">
+        <v>41</v>
+      </c>
+      <c r="AN111">
+        <v>37</v>
+      </c>
+      <c r="AO111">
+        <v>34</v>
+      </c>
+      <c r="AP111">
+        <v>28</v>
+      </c>
+      <c r="AQ111">
+        <v>36</v>
+      </c>
+      <c r="AR111">
+        <v>52</v>
+      </c>
+      <c r="AS111">
+        <v>34</v>
+      </c>
+      <c r="AT111">
+        <v>18</v>
+      </c>
+      <c r="AU111">
+        <v>30</v>
+      </c>
+      <c r="AV111">
+        <v>37</v>
+      </c>
+      <c r="AW111">
+        <v>23</v>
+      </c>
+      <c r="AX111">
+        <v>19</v>
+      </c>
+      <c r="AY111">
+        <v>14</v>
+      </c>
+      <c r="AZ111">
+        <v>37</v>
+      </c>
+      <c r="BA111">
+        <v>31</v>
+      </c>
+      <c r="BB111">
+        <v>36</v>
+      </c>
+      <c r="BC111">
+        <v>27</v>
+      </c>
+      <c r="BD111">
+        <v>23</v>
+      </c>
+      <c r="BE111">
+        <v>29</v>
+      </c>
+      <c r="BF111">
+        <v>35</v>
+      </c>
+      <c r="BG111">
+        <v>20</v>
+      </c>
+      <c r="BH111">
+        <v>35</v>
       </c>
     </row>
     <row r="112" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="B112" t="e">
+      <c r="A112" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B112">
         <f t="shared" si="42"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C112" t="e">
+        <v>9.9038461538461533</v>
+      </c>
+      <c r="C112">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>2.9256111503954596</v>
       </c>
       <c r="D112">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E112">
         <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="F112" t="e">
+        <v>17</v>
+      </c>
+      <c r="F112">
         <f t="shared" si="46"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="G112" t="e">
+        <v>7.25</v>
+      </c>
+      <c r="G112">
         <f t="shared" si="47"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H112" s="11" t="e">
+        <v>12</v>
+      </c>
+      <c r="H112" s="11">
         <f t="shared" si="48"/>
-        <v>#NUM!</v>
+        <v>9</v>
+      </c>
+      <c r="I112">
+        <v>5</v>
+      </c>
+      <c r="J112">
+        <v>5</v>
+      </c>
+      <c r="K112">
+        <v>12</v>
+      </c>
+      <c r="L112">
+        <v>5</v>
+      </c>
+      <c r="M112">
+        <v>10</v>
+      </c>
+      <c r="N112">
+        <v>7</v>
+      </c>
+      <c r="O112">
+        <v>10</v>
+      </c>
+      <c r="P112">
+        <v>12</v>
+      </c>
+      <c r="Q112">
+        <v>8</v>
+      </c>
+      <c r="R112">
+        <v>8</v>
+      </c>
+      <c r="S112">
+        <v>11</v>
+      </c>
+      <c r="T112">
+        <v>12</v>
+      </c>
+      <c r="U112">
+        <v>13</v>
+      </c>
+      <c r="V112">
+        <v>12</v>
+      </c>
+      <c r="W112">
+        <v>16</v>
+      </c>
+      <c r="X112">
+        <v>16</v>
+      </c>
+      <c r="Y112">
+        <v>13</v>
+      </c>
+      <c r="Z112">
+        <v>11</v>
+      </c>
+      <c r="AA112">
+        <v>9</v>
+      </c>
+      <c r="AB112">
+        <v>13</v>
+      </c>
+      <c r="AC112">
+        <v>11</v>
+      </c>
+      <c r="AD112">
+        <v>12</v>
+      </c>
+      <c r="AE112">
+        <v>6</v>
+      </c>
+      <c r="AF112">
+        <v>6</v>
+      </c>
+      <c r="AG112">
+        <v>9</v>
+      </c>
+      <c r="AH112">
+        <v>17</v>
+      </c>
+      <c r="AI112">
+        <v>14</v>
+      </c>
+      <c r="AJ112">
+        <v>12</v>
+      </c>
+      <c r="AK112">
+        <v>6</v>
+      </c>
+      <c r="AL112">
+        <v>7</v>
+      </c>
+      <c r="AM112">
+        <v>12</v>
+      </c>
+      <c r="AN112">
+        <v>9</v>
+      </c>
+      <c r="AO112">
+        <v>9</v>
+      </c>
+      <c r="AP112">
+        <v>9</v>
+      </c>
+      <c r="AQ112">
+        <v>12</v>
+      </c>
+      <c r="AR112">
+        <v>7</v>
+      </c>
+      <c r="AS112">
+        <v>9</v>
+      </c>
+      <c r="AT112">
+        <v>9</v>
+      </c>
+      <c r="AU112">
+        <v>7</v>
+      </c>
+      <c r="AV112">
+        <v>12</v>
+      </c>
+      <c r="AW112">
+        <v>13</v>
+      </c>
+      <c r="AX112">
+        <v>7</v>
+      </c>
+      <c r="AY112">
+        <v>7</v>
+      </c>
+      <c r="AZ112">
+        <v>9</v>
+      </c>
+      <c r="BA112">
+        <v>9</v>
+      </c>
+      <c r="BB112">
+        <v>8</v>
+      </c>
+      <c r="BC112">
+        <v>12</v>
+      </c>
+      <c r="BD112">
+        <v>7</v>
+      </c>
+      <c r="BE112">
+        <v>10</v>
+      </c>
+      <c r="BF112">
+        <v>9</v>
+      </c>
+      <c r="BG112">
+        <v>8</v>
+      </c>
+      <c r="BH112">
+        <v>13</v>
       </c>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>